<commit_message>
Demo Level Draft Update
About finished half of demo level blueprint and made a rough outline of the other half. Also added Keys to the GDD.
</commit_message>
<xml_diff>
--- a/Game Design Documentation/Demo Level Map Draft.xlsx
+++ b/Game Design Documentation/Demo Level Map Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://osekk-my.sharepoint.com/personal/s4voto00_students_osao_fi/Documents/Tiedostot/Github/CartoonViolence/Game Design Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="742" documentId="11_F25DC773A252ABDACC1048BB699D52725ADE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9880470-5E2C-482A-8C72-3F0CC786F441}"/>
+  <xr:revisionPtr revIDLastSave="1530" documentId="11_F25DC773A252ABDACC1048BB699D52725ADE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98A30EB2-707E-4F87-8B79-549D2AF35D3D}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="9960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,6 +416,30 @@
     <author>Touko Erkki Tapani Vornanen</author>
   </authors>
   <commentList>
+    <comment ref="EU2" authorId="0" shapeId="0" xr:uid="{F053257E-CAE8-4C15-88AA-0682B3F26612}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is on the roof, the only place where scrolling is smooth between screens. When you pick this up, a silhouette of Mrs. Longsong emerges in the background and leaps towards the screen. She just goes over Frank though, it's purely for a scare.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D4" authorId="0" shapeId="0" xr:uid="{C1A9C2E8-16CD-4862-823C-AF7258818C31}">
       <text>
         <r>
@@ -464,7 +488,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK19" authorId="0" shapeId="0" xr:uid="{294DF8DA-5C62-4C56-AEC1-C25D7AC21EFF}">
+    <comment ref="Z14" authorId="0" shapeId="0" xr:uid="{EE8505EE-1986-4FBB-AC4A-DE196A9C9343}">
       <text>
         <r>
           <rPr>
@@ -472,6 +496,31 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Migraine Morton
+He's here to show you that bomb blasts agitate them. Can't reach Frank.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BE14" authorId="0" shapeId="0" xr:uid="{6A205A62-6973-403C-87C7-F5CCD8BFB0E7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t>Touko Erkki Tapani Vornanen:</t>
@@ -484,7 +533,80 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Mr. Patches' homage secret. You have to use Bombs a lot here.</t>
+Frank has to either drop an anvil or a bomb here to break the floor, then gently lower himself down because otherwise he dies of fall damage.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AT16" authorId="0" shapeId="0" xr:uid="{842C90FC-F64A-49E5-A78B-ED1C8BBF4E98}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Lipsmack</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD19" authorId="0" shapeId="0" xr:uid="{294DF8DA-5C62-4C56-AEC1-C25D7AC21EFF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mr. Patches' homage secret. You have to use Bombs a lot here.
+I'm thinking of it being a prop warehouse with a lot of Migraine Mortons, so you have to use Bombs wisely. (Finish later)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BF20" authorId="0" shapeId="0" xr:uid="{EC7A1721-DE12-4050-8D9C-A9F64E2827BD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Migraine Morton</t>
         </r>
       </text>
     </comment>
@@ -562,6 +684,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="CQ23" authorId="0" shapeId="0" xr:uid="{0B4BA51F-22A6-4BC7-B1D6-AE6FCC9B057D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Opens or closes the shutter.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AD24" authorId="0" shapeId="0" xr:uid="{912D4762-3D04-4ADA-9137-D22C9B8D02A1}">
       <text>
         <r>
@@ -583,6 +729,105 @@
           </rPr>
           <t xml:space="preserve">
 This shutter is open by default.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T26" authorId="0" shapeId="0" xr:uid="{43260E7F-BE34-474C-A0FF-3F29BFC89174}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+There's a closet here so the player can try it out.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BY26" authorId="0" shapeId="0" xr:uid="{FC5DB650-4D98-4A73-8F19-3FB2E1766243}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ducker
+Walks back and forth on the spots marked with ↔. Unloaded.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CR26" authorId="0" shapeId="0" xr:uid="{FEE6A444-7CCC-4845-9009-2D446624E1D3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ducker
+Walks back and forth on the spots marked with ↔. Unloaded.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BX27" authorId="0" shapeId="0" xr:uid="{45AF132E-E0A3-4B10-835F-82FB2DD5531D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Here's a sneaky breakable floor. You have to draw your Bomb while the Ducker is not looking and then run, because the hissing of the fuse will alert him.
+Knocking the Ducker out and then laying the Bomb also works.</t>
         </r>
       </text>
     </comment>
@@ -704,6 +949,350 @@
           <t xml:space="preserve">
 Ducker
 You can only see his eyes and hear the slap of his feet as he walks off-screen.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BB29" authorId="0" shapeId="0" xr:uid="{4DB33601-4343-4B00-8741-87B98CE4EF4B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ducker x 2
+When you drop down to this floor, the Duckers appear from the shadows and a small scene plays. Afterwards Frank runs through the door automatically and has his realization that his life is in actual danger.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BK29" authorId="0" shapeId="0" xr:uid="{18E98016-3699-4350-8DC7-AD1D45C8E69D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If you try to go back, the Duckers will just shoot Frank.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CW32" authorId="0" shapeId="0" xr:uid="{167E8124-09EE-467F-B70F-82820E858439}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+You could probably show here what Annows look like.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BQ35" authorId="0" shapeId="0" xr:uid="{C14577E5-0970-4D24-A90A-50D98A5ECD46}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mrs. Creeps' secret. A mannequin storeroom covered in spider web, with some mannequins hanging from the ceiling. You have to mostly utilize the Campfire here.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CF35" authorId="0" shapeId="0" xr:uid="{BA6AA6BD-49FC-4BAA-BE54-039FDB549F14}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Opens or closes the shutter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CH35" authorId="0" shapeId="0" xr:uid="{D343D244-20BC-4632-B344-53CE6AA0BA31}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ducker
+Loaded, will shoot on sight. Stationary.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DX37" authorId="0" shapeId="0" xr:uid="{FDD08983-F57B-40F5-B2DD-EBD86D7E79D8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mrs. Longsong's secret. You climb up and up, dealing mostly with wet areas that force you to think how to use your Bombs and Campfires.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CF38" authorId="0" shapeId="0" xr:uid="{08E132D4-CD4D-49F2-9856-2950D0EB5346}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Migraine Morton
+You must agitate him, shows the player both that they can attack above and below, but also makes the Ducker flee.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CK38" authorId="0" shapeId="0" xr:uid="{571264F7-854C-41FA-A334-02B639A2B7CA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ducker
+Unloaded, Stationary.
+Runs to the other screen, if you lure the Morton there, he will kill the Ducker before focusing on you again.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CR44" authorId="0" shapeId="0" xr:uid="{8E969225-FBD9-479A-924B-5F0C6A278995}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Opens the shutter, dropping the Morton down to chase you.
+If you came from the secret, nothing happens.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FK46" authorId="0" shapeId="0" xr:uid="{36F2BAE0-F069-4BEA-BEC7-E6DBFDB87083}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Again, just in case someone actually manages to get here.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FA47" authorId="0" shapeId="0" xr:uid="{6E66CF02-2305-461D-8F46-705A678F6DBE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This floor breaks when you walk on it. Frank should complain that he keeps falling down today, prompting Mr. Phant to show himself.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FE53" authorId="0" shapeId="0" xr:uid="{BB4D8B84-454A-4568-942D-9EFAB6A4680A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mr. Phant emerges from this shadow. After a brief scene, he becomes hostile and starts chasing you.
+The chase ends near the Mrs. Creeps secret.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CJ56" authorId="0" shapeId="0" xr:uid="{C4D9245B-88C2-4BB7-B8E2-399EAB5CD5D7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+When you collect this, you'll hear skittering and Mrs. Creeps peeks out of a crack in the wall. She giggles and leaves.
+Frank then has to climb up and reach a door that skips a few rooms in the regular level.</t>
         </r>
       </text>
     </comment>
@@ -712,7 +1301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Screen Template</t>
   </si>
@@ -868,6 +1457,30 @@
   <si>
     <t>←</t>
   </si>
+  <si>
+    <t>DUCK!</t>
+  </si>
+  <si>
+    <t>↔</t>
+  </si>
+  <si>
+    <t>Burnable (Web, vines, etc.)</t>
+  </si>
+  <si>
+    <t>SORRY</t>
+  </si>
+  <si>
+    <t>NOTHING</t>
+  </si>
+  <si>
+    <t>↓↓</t>
+  </si>
+  <si>
+    <t>To Dressing Rooms</t>
+  </si>
+  <si>
+    <t>END OF DEMO</t>
+  </si>
 </sst>
 </file>
 
@@ -995,7 +1608,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="77">
+  <borders count="114">
     <border>
       <left/>
       <right/>
@@ -1788,17 +2401,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
     <border diagonalUp="1">
       <left style="double">
         <color indexed="64"/>
@@ -1847,93 +2449,517 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDotDot">
+        <color indexed="64"/>
+      </left>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDotDot">
+        <color indexed="64"/>
+      </left>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDotDot">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
     <border diagonalUp="1">
       <left style="double">
         <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="double">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="slantDashDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="slantDashDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="slantDashDot">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dashDotDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashDot">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="slantDashDot">
+        <color theme="5"/>
+      </top>
+      <bottom style="mediumDashDot">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashDot">
+        <color theme="9"/>
+      </left>
+      <right style="mediumDashDot">
+        <color theme="9"/>
+      </right>
+      <top style="mediumDashDot">
+        <color theme="9"/>
+      </top>
+      <bottom style="mediumDashDot">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="mediumDashDot">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="double">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1">
+      <left/>
+      <right style="double">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal style="double">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="dashDotDot">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashDotDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDotDot">
+        <color indexed="64"/>
+      </left>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="slantDashDot">
+        <color theme="7"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal style="double">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="slantDashDot">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1">
+      <left style="double">
+        <color rgb="FF7030A0"/>
       </left>
       <right/>
       <top style="double">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal style="double">
         <color indexed="64"/>
       </diagonal>
+    </border>
+    <border diagonalUp="1">
+      <left style="double">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="double">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="mediumDashDotDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashDotDot">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border diagonalUp="1">
       <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
+      <right/>
+      <top/>
+      <bottom style="dashDotDot">
+        <color rgb="FF7030A0"/>
       </bottom>
       <diagonal style="double">
-        <color indexed="64"/>
+        <color rgb="FF7030A0"/>
       </diagonal>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
+    <border diagonalUp="1">
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
+      <top/>
+      <bottom/>
+      <diagonal style="double">
+        <color rgb="FF7030A0"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -2052,14 +3078,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2068,25 +3093,107 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="65" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="69" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="68" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="73" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="78" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="80" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="78" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="80" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="91" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="96" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="97" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="98" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="99" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="100" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="101" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="102" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="103" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="104" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="105" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="106" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="103" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="109" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="110" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="111" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="112" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="113" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -2374,7 +3481,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K10" sqref="B2:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2535,7 +3642,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M17" s="129"/>
+    </row>
+    <row r="18" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="18">
         <v>1</v>
       </c>
@@ -2546,9 +3656,14 @@
       <c r="I18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L18" s="128"/>
+      <c r="M18" s="130"/>
+      <c r="N18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="21" t="s">
         <v>21</v>
       </c>
@@ -2556,12 +3671,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>20</v>
       </c>
@@ -2576,8 +3691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2B2FEB-625D-42F7-933A-9E09CE4A3EF3}">
   <dimension ref="C17:BL45"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD31" sqref="AD31"/>
+    <sheetView topLeftCell="H22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z30" sqref="Z30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2806,7 +3921,7 @@
       <c r="C24" s="22"/>
       <c r="M24" s="2"/>
       <c r="R24" s="26"/>
-      <c r="V24" s="26"/>
+      <c r="V24" s="111"/>
       <c r="W24" s="2"/>
       <c r="X24" s="39"/>
       <c r="Z24" s="41"/>
@@ -2825,7 +3940,7 @@
       <c r="C25" s="22"/>
       <c r="M25" s="2"/>
       <c r="R25" s="22"/>
-      <c r="V25" s="22"/>
+      <c r="V25" s="112"/>
       <c r="W25" s="38"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="40"/>
@@ -2862,13 +3977,13 @@
       <c r="S26" s="1"/>
       <c r="T26" s="4"/>
       <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="3"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
-      <c r="AA26" s="1"/>
-      <c r="AB26" s="1"/>
+      <c r="V26" s="90"/>
+      <c r="W26" s="92"/>
+      <c r="X26" s="90"/>
+      <c r="Y26" s="90"/>
+      <c r="Z26" s="90"/>
+      <c r="AA26" s="90"/>
+      <c r="AB26" s="90"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
@@ -3107,10 +4222,10 @@
       <c r="M37" s="22"/>
       <c r="N37" s="11"/>
       <c r="O37" s="22"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="86" t="s">
+      <c r="P37" s="152" t="s">
         <v>44</v>
       </c>
+      <c r="Q37" s="86"/>
       <c r="S37" s="31" t="s">
         <v>39</v>
       </c>
@@ -3152,10 +4267,10 @@
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
-      <c r="V41" s="97" t="s">
+      <c r="V41" s="96"/>
+      <c r="W41" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="W41" s="12"/>
     </row>
     <row r="42" spans="13:64" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M42" s="22"/>
@@ -3198,10 +4313,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A88EDC-4468-4B92-BB23-9A52F08C9D3C}">
-  <dimension ref="A2:AP30"/>
+  <dimension ref="A1:FP57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="DE35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DW40" sqref="DW40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3209,42 +4324,88 @@
     <col min="1" max="305" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-    </row>
-    <row r="3" spans="1:42" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22"/>
+    <row r="1" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="DR1" s="109"/>
+      <c r="DT1" s="167"/>
+      <c r="EV1" s="134"/>
+    </row>
+    <row r="2" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="132"/>
+      <c r="M2" s="132"/>
+      <c r="N2" s="132"/>
+      <c r="O2" s="132"/>
+      <c r="P2" s="132"/>
+      <c r="Q2" s="132"/>
+      <c r="R2" s="132"/>
+      <c r="S2" s="132"/>
+      <c r="T2" s="132"/>
+      <c r="U2" s="132"/>
+      <c r="V2" s="132"/>
+      <c r="DR2" s="109"/>
+      <c r="DS2" s="166"/>
+      <c r="DT2" s="165"/>
+      <c r="DU2" s="132"/>
+      <c r="DV2" s="132"/>
+      <c r="DW2" s="132"/>
+      <c r="DX2" s="132"/>
+      <c r="DY2" s="132"/>
+      <c r="DZ2" s="132"/>
+      <c r="EA2" s="132"/>
+      <c r="EB2" s="132"/>
+      <c r="EC2" s="132"/>
+      <c r="ED2" s="132"/>
+      <c r="EE2" s="132"/>
+      <c r="EF2" s="132"/>
+      <c r="EG2" s="132"/>
+      <c r="EH2" s="132"/>
+      <c r="EI2" s="132"/>
+      <c r="EJ2" s="132"/>
+      <c r="EK2" s="132"/>
+      <c r="EL2" s="132"/>
+      <c r="EM2" s="132"/>
+      <c r="EN2" s="132"/>
+      <c r="EO2" s="132"/>
+      <c r="EP2" s="132"/>
+      <c r="EQ2" s="132"/>
+      <c r="ER2" s="132"/>
+      <c r="ES2" s="132"/>
+      <c r="ET2" s="132"/>
+      <c r="EU2" s="149" t="s">
+        <v>21</v>
+      </c>
+      <c r="EV2" s="144"/>
+    </row>
+    <row r="3" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="134"/>
       <c r="L3" s="2"/>
-      <c r="V3" s="26"/>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="B4" s="22"/>
+      <c r="V3" s="133"/>
+      <c r="DR3" s="134"/>
+      <c r="EB3" s="2"/>
+      <c r="EV3" s="22"/>
+    </row>
+    <row r="4" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="B4" s="134"/>
       <c r="L4" s="2"/>
-      <c r="V4" s="22"/>
-    </row>
-    <row r="5" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="22"/>
+      <c r="V4" s="134"/>
+      <c r="DR4" s="134"/>
+      <c r="EB4" s="2"/>
+      <c r="EV4" s="22"/>
+    </row>
+    <row r="5" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="134"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="30" t="s">
+        <v>21</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -3262,20 +4423,38 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="27"/>
-    </row>
-    <row r="6" spans="1:42" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="22"/>
+      <c r="V5" s="135"/>
+      <c r="DR5" s="134"/>
+      <c r="DS5" s="1"/>
+      <c r="DT5" s="1"/>
+      <c r="DU5" s="1"/>
+      <c r="DV5" s="1"/>
+      <c r="DW5" s="1"/>
+      <c r="DX5" s="1"/>
+      <c r="DY5" s="1"/>
+      <c r="DZ5" s="1"/>
+      <c r="EA5" s="1"/>
+      <c r="EB5" s="3"/>
+      <c r="EV5" s="22"/>
+    </row>
+    <row r="6" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="134"/>
       <c r="L6" s="2"/>
-      <c r="V6" s="22"/>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="B7" s="22"/>
+      <c r="V6" s="134"/>
+      <c r="DR6" s="134"/>
+      <c r="EB6" s="2"/>
+      <c r="EV6" s="22"/>
+    </row>
+    <row r="7" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="B7" s="134"/>
       <c r="L7" s="2"/>
-      <c r="V7" s="22"/>
-    </row>
-    <row r="8" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="22"/>
+      <c r="V7" s="134"/>
+      <c r="DR7" s="134"/>
+      <c r="EB7" s="2"/>
+      <c r="EV7" s="22"/>
+    </row>
+    <row r="8" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="134"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -3295,20 +4474,38 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="27"/>
-    </row>
-    <row r="9" spans="1:42" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="22"/>
+      <c r="V8" s="135"/>
+      <c r="DR8" s="134"/>
+      <c r="DS8" s="1"/>
+      <c r="DT8" s="1"/>
+      <c r="DU8" s="1"/>
+      <c r="DV8" s="1"/>
+      <c r="DW8" s="1"/>
+      <c r="DX8" s="1"/>
+      <c r="DY8" s="1"/>
+      <c r="DZ8" s="1"/>
+      <c r="EA8" s="1"/>
+      <c r="EB8" s="3"/>
+      <c r="EV8" s="22"/>
+    </row>
+    <row r="9" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="134"/>
       <c r="L9" s="2"/>
-      <c r="V9" s="22"/>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="B10" s="22"/>
+      <c r="V9" s="134"/>
+      <c r="DR9" s="134"/>
+      <c r="EB9" s="2"/>
+      <c r="EV9" s="22"/>
+    </row>
+    <row r="10" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="B10" s="134"/>
       <c r="L10" s="2"/>
-      <c r="V10" s="22"/>
-    </row>
-    <row r="11" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="22"/>
+      <c r="V10" s="134"/>
+      <c r="DR10" s="134"/>
+      <c r="EB10" s="2"/>
+      <c r="EV10" s="22"/>
+    </row>
+    <row r="11" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="134"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -3328,17 +4525,17 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
+      <c r="V11" s="135"/>
+      <c r="W11" s="137"/>
+      <c r="X11" s="132"/>
+      <c r="Y11" s="132"/>
+      <c r="Z11" s="132"/>
+      <c r="AA11" s="132"/>
+      <c r="AB11" s="132"/>
+      <c r="AC11" s="132"/>
+      <c r="AD11" s="132"/>
+      <c r="AE11" s="132"/>
+      <c r="AF11" s="132"/>
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
@@ -3349,23 +4546,76 @@
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
       <c r="AP11" s="1"/>
-    </row>
-    <row r="12" spans="1:42" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="22"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
+      <c r="BE11" s="1"/>
+      <c r="BF11" s="1"/>
+      <c r="BG11" s="1"/>
+      <c r="BH11" s="1"/>
+      <c r="BI11" s="1"/>
+      <c r="BJ11" s="1"/>
+      <c r="DR11" s="134"/>
+      <c r="DS11" s="1"/>
+      <c r="DT11" s="1"/>
+      <c r="DU11" s="1"/>
+      <c r="DV11" s="1"/>
+      <c r="DW11" s="1"/>
+      <c r="DX11" s="1"/>
+      <c r="DY11" s="1"/>
+      <c r="DZ11" s="1"/>
+      <c r="EA11" s="1"/>
+      <c r="EB11" s="3"/>
+      <c r="EV11" s="22"/>
+    </row>
+    <row r="12" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="134"/>
       <c r="L12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="AF12" s="2"/>
+      <c r="V12" s="26"/>
+      <c r="AF12" s="133"/>
+      <c r="AI12" s="41"/>
+      <c r="AK12" s="41"/>
+      <c r="AM12" s="41"/>
+      <c r="AO12" s="41"/>
       <c r="AP12" s="26"/>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="B13" s="22"/>
+      <c r="AZ12" s="115"/>
+      <c r="BJ12" s="26"/>
+      <c r="DR12" s="134"/>
+      <c r="EB12" s="2"/>
+      <c r="EV12" s="22"/>
+    </row>
+    <row r="13" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="B13" s="134"/>
       <c r="L13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="AF13" s="2"/>
-      <c r="AP13" s="22"/>
-    </row>
-    <row r="14" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="22"/>
+      <c r="V13" s="22"/>
+      <c r="AF13" s="134"/>
+      <c r="AH13" s="49"/>
+      <c r="AJ13" s="49"/>
+      <c r="AL13" s="49"/>
+      <c r="AN13" s="49"/>
+      <c r="AP13" s="37"/>
+      <c r="AW13" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="AZ13" s="2"/>
+      <c r="BJ13" s="22"/>
+      <c r="DR13" s="134"/>
+      <c r="EB13" s="2"/>
+      <c r="EV13" s="22"/>
+    </row>
+    <row r="14" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="134"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -3385,44 +4635,104 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
-      <c r="V14" s="3"/>
+      <c r="V14" s="27"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
+      <c r="Z14" s="84"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
-      <c r="AF14" s="3"/>
-      <c r="AG14" s="1"/>
+      <c r="AF14" s="135"/>
+      <c r="AG14" s="40"/>
       <c r="AH14" s="1"/>
-      <c r="AI14" s="1"/>
+      <c r="AI14" s="40"/>
       <c r="AJ14" s="1"/>
-      <c r="AK14" s="1"/>
+      <c r="AK14" s="40"/>
       <c r="AL14" s="1"/>
-      <c r="AM14" s="1"/>
+      <c r="AM14" s="40"/>
       <c r="AN14" s="1"/>
-      <c r="AO14" s="1"/>
+      <c r="AO14" s="40"/>
       <c r="AP14" s="27"/>
-    </row>
-    <row r="15" spans="1:42" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="22"/>
+      <c r="AQ14" s="23"/>
+      <c r="AR14" s="109"/>
+      <c r="AS14" s="1"/>
+      <c r="AT14" s="1"/>
+      <c r="AU14" s="109"/>
+      <c r="AV14" s="109"/>
+      <c r="AW14" s="109"/>
+      <c r="AX14" s="109"/>
+      <c r="AY14" s="109"/>
+      <c r="AZ14" s="2"/>
+      <c r="BA14" s="109"/>
+      <c r="BB14" s="109"/>
+      <c r="BC14" s="109"/>
+      <c r="BD14" s="1"/>
+      <c r="BE14" s="1"/>
+      <c r="BF14" s="109"/>
+      <c r="BG14" s="109"/>
+      <c r="BH14" s="1"/>
+      <c r="BI14" s="1"/>
+      <c r="BJ14" s="22"/>
+      <c r="DR14" s="134"/>
+      <c r="DS14" s="1"/>
+      <c r="DT14" s="1"/>
+      <c r="DU14" s="1"/>
+      <c r="DV14" s="1"/>
+      <c r="DW14" s="1"/>
+      <c r="DX14" s="1"/>
+      <c r="DY14" s="1"/>
+      <c r="DZ14" s="1"/>
+      <c r="EA14" s="1"/>
+      <c r="EB14" s="3"/>
+      <c r="EV14" s="22"/>
+    </row>
+    <row r="15" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="134"/>
       <c r="L15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="AF15" s="2"/>
+      <c r="V15" s="22"/>
+      <c r="W15" s="87"/>
+      <c r="Y15" s="41"/>
+      <c r="AA15" s="41"/>
+      <c r="AC15" s="41"/>
+      <c r="AE15" s="41"/>
+      <c r="AF15" s="134"/>
       <c r="AP15" s="22"/>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="B16" s="22"/>
+      <c r="AS15" s="26"/>
+      <c r="AT15" s="81"/>
+      <c r="AZ15" s="2"/>
+      <c r="BD15" s="26"/>
+      <c r="BJ15" s="22"/>
+      <c r="DR15" s="134"/>
+      <c r="EB15" s="2"/>
+      <c r="EV15" s="22"/>
+    </row>
+    <row r="16" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="B16" s="134"/>
       <c r="L16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="AF16" s="2"/>
+      <c r="V16" s="22"/>
+      <c r="X16" s="49"/>
+      <c r="Z16" s="49"/>
+      <c r="AB16" s="49"/>
+      <c r="AD16" s="49"/>
+      <c r="AF16" s="138"/>
       <c r="AP16" s="22"/>
-    </row>
-    <row r="17" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="22"/>
+      <c r="AS16" s="22"/>
+      <c r="AT16" s="12"/>
+      <c r="AU16" s="86" t="s">
+        <v>44</v>
+      </c>
+      <c r="AZ16" s="2"/>
+      <c r="BD16" s="22"/>
+      <c r="BJ16" s="22"/>
+      <c r="DR16" s="134"/>
+      <c r="EB16" s="2"/>
+      <c r="EV16" s="22"/>
+    </row>
+    <row r="17" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="134"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -3442,77 +4752,129 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="1"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="48"/>
       <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
+      <c r="Y17" s="40"/>
       <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
+      <c r="AA17" s="40"/>
       <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
+      <c r="AC17" s="40"/>
       <c r="AD17" s="1"/>
-      <c r="AE17" s="1"/>
-      <c r="AF17" s="3"/>
-      <c r="AG17" s="1"/>
-      <c r="AH17" s="1"/>
-      <c r="AI17" s="1"/>
-      <c r="AJ17" s="1"/>
-      <c r="AK17" s="1"/>
-      <c r="AL17" s="1"/>
-      <c r="AM17" s="1"/>
-      <c r="AN17" s="1"/>
-      <c r="AO17" s="1"/>
-      <c r="AP17" s="27"/>
-    </row>
-    <row r="18" spans="1:42" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="22"/>
+      <c r="AE17" s="40"/>
+      <c r="AF17" s="135"/>
+      <c r="AG17" s="109"/>
+      <c r="AH17" s="109"/>
+      <c r="AI17" s="109"/>
+      <c r="AJ17" s="109"/>
+      <c r="AK17" s="109"/>
+      <c r="AL17" s="109"/>
+      <c r="AM17" s="109"/>
+      <c r="AN17" s="109"/>
+      <c r="AO17" s="109"/>
+      <c r="AP17" s="22"/>
+      <c r="AQ17" s="23"/>
+      <c r="AR17" s="109"/>
+      <c r="AS17" s="27"/>
+      <c r="AT17" s="116"/>
+      <c r="AU17" s="1"/>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="1"/>
+      <c r="AY17" s="1"/>
+      <c r="AZ17" s="3"/>
+      <c r="BA17" s="1"/>
+      <c r="BB17" s="1"/>
+      <c r="BC17" s="1"/>
+      <c r="BD17" s="27"/>
+      <c r="BE17" s="23"/>
+      <c r="BF17" s="109"/>
+      <c r="BG17" s="109"/>
+      <c r="BH17" s="109"/>
+      <c r="BI17" s="1"/>
+      <c r="BJ17" s="27"/>
+      <c r="DR17" s="134"/>
+      <c r="DS17" s="1"/>
+      <c r="DT17" s="1"/>
+      <c r="DU17" s="1"/>
+      <c r="DV17" s="1"/>
+      <c r="DW17" s="1"/>
+      <c r="DX17" s="1"/>
+      <c r="DY17" s="1"/>
+      <c r="DZ17" s="1"/>
+      <c r="EA17" s="1"/>
+      <c r="EB17" s="3"/>
+      <c r="EV17" s="22"/>
+    </row>
+    <row r="18" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="134"/>
       <c r="L18" s="2"/>
       <c r="V18" s="2"/>
-      <c r="AF18" s="2"/>
+      <c r="W18" s="107"/>
+      <c r="AF18" s="136"/>
       <c r="AP18" s="22"/>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="B19" s="22"/>
+      <c r="AZ18" s="26"/>
+      <c r="BA18" s="87"/>
+      <c r="BC18" s="41"/>
+      <c r="BD18" s="26"/>
+      <c r="BH18" s="22"/>
+      <c r="BI18" s="87"/>
+      <c r="BJ18" s="26"/>
+      <c r="DR18" s="134"/>
+      <c r="EB18" s="2"/>
+      <c r="EV18" s="22"/>
+    </row>
+    <row r="19" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="B19" s="134"/>
       <c r="L19" s="2"/>
       <c r="V19" s="2"/>
-      <c r="AF19" s="2"/>
-      <c r="AK19" s="50" t="s">
+      <c r="W19" s="108"/>
+      <c r="AD19" s="50" t="s">
         <v>32</v>
       </c>
+      <c r="AF19" s="60"/>
       <c r="AP19" s="22"/>
-    </row>
-    <row r="20" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="22"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-      <c r="AD20" s="1"/>
-      <c r="AE20" s="1"/>
-      <c r="AF20" s="3"/>
+      <c r="AZ19" s="22"/>
+      <c r="BB19" s="49"/>
+      <c r="BD19" s="37"/>
+      <c r="BH19" s="22"/>
+      <c r="BJ19" s="37"/>
+      <c r="DR19" s="134"/>
+      <c r="EB19" s="2"/>
+      <c r="EV19" s="22"/>
+    </row>
+    <row r="20" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="134"/>
+      <c r="C20" s="132"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="132"/>
+      <c r="F20" s="132"/>
+      <c r="G20" s="132"/>
+      <c r="H20" s="132"/>
+      <c r="I20" s="132"/>
+      <c r="J20" s="132"/>
+      <c r="K20" s="132"/>
+      <c r="L20" s="140"/>
+      <c r="M20" s="139"/>
+      <c r="N20" s="132"/>
+      <c r="O20" s="132"/>
+      <c r="P20" s="132"/>
+      <c r="Q20" s="132"/>
+      <c r="R20" s="132"/>
+      <c r="S20" s="132"/>
+      <c r="T20" s="132"/>
+      <c r="U20" s="132"/>
+      <c r="V20" s="140"/>
+      <c r="W20" s="141"/>
+      <c r="X20" s="132"/>
+      <c r="Y20" s="132"/>
+      <c r="Z20" s="132"/>
+      <c r="AA20" s="132"/>
+      <c r="AB20" s="132"/>
+      <c r="AC20" s="132"/>
+      <c r="AD20" s="132"/>
+      <c r="AE20" s="132"/>
+      <c r="AF20" s="142"/>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
@@ -3521,32 +4883,127 @@
       <c r="AL20" s="1"/>
       <c r="AM20" s="4"/>
       <c r="AN20" s="1"/>
-      <c r="AO20" s="1"/>
+      <c r="AO20" s="57"/>
       <c r="AP20" s="27"/>
-    </row>
-    <row r="21" spans="1:42" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AQ20" s="1"/>
+      <c r="AR20" s="1"/>
+      <c r="AS20" s="1"/>
+      <c r="AT20" s="1"/>
+      <c r="AU20" s="1"/>
+      <c r="AV20" s="1"/>
+      <c r="AW20" s="4"/>
+      <c r="AX20" s="4"/>
+      <c r="AY20" s="4"/>
+      <c r="AZ20" s="27"/>
+      <c r="BA20" s="48"/>
+      <c r="BB20" s="1"/>
+      <c r="BC20" s="40"/>
+      <c r="BD20" s="27"/>
+      <c r="BE20" s="118"/>
+      <c r="BF20" s="119"/>
+      <c r="BG20" s="117"/>
+      <c r="BH20" s="27"/>
+      <c r="BI20" s="48"/>
+      <c r="BJ20" s="27"/>
+      <c r="BK20" s="25"/>
+      <c r="BL20" s="1"/>
+      <c r="BM20" s="1"/>
+      <c r="BN20" s="1"/>
+      <c r="BO20" s="1"/>
+      <c r="BP20" s="1"/>
+      <c r="BQ20" s="1"/>
+      <c r="BR20" s="1"/>
+      <c r="BS20" s="1"/>
+      <c r="BT20" s="1"/>
+      <c r="BU20" s="1"/>
+      <c r="BV20" s="1"/>
+      <c r="BW20" s="1"/>
+      <c r="BX20" s="1"/>
+      <c r="BY20" s="1"/>
+      <c r="BZ20" s="1"/>
+      <c r="CA20" s="1"/>
+      <c r="CB20" s="1"/>
+      <c r="CC20" s="1"/>
+      <c r="CD20" s="1"/>
+      <c r="CE20" s="1"/>
+      <c r="CF20" s="1"/>
+      <c r="CG20" s="1"/>
+      <c r="CH20" s="1"/>
+      <c r="CI20" s="1"/>
+      <c r="CJ20" s="1"/>
+      <c r="CK20" s="1"/>
+      <c r="CL20" s="1"/>
+      <c r="CM20" s="1"/>
+      <c r="CN20" s="1"/>
+      <c r="CO20" s="1"/>
+      <c r="CP20" s="1"/>
+      <c r="CQ20" s="1"/>
+      <c r="CR20" s="1"/>
+      <c r="CS20" s="1"/>
+      <c r="CT20" s="1"/>
+      <c r="CU20" s="1"/>
+      <c r="CV20" s="1"/>
+      <c r="CW20" s="1"/>
+      <c r="CX20" s="1"/>
+      <c r="DR20" s="134"/>
+      <c r="DS20" s="1"/>
+      <c r="DT20" s="1"/>
+      <c r="DU20" s="1"/>
+      <c r="DV20" s="1"/>
+      <c r="DW20" s="1"/>
+      <c r="DX20" s="1"/>
+      <c r="DY20" s="1"/>
+      <c r="DZ20" s="1"/>
+      <c r="EA20" s="1"/>
+      <c r="EB20" s="3"/>
+      <c r="EV20" s="22"/>
+    </row>
+    <row r="21" spans="1:152" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="22"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="87"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="45"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="93"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="44"/>
       <c r="V21" s="2"/>
-      <c r="Y21" s="52"/>
-      <c r="Z21" s="41"/>
-      <c r="AA21" s="29"/>
-      <c r="AB21" s="41"/>
-      <c r="AC21" s="26"/>
-      <c r="AD21" s="107"/>
-      <c r="AE21" s="106"/>
-      <c r="AF21" s="108"/>
-      <c r="AG21" s="92"/>
+      <c r="Y21" s="53"/>
+      <c r="Z21" s="49"/>
+      <c r="AA21" s="109"/>
+      <c r="AB21" s="49"/>
+      <c r="AC21" s="22"/>
+      <c r="AD21" s="48"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="94"/>
+      <c r="AG21" s="91"/>
       <c r="AH21" s="42"/>
       <c r="AJ21" s="41"/>
       <c r="AN21" s="87"/>
       <c r="AO21" s="29"/>
       <c r="AP21" s="42"/>
-    </row>
-    <row r="22" spans="1:42" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AZ21" s="26"/>
+      <c r="BB21" s="41"/>
+      <c r="BD21" s="42"/>
+      <c r="BJ21" s="26"/>
+      <c r="BK21" s="87"/>
+      <c r="BM21" s="41"/>
+      <c r="BO21" s="41"/>
+      <c r="BQ21" s="41"/>
+      <c r="BS21" s="41"/>
+      <c r="BT21" s="26"/>
+      <c r="BU21" s="87"/>
+      <c r="BW21" s="41"/>
+      <c r="BY21" s="41"/>
+      <c r="CA21" s="41"/>
+      <c r="CC21" s="41"/>
+      <c r="CD21" s="26"/>
+      <c r="CE21" s="87"/>
+      <c r="CF21" s="26"/>
+      <c r="CN21" s="2"/>
+      <c r="CX21" s="22"/>
+      <c r="DR21" s="134"/>
+      <c r="EB21" s="2"/>
+      <c r="EV21" s="22"/>
+    </row>
+    <row r="22" spans="1:152" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="22"/>
       <c r="J22" s="22"/>
       <c r="K22" s="23"/>
@@ -3556,121 +5013,227 @@
       <c r="Z22" s="53"/>
       <c r="AA22" s="40"/>
       <c r="AB22" s="1"/>
-      <c r="AC22" s="95"/>
-      <c r="AD22" s="105"/>
-      <c r="AE22" s="105"/>
-      <c r="AF22" s="109"/>
+      <c r="AC22" s="94"/>
+      <c r="AD22" s="150" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE22" s="150" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF22" s="151" t="s">
+        <v>25</v>
+      </c>
       <c r="AG22" s="48"/>
       <c r="AH22" s="27"/>
-      <c r="AI22" s="94"/>
+      <c r="AI22" s="93"/>
       <c r="AN22" s="23"/>
       <c r="AO22" s="49"/>
       <c r="AP22" s="22"/>
-    </row>
-    <row r="23" spans="1:42" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AZ22" s="22"/>
+      <c r="BA22" s="93"/>
+      <c r="BC22" s="49"/>
+      <c r="BD22" s="22"/>
+      <c r="BJ22" s="22"/>
+      <c r="BL22" s="49"/>
+      <c r="BN22" s="49"/>
+      <c r="BP22" s="49"/>
+      <c r="BR22" s="49"/>
+      <c r="BT22" s="37"/>
+      <c r="BV22" s="49"/>
+      <c r="BX22" s="49"/>
+      <c r="BZ22" s="49"/>
+      <c r="CB22" s="49"/>
+      <c r="CD22" s="37"/>
+      <c r="CF22" s="37"/>
+      <c r="CN22" s="2"/>
+      <c r="CX22" s="22"/>
+      <c r="DR22" s="134"/>
+      <c r="EB22" s="2"/>
+      <c r="EV22" s="22"/>
+    </row>
+    <row r="23" spans="1:152" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="22"/>
       <c r="C23" s="23"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
       <c r="J23" s="22"/>
-      <c r="K23" s="94"/>
+      <c r="K23" s="93"/>
       <c r="L23" s="22"/>
       <c r="M23" s="44"/>
-      <c r="N23" s="88"/>
-      <c r="O23" s="88"/>
-      <c r="P23" s="88"/>
-      <c r="Q23" s="88"/>
-      <c r="R23" s="88"/>
-      <c r="S23" s="88"/>
-      <c r="T23" s="88"/>
-      <c r="U23" s="88"/>
       <c r="V23" s="2"/>
       <c r="W23" s="28"/>
-      <c r="X23" s="88"/>
-      <c r="Y23" s="88"/>
-      <c r="Z23" s="88"/>
-      <c r="AA23" s="105"/>
-      <c r="AB23" s="88"/>
+      <c r="AA23" s="150" t="s">
+        <v>25</v>
+      </c>
       <c r="AC23" s="22"/>
-      <c r="AD23" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE23" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF23" s="112" t="s">
-        <v>25</v>
-      </c>
-      <c r="AG23" s="88"/>
-      <c r="AH23" s="88"/>
-      <c r="AI23" s="88"/>
-      <c r="AJ23" s="88"/>
-      <c r="AK23" s="88"/>
-      <c r="AL23" s="88"/>
-      <c r="AM23" s="95"/>
+      <c r="AD23" s="103"/>
+      <c r="AE23" s="104"/>
+      <c r="AF23" s="105"/>
+      <c r="AM23" s="94"/>
       <c r="AN23" s="48"/>
       <c r="AO23" s="1"/>
-      <c r="AP23" s="95"/>
-    </row>
-    <row r="24" spans="1:42" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AP23" s="94"/>
+      <c r="AQ23" s="1"/>
+      <c r="AR23" s="1"/>
+      <c r="AS23" s="109"/>
+      <c r="AT23" s="109"/>
+      <c r="AU23" s="109"/>
+      <c r="AV23" s="1"/>
+      <c r="AW23" s="1"/>
+      <c r="AX23" s="1"/>
+      <c r="AY23" s="1"/>
+      <c r="AZ23" s="27"/>
+      <c r="BA23" s="23"/>
+      <c r="BB23" s="49"/>
+      <c r="BC23" s="109"/>
+      <c r="BD23" s="94"/>
+      <c r="BE23" s="109"/>
+      <c r="BF23" s="109"/>
+      <c r="BG23" s="1"/>
+      <c r="BH23" s="1"/>
+      <c r="BI23" s="1"/>
+      <c r="BJ23" s="27"/>
+      <c r="BK23" s="93"/>
+      <c r="BL23" s="109"/>
+      <c r="BM23" s="49"/>
+      <c r="BN23" s="109"/>
+      <c r="BO23" s="49"/>
+      <c r="BP23" s="109"/>
+      <c r="BQ23" s="49"/>
+      <c r="BR23" s="109"/>
+      <c r="BS23" s="49"/>
+      <c r="BT23" s="22"/>
+      <c r="BU23" s="48"/>
+      <c r="BV23" s="1"/>
+      <c r="BW23" s="40"/>
+      <c r="BX23" s="1"/>
+      <c r="BY23" s="40"/>
+      <c r="BZ23" s="1"/>
+      <c r="CA23" s="40"/>
+      <c r="CB23" s="1"/>
+      <c r="CC23" s="40"/>
+      <c r="CD23" s="27"/>
+      <c r="CE23" s="48"/>
+      <c r="CF23" s="27"/>
+      <c r="CG23" s="109"/>
+      <c r="CH23" s="109"/>
+      <c r="CI23" s="1"/>
+      <c r="CJ23" s="1"/>
+      <c r="CK23" s="1"/>
+      <c r="CL23" s="1"/>
+      <c r="CM23" s="1"/>
+      <c r="CN23" s="3"/>
+      <c r="CO23" s="1"/>
+      <c r="CP23" s="1"/>
+      <c r="CQ23" s="14">
+        <v>2</v>
+      </c>
+      <c r="CR23" s="109"/>
+      <c r="CS23" s="109"/>
+      <c r="CT23" s="109"/>
+      <c r="CU23" s="109"/>
+      <c r="CV23" s="109"/>
+      <c r="CW23" s="109"/>
+      <c r="CX23" s="22"/>
+      <c r="DR23" s="134"/>
+      <c r="DS23" s="1"/>
+      <c r="DT23" s="1"/>
+      <c r="DU23" s="1"/>
+      <c r="DV23" s="1"/>
+      <c r="DW23" s="1"/>
+      <c r="DX23" s="1"/>
+      <c r="DY23" s="1"/>
+      <c r="DZ23" s="1"/>
+      <c r="EA23" s="1"/>
+      <c r="EB23" s="3"/>
+      <c r="EV23" s="22"/>
+    </row>
+    <row r="24" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B24" s="22"/>
       <c r="J24" s="22"/>
       <c r="K24" s="23"/>
       <c r="L24" s="37"/>
       <c r="M24" s="22"/>
       <c r="V24" s="2"/>
-      <c r="AA24" s="96" t="s">
-        <v>25</v>
-      </c>
+      <c r="AA24" s="95"/>
       <c r="AD24" s="75">
         <v>1</v>
       </c>
       <c r="AF24" s="22"/>
       <c r="AP24" s="26"/>
-    </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AZ24" s="26"/>
+      <c r="BA24" s="93"/>
+      <c r="BC24" s="37"/>
+      <c r="BJ24" s="22"/>
+      <c r="BL24" s="49"/>
+      <c r="BN24" s="49"/>
+      <c r="BP24" s="49"/>
+      <c r="BR24" s="49"/>
+      <c r="BT24" s="37"/>
+      <c r="BX24" s="15"/>
+      <c r="BY24" s="15"/>
+      <c r="CB24" s="15"/>
+      <c r="CC24" s="15"/>
+      <c r="CD24" s="2"/>
+      <c r="CH24" s="22"/>
+      <c r="CI24" s="87"/>
+      <c r="CK24" s="41"/>
+      <c r="CM24" s="41"/>
+      <c r="CN24" s="26"/>
+      <c r="CO24" s="87"/>
+      <c r="CQ24" s="42"/>
+      <c r="CX24" s="22"/>
+      <c r="DR24" s="134"/>
+      <c r="EB24" s="2"/>
+      <c r="EV24" s="22"/>
+    </row>
+    <row r="25" spans="1:152" x14ac:dyDescent="0.3">
       <c r="B25" s="22"/>
       <c r="J25" s="22"/>
-      <c r="K25" s="94"/>
+      <c r="K25" s="93"/>
       <c r="L25" s="22"/>
       <c r="M25" s="44"/>
       <c r="V25" s="2"/>
       <c r="AF25" s="60"/>
       <c r="AP25" s="2"/>
-    </row>
-    <row r="26" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AZ25" s="22"/>
+      <c r="BB25" s="49"/>
+      <c r="BC25" s="22"/>
+      <c r="BJ25" s="22"/>
+      <c r="BK25" s="93"/>
+      <c r="BM25" s="49"/>
+      <c r="BO25" s="49"/>
+      <c r="BQ25" s="49"/>
+      <c r="BS25" s="49"/>
+      <c r="BT25" s="22"/>
+      <c r="BX25" s="15"/>
+      <c r="BY25" s="15"/>
+      <c r="CB25" s="15"/>
+      <c r="CC25" s="15"/>
+      <c r="CD25" s="2"/>
+      <c r="CH25" s="22"/>
+      <c r="CJ25" s="49"/>
+      <c r="CL25" s="49"/>
+      <c r="CN25" s="37"/>
+      <c r="CP25" s="49"/>
+      <c r="CQ25" s="22"/>
+      <c r="CX25" s="22"/>
+      <c r="DR25" s="134"/>
+      <c r="EB25" s="2"/>
+      <c r="EV25" s="22"/>
+    </row>
+    <row r="26" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="22"/>
       <c r="C26" s="23"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
       <c r="J26" s="22"/>
       <c r="K26" s="25"/>
-      <c r="L26" s="95"/>
+      <c r="L26" s="94"/>
       <c r="M26" s="27"/>
-      <c r="N26" s="88"/>
-      <c r="O26" s="88"/>
-      <c r="P26" s="88"/>
-      <c r="Q26" s="88"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
+      <c r="T26" s="106"/>
       <c r="U26" s="1"/>
       <c r="V26" s="3"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
-      <c r="Y26" s="88"/>
-      <c r="Z26" s="88"/>
-      <c r="AA26" s="88"/>
-      <c r="AB26" s="88"/>
-      <c r="AC26" s="88"/>
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
       <c r="AF26" s="61"/>
@@ -3684,58 +5247,219 @@
       <c r="AN26" s="1"/>
       <c r="AO26" s="1"/>
       <c r="AP26" s="3"/>
-    </row>
-    <row r="27" spans="1:42" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="89" t="s">
+      <c r="AQ26" s="1"/>
+      <c r="AR26" s="1"/>
+      <c r="AS26" s="1"/>
+      <c r="AT26" s="1"/>
+      <c r="AU26" s="1"/>
+      <c r="AV26" s="1"/>
+      <c r="AW26" s="57"/>
+      <c r="AX26" s="1"/>
+      <c r="AY26" s="1"/>
+      <c r="AZ26" s="27"/>
+      <c r="BA26" s="48"/>
+      <c r="BB26" s="1"/>
+      <c r="BC26" s="94"/>
+      <c r="BD26" s="109"/>
+      <c r="BE26" s="109"/>
+      <c r="BF26" s="109"/>
+      <c r="BG26" s="109"/>
+      <c r="BH26" s="109"/>
+      <c r="BI26" s="109"/>
+      <c r="BJ26" s="22"/>
+      <c r="BK26" s="1"/>
+      <c r="BL26" s="40"/>
+      <c r="BM26" s="1"/>
+      <c r="BN26" s="40"/>
+      <c r="BO26" s="1"/>
+      <c r="BP26" s="40"/>
+      <c r="BQ26" s="1"/>
+      <c r="BR26" s="40"/>
+      <c r="BS26" s="1"/>
+      <c r="BT26" s="94"/>
+      <c r="BU26" s="1"/>
+      <c r="BW26" s="1"/>
+      <c r="BX26" s="120"/>
+      <c r="BY26" s="123" t="s">
+        <v>47</v>
+      </c>
+      <c r="BZ26" s="121" t="s">
+        <v>47</v>
+      </c>
+      <c r="CA26" s="121" t="s">
+        <v>47</v>
+      </c>
+      <c r="CB26" s="122" t="s">
+        <v>47</v>
+      </c>
+      <c r="CC26" s="90"/>
+      <c r="CD26" s="3"/>
+      <c r="CE26" s="1"/>
+      <c r="CF26" s="1"/>
+      <c r="CG26" s="1"/>
+      <c r="CH26" s="27"/>
+      <c r="CI26" s="93"/>
+      <c r="CJ26" s="109"/>
+      <c r="CK26" s="49"/>
+      <c r="CL26" s="109"/>
+      <c r="CM26" s="49"/>
+      <c r="CN26" s="22"/>
+      <c r="CO26" s="93"/>
+      <c r="CP26" s="109"/>
+      <c r="CQ26" s="37"/>
+      <c r="CR26" s="153" t="s">
+        <v>47</v>
+      </c>
+      <c r="CS26" s="121" t="s">
+        <v>47</v>
+      </c>
+      <c r="CT26" s="121" t="s">
+        <v>47</v>
+      </c>
+      <c r="CU26" s="121" t="s">
+        <v>47</v>
+      </c>
+      <c r="CV26" s="154" t="s">
+        <v>47</v>
+      </c>
+      <c r="CW26" s="154" t="s">
+        <v>47</v>
+      </c>
+      <c r="CX26" s="155" t="s">
+        <v>47</v>
+      </c>
+      <c r="DR26" s="134"/>
+      <c r="DS26" s="1"/>
+      <c r="DT26" s="1"/>
+      <c r="DU26" s="1"/>
+      <c r="DV26" s="1"/>
+      <c r="DW26" s="1"/>
+      <c r="DX26" s="1"/>
+      <c r="DY26" s="1"/>
+      <c r="DZ26" s="1"/>
+      <c r="EA26" s="1"/>
+      <c r="EB26" s="3"/>
+      <c r="EV26" s="22"/>
+    </row>
+    <row r="27" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="K27" s="98"/>
-      <c r="L27" s="99"/>
-      <c r="M27" s="102"/>
+      <c r="K27" s="97"/>
+      <c r="L27" s="98"/>
+      <c r="M27" s="100"/>
       <c r="R27" s="26"/>
-      <c r="S27" s="87"/>
+      <c r="S27" s="93"/>
       <c r="U27" s="41"/>
       <c r="V27" s="26"/>
       <c r="AD27" s="26"/>
       <c r="AE27" s="87"/>
       <c r="AF27" s="26"/>
-      <c r="AG27" s="98"/>
-      <c r="AH27" s="98"/>
-      <c r="AI27" s="98"/>
-      <c r="AJ27" s="98"/>
-      <c r="AK27" s="98"/>
-      <c r="AL27" s="98"/>
-      <c r="AM27" s="98"/>
-      <c r="AN27" s="98"/>
-      <c r="AO27" s="98"/>
-      <c r="AP27" s="99"/>
-    </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AG27" s="97"/>
+      <c r="AH27" s="97"/>
+      <c r="AI27" s="97"/>
+      <c r="AJ27" s="97"/>
+      <c r="AK27" s="97"/>
+      <c r="AL27" s="97"/>
+      <c r="AM27" s="97"/>
+      <c r="AN27" s="97"/>
+      <c r="AO27" s="15"/>
+      <c r="AP27" s="98"/>
+      <c r="AQ27" s="15"/>
+      <c r="AR27" s="15"/>
+      <c r="AS27" s="97"/>
+      <c r="AT27" s="15"/>
+      <c r="AU27" s="15"/>
+      <c r="AV27" s="15"/>
+      <c r="AW27" s="15"/>
+      <c r="AX27" s="15"/>
+      <c r="AY27" s="15"/>
+      <c r="AZ27" s="99"/>
+      <c r="BA27" s="15"/>
+      <c r="BB27" s="15"/>
+      <c r="BC27" s="15"/>
+      <c r="BJ27" s="22"/>
+      <c r="BT27" s="2"/>
+      <c r="BW27" s="26"/>
+      <c r="BY27" s="124"/>
+      <c r="BZ27" s="87"/>
+      <c r="CA27" s="29"/>
+      <c r="CB27" s="41"/>
+      <c r="CD27" s="42"/>
+      <c r="CF27" s="41"/>
+      <c r="CH27" s="41"/>
+      <c r="CJ27" s="49"/>
+      <c r="CL27" s="49"/>
+      <c r="CN27" s="37"/>
+      <c r="CP27" s="49"/>
+      <c r="CR27" s="42"/>
+      <c r="CW27" s="21">
+        <v>2</v>
+      </c>
+      <c r="CX27" s="22"/>
+      <c r="DR27" s="134"/>
+      <c r="EB27" s="2"/>
+      <c r="EV27" s="22"/>
+    </row>
+    <row r="28" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>43</v>
       </c>
       <c r="B28" s="60"/>
-      <c r="K28" s="100"/>
-      <c r="L28" s="101"/>
-      <c r="M28" s="103"/>
-      <c r="N28" s="88"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="99"/>
+      <c r="M28" s="101"/>
       <c r="R28" s="22"/>
       <c r="T28" s="49"/>
       <c r="V28" s="37"/>
       <c r="AD28" s="22"/>
       <c r="AF28" s="37"/>
-      <c r="AG28" s="100"/>
-      <c r="AH28" s="100"/>
-      <c r="AI28" s="100"/>
-      <c r="AJ28" s="100"/>
-      <c r="AK28" s="100"/>
-      <c r="AL28" s="100"/>
-      <c r="AM28" s="100"/>
-      <c r="AN28" s="100"/>
-      <c r="AO28" s="100"/>
-      <c r="AP28" s="101"/>
-    </row>
-    <row r="29" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AG28" s="15"/>
+      <c r="AH28" s="15"/>
+      <c r="AI28" s="15"/>
+      <c r="AJ28" s="15"/>
+      <c r="AK28" s="15"/>
+      <c r="AL28" s="15"/>
+      <c r="AM28" s="15"/>
+      <c r="AN28" s="15"/>
+      <c r="AO28" s="15"/>
+      <c r="AP28" s="99"/>
+      <c r="AQ28" s="15"/>
+      <c r="AR28" s="15"/>
+      <c r="AS28" s="114"/>
+      <c r="AT28" s="15"/>
+      <c r="AU28" s="15"/>
+      <c r="AV28" s="15"/>
+      <c r="AW28" s="15"/>
+      <c r="AX28" s="15"/>
+      <c r="AY28" s="15"/>
+      <c r="AZ28" s="99"/>
+      <c r="BA28" s="15"/>
+      <c r="BB28" s="15"/>
+      <c r="BC28" s="15"/>
+      <c r="BJ28" s="60"/>
+      <c r="BT28" s="2"/>
+      <c r="BW28" s="22"/>
+      <c r="BY28" s="22"/>
+      <c r="CA28" s="49"/>
+      <c r="CC28" s="49"/>
+      <c r="CD28" s="22"/>
+      <c r="CE28" s="93"/>
+      <c r="CG28" s="49"/>
+      <c r="CI28" s="49"/>
+      <c r="CK28" s="49"/>
+      <c r="CM28" s="49"/>
+      <c r="CN28" s="22"/>
+      <c r="CO28" s="93"/>
+      <c r="CP28" s="1"/>
+      <c r="CQ28" s="40"/>
+      <c r="CR28" s="27"/>
+      <c r="CX28" s="22"/>
+      <c r="DR28" s="134"/>
+      <c r="EB28" s="2"/>
+      <c r="EV28" s="22"/>
+    </row>
+    <row r="29" spans="1:152" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="60"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -3745,14 +5469,14 @@
       <c r="H29" s="1"/>
       <c r="I29" s="58"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="91"/>
-      <c r="L29" s="93"/>
-      <c r="M29" s="91"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="92"/>
+      <c r="M29" s="90"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="54"/>
       <c r="Q29" s="54"/>
-      <c r="R29" s="90"/>
+      <c r="R29" s="89"/>
       <c r="S29" s="48"/>
       <c r="T29" s="1"/>
       <c r="U29" s="40"/>
@@ -3769,18 +5493,1245 @@
       <c r="AD29" s="27"/>
       <c r="AE29" s="48"/>
       <c r="AF29" s="27"/>
-      <c r="AG29" s="104"/>
-      <c r="AH29" s="91"/>
-      <c r="AI29" s="91"/>
-      <c r="AJ29" s="91"/>
-      <c r="AK29" s="91"/>
-      <c r="AL29" s="91"/>
+      <c r="AG29" s="102"/>
+      <c r="AH29" s="90"/>
+      <c r="AI29" s="90"/>
+      <c r="AJ29" s="90"/>
+      <c r="AK29" s="90"/>
+      <c r="AL29" s="90"/>
       <c r="AM29" s="84"/>
-      <c r="AN29" s="91"/>
-      <c r="AO29" s="91"/>
-      <c r="AP29" s="93"/>
-    </row>
-    <row r="30" spans="1:42" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="AN29" s="90"/>
+      <c r="AO29" s="90"/>
+      <c r="AP29" s="92"/>
+      <c r="AQ29" s="90"/>
+      <c r="AR29" s="90"/>
+      <c r="AS29" s="90"/>
+      <c r="AT29" s="90"/>
+      <c r="AU29" s="90"/>
+      <c r="AV29" s="90"/>
+      <c r="AW29" s="90"/>
+      <c r="AX29" s="90"/>
+      <c r="AY29" s="90"/>
+      <c r="AZ29" s="92"/>
+      <c r="BA29" s="90"/>
+      <c r="BB29" s="84"/>
+      <c r="BC29" s="90"/>
+      <c r="BD29" s="1"/>
+      <c r="BE29" s="1"/>
+      <c r="BF29" s="1"/>
+      <c r="BG29" s="1"/>
+      <c r="BH29" s="1"/>
+      <c r="BI29" s="1"/>
+      <c r="BJ29" s="61"/>
+      <c r="BK29" s="146"/>
+      <c r="BL29" s="132"/>
+      <c r="BM29" s="132"/>
+      <c r="BN29" s="132"/>
+      <c r="BO29" s="132"/>
+      <c r="BP29" s="147"/>
+      <c r="BQ29" s="132"/>
+      <c r="BR29" s="132"/>
+      <c r="BS29" s="132"/>
+      <c r="BT29" s="140"/>
+      <c r="BU29" s="1"/>
+      <c r="BV29" s="1"/>
+      <c r="BW29" s="27"/>
+      <c r="BX29" s="125"/>
+      <c r="BY29" s="35"/>
+      <c r="BZ29" s="48"/>
+      <c r="CA29" s="1"/>
+      <c r="CB29" s="40"/>
+      <c r="CC29" s="1"/>
+      <c r="CD29" s="94"/>
+      <c r="CE29" s="1"/>
+      <c r="CF29" s="40"/>
+      <c r="CG29" s="1"/>
+      <c r="CH29" s="40"/>
+      <c r="CI29" s="1"/>
+      <c r="CJ29" s="40"/>
+      <c r="CK29" s="1"/>
+      <c r="CL29" s="40"/>
+      <c r="CM29" s="1"/>
+      <c r="CN29" s="94"/>
+      <c r="CO29" s="156"/>
+      <c r="CP29" s="4"/>
+      <c r="CQ29" s="1"/>
+      <c r="CR29" s="1"/>
+      <c r="CS29" s="1"/>
+      <c r="CT29" s="1"/>
+      <c r="CU29" s="1"/>
+      <c r="CV29" s="1"/>
+      <c r="CW29" s="54"/>
+      <c r="CX29" s="89"/>
+      <c r="DR29" s="134"/>
+      <c r="DS29" s="1"/>
+      <c r="DT29" s="1"/>
+      <c r="DU29" s="1"/>
+      <c r="DV29" s="1"/>
+      <c r="DW29" s="1"/>
+      <c r="DX29" s="1"/>
+      <c r="DY29" s="1"/>
+      <c r="DZ29" s="1"/>
+      <c r="EA29" s="1"/>
+      <c r="EB29" s="3"/>
+      <c r="EV29" s="22"/>
+    </row>
+    <row r="30" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="BJ30" s="136"/>
+      <c r="BK30" s="49"/>
+      <c r="BM30" s="49"/>
+      <c r="BO30" s="49"/>
+      <c r="BQ30" s="49"/>
+      <c r="BS30" s="49"/>
+      <c r="BT30" s="133"/>
+      <c r="CA30" s="22"/>
+      <c r="CC30" s="41"/>
+      <c r="CD30" s="26"/>
+      <c r="CM30" s="26"/>
+      <c r="CN30" s="26"/>
+      <c r="CO30" s="45"/>
+      <c r="CP30" s="22"/>
+      <c r="CQ30" s="87"/>
+      <c r="CS30" s="41"/>
+      <c r="CU30" s="41"/>
+      <c r="CV30" s="26"/>
+      <c r="CX30" s="157"/>
+      <c r="DR30" s="134"/>
+      <c r="EB30" s="2"/>
+      <c r="EV30" s="22"/>
+    </row>
+    <row r="31" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ31" s="134"/>
+      <c r="BL31" s="49"/>
+      <c r="BN31" s="49"/>
+      <c r="BP31" s="49"/>
+      <c r="BR31" s="49"/>
+      <c r="BT31" s="138"/>
+      <c r="CA31" s="22"/>
+      <c r="CB31" s="93"/>
+      <c r="CD31" s="37"/>
+      <c r="CM31" s="22"/>
+      <c r="CN31" s="43"/>
+      <c r="CO31" s="27"/>
+      <c r="CP31" s="22"/>
+      <c r="CR31" s="49"/>
+      <c r="CT31" s="49"/>
+      <c r="CV31" s="37"/>
+      <c r="CX31" s="22"/>
+      <c r="DR31" s="134"/>
+      <c r="EB31" s="2"/>
+      <c r="EV31" s="22"/>
+    </row>
+    <row r="32" spans="1:152" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ32" s="134"/>
+      <c r="BK32" s="40"/>
+      <c r="BL32" s="1"/>
+      <c r="BM32" s="40"/>
+      <c r="BN32" s="1"/>
+      <c r="BO32" s="40"/>
+      <c r="BP32" s="1"/>
+      <c r="BQ32" s="40"/>
+      <c r="BR32" s="1"/>
+      <c r="BS32" s="40"/>
+      <c r="BT32" s="135"/>
+      <c r="BU32" s="109"/>
+      <c r="BV32" s="109"/>
+      <c r="BW32" s="109"/>
+      <c r="BX32" s="1"/>
+      <c r="BY32" s="1"/>
+      <c r="BZ32" s="1"/>
+      <c r="CA32" s="27"/>
+      <c r="CB32" s="23"/>
+      <c r="CC32" s="49"/>
+      <c r="CD32" s="22"/>
+      <c r="CE32" s="23"/>
+      <c r="CF32" s="109"/>
+      <c r="CG32" s="109"/>
+      <c r="CH32" s="109"/>
+      <c r="CI32" s="1"/>
+      <c r="CJ32" s="1"/>
+      <c r="CK32" s="1"/>
+      <c r="CL32" s="1"/>
+      <c r="CM32" s="1"/>
+      <c r="CN32" s="3"/>
+      <c r="CO32" s="110"/>
+      <c r="CP32" s="27"/>
+      <c r="CQ32" s="48"/>
+      <c r="CR32" s="1"/>
+      <c r="CS32" s="40"/>
+      <c r="CT32" s="1"/>
+      <c r="CU32" s="40"/>
+      <c r="CV32" s="27"/>
+      <c r="CW32" s="1"/>
+      <c r="CX32" s="27"/>
+      <c r="DR32" s="134"/>
+      <c r="DS32" s="1"/>
+      <c r="DT32" s="1"/>
+      <c r="DU32" s="1"/>
+      <c r="DV32" s="1"/>
+      <c r="DW32" s="1"/>
+      <c r="DX32" s="1"/>
+      <c r="DY32" s="1"/>
+      <c r="DZ32" s="1"/>
+      <c r="EA32" s="1"/>
+      <c r="EB32" s="3"/>
+      <c r="EV32" s="22"/>
+    </row>
+    <row r="33" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="BJ33" s="134"/>
+      <c r="BT33" s="134"/>
+      <c r="BW33" s="22"/>
+      <c r="BX33" s="87"/>
+      <c r="BZ33" s="41"/>
+      <c r="CB33" s="49"/>
+      <c r="CD33" s="37"/>
+      <c r="CL33" s="64"/>
+      <c r="CN33" s="115"/>
+      <c r="CV33" s="109"/>
+      <c r="CW33" s="109"/>
+      <c r="CX33" s="22"/>
+      <c r="DR33" s="134"/>
+      <c r="EB33" s="2"/>
+      <c r="EV33" s="22"/>
+    </row>
+    <row r="34" spans="62:172" x14ac:dyDescent="0.3">
+      <c r="BJ34" s="134"/>
+      <c r="BT34" s="134"/>
+      <c r="BW34" s="22"/>
+      <c r="BX34" s="23"/>
+      <c r="BY34" s="49"/>
+      <c r="CA34" s="49"/>
+      <c r="CC34" s="49"/>
+      <c r="CD34" s="22"/>
+      <c r="CL34" s="65"/>
+      <c r="CM34" s="161">
+        <v>3</v>
+      </c>
+      <c r="CN34" s="2"/>
+      <c r="CV34" s="109"/>
+      <c r="CW34" s="109"/>
+      <c r="CX34" s="22"/>
+      <c r="DR34" s="134"/>
+      <c r="EB34" s="2"/>
+      <c r="EV34" s="22"/>
+    </row>
+    <row r="35" spans="62:172" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ35" s="134"/>
+      <c r="BK35" s="109"/>
+      <c r="BL35" s="109"/>
+      <c r="BM35" s="109"/>
+      <c r="BN35" s="109"/>
+      <c r="BO35" s="109"/>
+      <c r="BP35" s="109"/>
+      <c r="BQ35" s="127" t="s">
+        <v>32</v>
+      </c>
+      <c r="BR35" s="109"/>
+      <c r="BS35" s="109"/>
+      <c r="BT35" s="134"/>
+      <c r="BU35" s="109"/>
+      <c r="BV35" s="109"/>
+      <c r="BW35" s="22"/>
+      <c r="BX35" s="93"/>
+      <c r="BY35" s="109"/>
+      <c r="BZ35" s="49"/>
+      <c r="CA35" s="109"/>
+      <c r="CB35" s="49"/>
+      <c r="CC35" s="109"/>
+      <c r="CD35" s="37"/>
+      <c r="CE35" s="1"/>
+      <c r="CF35" s="77">
+        <v>3</v>
+      </c>
+      <c r="CG35" s="1"/>
+      <c r="CH35" s="158"/>
+      <c r="CI35" s="1"/>
+      <c r="CJ35" s="1"/>
+      <c r="CK35" s="1"/>
+      <c r="CL35" s="66"/>
+      <c r="CM35" s="1"/>
+      <c r="CN35" s="3"/>
+      <c r="CO35" s="1"/>
+      <c r="CP35" s="1"/>
+      <c r="CQ35" s="109"/>
+      <c r="CR35" s="109"/>
+      <c r="CS35" s="1"/>
+      <c r="CT35" s="1"/>
+      <c r="CU35" s="1"/>
+      <c r="CV35" s="109"/>
+      <c r="CW35" s="109"/>
+      <c r="CX35" s="27"/>
+      <c r="DR35" s="134"/>
+      <c r="DS35" s="1"/>
+      <c r="DT35" s="1"/>
+      <c r="DU35" s="1"/>
+      <c r="DV35" s="1"/>
+      <c r="DW35" s="1"/>
+      <c r="DX35" s="1"/>
+      <c r="DY35" s="1"/>
+      <c r="DZ35" s="1"/>
+      <c r="EA35" s="1"/>
+      <c r="EB35" s="3"/>
+      <c r="EV35" s="22"/>
+    </row>
+    <row r="36" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="BJ36" s="134"/>
+      <c r="BT36" s="134"/>
+      <c r="BW36" s="22"/>
+      <c r="BX36" s="23"/>
+      <c r="BY36" s="49"/>
+      <c r="CA36" s="49"/>
+      <c r="CC36" s="49"/>
+      <c r="CD36" s="22"/>
+      <c r="CN36" s="2"/>
+      <c r="CR36" s="109"/>
+      <c r="CS36" s="109"/>
+      <c r="CU36" s="26"/>
+      <c r="CW36" s="22"/>
+      <c r="CX36" s="45"/>
+      <c r="DR36" s="134"/>
+      <c r="EB36" s="2"/>
+      <c r="EV36" s="22"/>
+    </row>
+    <row r="37" spans="62:172" x14ac:dyDescent="0.3">
+      <c r="BJ37" s="134"/>
+      <c r="BT37" s="60"/>
+      <c r="BW37" s="22"/>
+      <c r="BX37" s="93"/>
+      <c r="BZ37" s="49"/>
+      <c r="CB37" s="49"/>
+      <c r="CD37" s="37"/>
+      <c r="CN37" s="2"/>
+      <c r="CR37" s="109"/>
+      <c r="CS37" s="109"/>
+      <c r="CT37" s="109"/>
+      <c r="CU37" s="22"/>
+      <c r="CW37" s="22"/>
+      <c r="CX37" s="22"/>
+      <c r="DR37" s="134"/>
+      <c r="DX37" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="EB37" s="2"/>
+      <c r="EV37" s="22"/>
+    </row>
+    <row r="38" spans="62:172" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ38" s="134"/>
+      <c r="BK38" s="1"/>
+      <c r="BL38" s="131"/>
+      <c r="BM38" s="131"/>
+      <c r="BN38" s="1"/>
+      <c r="BO38" s="1"/>
+      <c r="BP38" s="1"/>
+      <c r="BQ38" s="1"/>
+      <c r="BR38" s="57"/>
+      <c r="BS38" s="1"/>
+      <c r="BT38" s="61"/>
+      <c r="BU38" s="132"/>
+      <c r="BV38" s="132"/>
+      <c r="BW38" s="145"/>
+      <c r="BX38" s="143"/>
+      <c r="BY38" s="148"/>
+      <c r="BZ38" s="132"/>
+      <c r="CA38" s="148"/>
+      <c r="CB38" s="132"/>
+      <c r="CC38" s="148"/>
+      <c r="CD38" s="145"/>
+      <c r="CE38" s="143"/>
+      <c r="CF38" s="84"/>
+      <c r="CG38" s="132"/>
+      <c r="CH38" s="132"/>
+      <c r="CI38" s="132"/>
+      <c r="CJ38" s="132"/>
+      <c r="CK38" s="158"/>
+      <c r="CL38" s="132"/>
+      <c r="CM38" s="132"/>
+      <c r="CN38" s="140"/>
+      <c r="CO38" s="110"/>
+      <c r="CP38" s="1"/>
+      <c r="CQ38" s="85"/>
+      <c r="CR38" s="162">
+        <v>4</v>
+      </c>
+      <c r="CS38" s="1"/>
+      <c r="CT38" s="1"/>
+      <c r="CU38" s="27"/>
+      <c r="CV38" s="4"/>
+      <c r="CW38" s="35"/>
+      <c r="CX38" s="43"/>
+      <c r="CY38" s="25"/>
+      <c r="CZ38" s="1"/>
+      <c r="DA38" s="1"/>
+      <c r="DB38" s="1"/>
+      <c r="DC38" s="1"/>
+      <c r="DD38" s="1"/>
+      <c r="DE38" s="1"/>
+      <c r="DF38" s="1"/>
+      <c r="DG38" s="1"/>
+      <c r="DH38" s="1"/>
+      <c r="DI38" s="1"/>
+      <c r="DJ38" s="1"/>
+      <c r="DK38" s="1"/>
+      <c r="DL38" s="1"/>
+      <c r="DM38" s="1"/>
+      <c r="DN38" s="1"/>
+      <c r="DO38" s="1"/>
+      <c r="DP38" s="1"/>
+      <c r="DQ38" s="1"/>
+      <c r="DR38" s="135"/>
+      <c r="DS38" s="137"/>
+      <c r="DT38" s="132"/>
+      <c r="DU38" s="132"/>
+      <c r="DV38" s="132"/>
+      <c r="DW38" s="132"/>
+      <c r="DX38" s="132"/>
+      <c r="DY38" s="132"/>
+      <c r="DZ38" s="132"/>
+      <c r="EA38" s="132"/>
+      <c r="EB38" s="140"/>
+      <c r="EC38" s="1"/>
+      <c r="ED38" s="1"/>
+      <c r="EE38" s="1"/>
+      <c r="EF38" s="1"/>
+      <c r="EG38" s="1"/>
+      <c r="EH38" s="1"/>
+      <c r="EI38" s="1"/>
+      <c r="EJ38" s="1"/>
+      <c r="EK38" s="1"/>
+      <c r="EL38" s="1"/>
+      <c r="EM38" s="1"/>
+      <c r="EN38" s="1"/>
+      <c r="EO38" s="1"/>
+      <c r="EP38" s="1"/>
+      <c r="EQ38" s="1"/>
+      <c r="ER38" s="1"/>
+      <c r="ES38" s="1"/>
+      <c r="ET38" s="1"/>
+      <c r="EU38" s="1"/>
+      <c r="EV38" s="27"/>
+      <c r="EW38" s="1"/>
+      <c r="EX38" s="1"/>
+      <c r="EY38" s="1"/>
+      <c r="EZ38" s="1"/>
+      <c r="FA38" s="1"/>
+      <c r="FB38" s="1"/>
+      <c r="FC38" s="1"/>
+      <c r="FD38" s="1"/>
+      <c r="FE38" s="1"/>
+      <c r="FF38" s="1"/>
+      <c r="FG38" s="1"/>
+      <c r="FH38" s="1"/>
+      <c r="FI38" s="1"/>
+      <c r="FJ38" s="1"/>
+      <c r="FK38" s="1"/>
+      <c r="FL38" s="1"/>
+      <c r="FM38" s="1"/>
+      <c r="FN38" s="1"/>
+      <c r="FO38" s="1"/>
+      <c r="FP38" s="1"/>
+    </row>
+    <row r="39" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="BJ39" s="134"/>
+      <c r="BT39" s="2"/>
+      <c r="CD39" s="2"/>
+      <c r="CN39" s="134"/>
+      <c r="CO39" s="15"/>
+      <c r="CP39" s="45"/>
+      <c r="CW39" s="22"/>
+      <c r="CX39" s="22"/>
+      <c r="DH39" s="26"/>
+      <c r="DR39" s="2"/>
+      <c r="EB39" s="2"/>
+      <c r="EL39" s="2"/>
+      <c r="EV39" s="22"/>
+      <c r="FF39" s="22"/>
+      <c r="FP39" s="26"/>
+    </row>
+    <row r="40" spans="62:172" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ40" s="134"/>
+      <c r="BT40" s="2"/>
+      <c r="CD40" s="2"/>
+      <c r="CN40" s="60"/>
+      <c r="CO40" s="15"/>
+      <c r="CP40" s="156"/>
+      <c r="CW40" s="22"/>
+      <c r="CX40" s="44"/>
+      <c r="DH40" s="22"/>
+      <c r="DR40" s="2"/>
+      <c r="EB40" s="2"/>
+      <c r="EL40" s="2"/>
+      <c r="EV40" s="22"/>
+      <c r="FF40" s="22"/>
+      <c r="FP40" s="22"/>
+    </row>
+    <row r="41" spans="62:172" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ41" s="134"/>
+      <c r="BK41" s="1"/>
+      <c r="BL41" s="1"/>
+      <c r="BM41" s="1"/>
+      <c r="BN41" s="1"/>
+      <c r="BO41" s="1"/>
+      <c r="BP41" s="1"/>
+      <c r="BQ41" s="1"/>
+      <c r="BR41" s="1"/>
+      <c r="BS41" s="1"/>
+      <c r="BT41" s="3"/>
+      <c r="BU41" s="1"/>
+      <c r="BV41" s="1"/>
+      <c r="BW41" s="1"/>
+      <c r="BX41" s="1"/>
+      <c r="BY41" s="1"/>
+      <c r="BZ41" s="1"/>
+      <c r="CA41" s="1"/>
+      <c r="CB41" s="1"/>
+      <c r="CC41" s="1"/>
+      <c r="CD41" s="3"/>
+      <c r="CE41" s="1"/>
+      <c r="CF41" s="1"/>
+      <c r="CG41" s="1"/>
+      <c r="CH41" s="1"/>
+      <c r="CI41" s="1"/>
+      <c r="CJ41" s="1"/>
+      <c r="CK41" s="1"/>
+      <c r="CL41" s="1"/>
+      <c r="CM41" s="1"/>
+      <c r="CN41" s="61"/>
+      <c r="CO41" s="90"/>
+      <c r="CP41" s="90"/>
+      <c r="CQ41" s="109"/>
+      <c r="CR41" s="109"/>
+      <c r="CT41" s="1"/>
+      <c r="CU41" s="1"/>
+      <c r="CV41" s="1"/>
+      <c r="CW41" s="27"/>
+      <c r="CX41" s="27"/>
+      <c r="CY41" s="23"/>
+      <c r="CZ41" s="109"/>
+      <c r="DA41" s="109"/>
+      <c r="DB41" s="109"/>
+      <c r="DC41" s="109"/>
+      <c r="DD41" s="109"/>
+      <c r="DE41" s="109"/>
+      <c r="DF41" s="109"/>
+      <c r="DG41" s="109"/>
+      <c r="DH41" s="22"/>
+      <c r="DI41" s="1"/>
+      <c r="DJ41" s="1"/>
+      <c r="DK41" s="1"/>
+      <c r="DL41" s="1"/>
+      <c r="DM41" s="1"/>
+      <c r="DN41" s="1"/>
+      <c r="DO41" s="1"/>
+      <c r="DP41" s="1"/>
+      <c r="DQ41" s="1"/>
+      <c r="DR41" s="3"/>
+      <c r="DS41" s="1"/>
+      <c r="DT41" s="1"/>
+      <c r="DU41" s="1"/>
+      <c r="DV41" s="1"/>
+      <c r="DW41" s="1"/>
+      <c r="DX41" s="1"/>
+      <c r="DY41" s="1"/>
+      <c r="DZ41" s="1"/>
+      <c r="EA41" s="1"/>
+      <c r="EB41" s="3"/>
+      <c r="EC41" s="1"/>
+      <c r="ED41" s="1"/>
+      <c r="EE41" s="1"/>
+      <c r="EF41" s="1"/>
+      <c r="EG41" s="1"/>
+      <c r="EH41" s="1"/>
+      <c r="EI41" s="1"/>
+      <c r="EJ41" s="1"/>
+      <c r="EK41" s="1"/>
+      <c r="EL41" s="3"/>
+      <c r="EM41" s="1"/>
+      <c r="EN41" s="1"/>
+      <c r="EO41" s="1"/>
+      <c r="EP41" s="1"/>
+      <c r="EQ41" s="1"/>
+      <c r="ER41" s="1"/>
+      <c r="ES41" s="1"/>
+      <c r="ET41" s="1"/>
+      <c r="EU41" s="1"/>
+      <c r="EV41" s="27"/>
+      <c r="EW41" s="109"/>
+      <c r="EX41" s="109"/>
+      <c r="EY41" s="109"/>
+      <c r="EZ41" s="109"/>
+      <c r="FA41" s="109"/>
+      <c r="FB41" s="109"/>
+      <c r="FC41" s="109"/>
+      <c r="FD41" s="109"/>
+      <c r="FE41" s="109"/>
+      <c r="FF41" s="22"/>
+      <c r="FG41" s="23"/>
+      <c r="FH41" s="109"/>
+      <c r="FI41" s="109"/>
+      <c r="FJ41" s="109"/>
+      <c r="FK41" s="109"/>
+      <c r="FL41" s="109"/>
+      <c r="FM41" s="109"/>
+      <c r="FN41" s="109"/>
+      <c r="FO41" s="109"/>
+      <c r="FP41" s="22"/>
+    </row>
+    <row r="42" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="BJ42" s="134"/>
+      <c r="BT42" s="2"/>
+      <c r="CD42" s="2"/>
+      <c r="CN42" s="134"/>
+      <c r="CO42" s="159"/>
+      <c r="CP42" s="26"/>
+      <c r="CX42" s="26"/>
+      <c r="DH42" s="22"/>
+      <c r="DR42" s="2"/>
+      <c r="EB42" s="2"/>
+      <c r="EL42" s="2"/>
+      <c r="EV42" s="22"/>
+      <c r="FF42" s="22"/>
+      <c r="FJ42" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="FP42" s="22"/>
+    </row>
+    <row r="43" spans="62:172" x14ac:dyDescent="0.3">
+      <c r="BJ43" s="134"/>
+      <c r="BT43" s="2"/>
+      <c r="CD43" s="2"/>
+      <c r="CN43" s="134"/>
+      <c r="CP43" s="37"/>
+      <c r="CX43" s="60"/>
+      <c r="DH43" s="22"/>
+      <c r="DR43" s="2"/>
+      <c r="EB43" s="2"/>
+      <c r="EL43" s="2"/>
+      <c r="EV43" s="22"/>
+      <c r="FF43" s="22"/>
+      <c r="FP43" s="22"/>
+    </row>
+    <row r="44" spans="62:172" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ44" s="134"/>
+      <c r="BK44" s="1"/>
+      <c r="BL44" s="1"/>
+      <c r="BM44" s="1"/>
+      <c r="BN44" s="1"/>
+      <c r="BO44" s="1"/>
+      <c r="BP44" s="1"/>
+      <c r="BQ44" s="1"/>
+      <c r="BR44" s="1"/>
+      <c r="BS44" s="1"/>
+      <c r="BT44" s="3"/>
+      <c r="BU44" s="1"/>
+      <c r="BV44" s="1"/>
+      <c r="BW44" s="1"/>
+      <c r="BX44" s="1"/>
+      <c r="BY44" s="1"/>
+      <c r="BZ44" s="1"/>
+      <c r="CA44" s="1"/>
+      <c r="CB44" s="1"/>
+      <c r="CC44" s="1"/>
+      <c r="CD44" s="3"/>
+      <c r="CE44" s="1"/>
+      <c r="CF44" s="1"/>
+      <c r="CG44" s="1"/>
+      <c r="CH44" s="1"/>
+      <c r="CI44" s="1"/>
+      <c r="CJ44" s="1"/>
+      <c r="CK44" s="1"/>
+      <c r="CL44" s="1"/>
+      <c r="CM44" s="1"/>
+      <c r="CN44" s="135"/>
+      <c r="CO44" s="160"/>
+      <c r="CP44" s="22"/>
+      <c r="CQ44" s="18">
+        <v>4</v>
+      </c>
+      <c r="CR44" s="18">
+        <v>4</v>
+      </c>
+      <c r="CS44" s="18">
+        <v>4</v>
+      </c>
+      <c r="CT44" s="1"/>
+      <c r="CU44" s="1"/>
+      <c r="CV44" s="1"/>
+      <c r="CW44" s="1"/>
+      <c r="CX44" s="61"/>
+      <c r="CY44" s="1"/>
+      <c r="CZ44" s="1"/>
+      <c r="DA44" s="147"/>
+      <c r="DB44" s="1"/>
+      <c r="DD44" s="109"/>
+      <c r="DE44" s="109"/>
+      <c r="DF44" s="109"/>
+      <c r="DG44" s="109"/>
+      <c r="DH44" s="22"/>
+      <c r="DI44" s="1"/>
+      <c r="DJ44" s="1"/>
+      <c r="DK44" s="1"/>
+      <c r="DL44" s="1"/>
+      <c r="DM44" s="1"/>
+      <c r="DN44" s="1"/>
+      <c r="DO44" s="1"/>
+      <c r="DP44" s="1"/>
+      <c r="DQ44" s="1"/>
+      <c r="DR44" s="3"/>
+      <c r="DS44" s="1"/>
+      <c r="DT44" s="1"/>
+      <c r="DU44" s="1"/>
+      <c r="DV44" s="1"/>
+      <c r="DW44" s="1"/>
+      <c r="DX44" s="1"/>
+      <c r="DY44" s="1"/>
+      <c r="DZ44" s="1"/>
+      <c r="EA44" s="1"/>
+      <c r="EB44" s="3"/>
+      <c r="EC44" s="1"/>
+      <c r="ED44" s="1"/>
+      <c r="EE44" s="1"/>
+      <c r="EF44" s="1"/>
+      <c r="EG44" s="1"/>
+      <c r="EH44" s="1"/>
+      <c r="EI44" s="1"/>
+      <c r="EJ44" s="1"/>
+      <c r="EK44" s="1"/>
+      <c r="EL44" s="3"/>
+      <c r="EM44" s="1"/>
+      <c r="EN44" s="1"/>
+      <c r="EO44" s="1"/>
+      <c r="EP44" s="1"/>
+      <c r="EQ44" s="1"/>
+      <c r="ER44" s="1"/>
+      <c r="ES44" s="1"/>
+      <c r="ET44" s="1"/>
+      <c r="EU44" s="1"/>
+      <c r="EV44" s="27"/>
+      <c r="EW44" s="109"/>
+      <c r="EX44" s="109"/>
+      <c r="EY44" s="109"/>
+      <c r="EZ44" s="109"/>
+      <c r="FA44" s="109"/>
+      <c r="FB44" s="109"/>
+      <c r="FC44" s="109"/>
+      <c r="FD44" s="109"/>
+      <c r="FE44" s="109"/>
+      <c r="FF44" s="22"/>
+      <c r="FG44" s="23"/>
+      <c r="FH44" s="109"/>
+      <c r="FI44" s="109"/>
+      <c r="FJ44" s="109"/>
+      <c r="FK44" s="109"/>
+      <c r="FL44" s="126" t="s">
+        <v>50</v>
+      </c>
+      <c r="FM44" s="109"/>
+      <c r="FN44" s="109"/>
+      <c r="FO44" s="109"/>
+      <c r="FP44" s="22"/>
+    </row>
+    <row r="45" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="BJ45" s="134"/>
+      <c r="BT45" s="2"/>
+      <c r="CD45" s="2"/>
+      <c r="CN45" s="134"/>
+      <c r="CP45" s="49"/>
+      <c r="CR45" s="49"/>
+      <c r="CT45" s="41"/>
+      <c r="CV45" s="41"/>
+      <c r="CX45" s="42"/>
+      <c r="CZ45" s="41"/>
+      <c r="DB45" s="42"/>
+      <c r="DH45" s="2"/>
+      <c r="DR45" s="2"/>
+      <c r="EB45" s="2"/>
+      <c r="EL45" s="2"/>
+      <c r="EV45" s="22"/>
+      <c r="FF45" s="2"/>
+      <c r="FP45" s="22"/>
+    </row>
+    <row r="46" spans="62:172" x14ac:dyDescent="0.3">
+      <c r="BJ46" s="134"/>
+      <c r="BT46" s="2"/>
+      <c r="CD46" s="2"/>
+      <c r="CN46" s="134"/>
+      <c r="CO46" s="160"/>
+      <c r="CP46" s="109"/>
+      <c r="CQ46" s="49"/>
+      <c r="CS46" s="49"/>
+      <c r="CU46" s="49"/>
+      <c r="CW46" s="49"/>
+      <c r="CX46" s="22"/>
+      <c r="CY46" s="93"/>
+      <c r="DA46" s="49"/>
+      <c r="DB46" s="22"/>
+      <c r="DH46" s="2"/>
+      <c r="DR46" s="2"/>
+      <c r="EB46" s="2"/>
+      <c r="EL46" s="2"/>
+      <c r="EV46" s="60"/>
+      <c r="FF46" s="2"/>
+      <c r="FP46" s="22"/>
+    </row>
+    <row r="47" spans="62:172" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ47" s="134"/>
+      <c r="BK47" s="137"/>
+      <c r="BL47" s="132"/>
+      <c r="BM47" s="132"/>
+      <c r="BN47" s="132"/>
+      <c r="BO47" s="132"/>
+      <c r="BP47" s="132"/>
+      <c r="BQ47" s="132"/>
+      <c r="BR47" s="132"/>
+      <c r="BS47" s="132"/>
+      <c r="BT47" s="140"/>
+      <c r="BU47" s="110"/>
+      <c r="BV47" s="1"/>
+      <c r="BW47" s="1"/>
+      <c r="BX47" s="1"/>
+      <c r="BY47" s="1"/>
+      <c r="BZ47" s="1"/>
+      <c r="CA47" s="1"/>
+      <c r="CB47" s="1"/>
+      <c r="CC47" s="1"/>
+      <c r="CD47" s="3"/>
+      <c r="CE47" s="1"/>
+      <c r="CF47" s="1"/>
+      <c r="CG47" s="1"/>
+      <c r="CH47" s="1"/>
+      <c r="CI47" s="1"/>
+      <c r="CJ47" s="1"/>
+      <c r="CK47" s="1"/>
+      <c r="CL47" s="1"/>
+      <c r="CM47" s="1"/>
+      <c r="CN47" s="135"/>
+      <c r="CO47" s="1"/>
+      <c r="CP47" s="40"/>
+      <c r="CQ47" s="1"/>
+      <c r="CR47" s="40"/>
+      <c r="CS47" s="1"/>
+      <c r="CT47" s="40"/>
+      <c r="CU47" s="1"/>
+      <c r="CV47" s="40"/>
+      <c r="CW47" s="1"/>
+      <c r="CX47" s="94"/>
+      <c r="CY47" s="1"/>
+      <c r="CZ47" s="40"/>
+      <c r="DA47" s="1"/>
+      <c r="DB47" s="94"/>
+      <c r="DC47" s="1"/>
+      <c r="DD47" s="1"/>
+      <c r="DE47" s="1"/>
+      <c r="DF47" s="1"/>
+      <c r="DG47" s="1"/>
+      <c r="DH47" s="3"/>
+      <c r="DI47" s="1"/>
+      <c r="DJ47" s="1"/>
+      <c r="DK47" s="1"/>
+      <c r="DL47" s="1"/>
+      <c r="DM47" s="1"/>
+      <c r="DN47" s="1"/>
+      <c r="DO47" s="1"/>
+      <c r="DP47" s="1"/>
+      <c r="DQ47" s="1"/>
+      <c r="DR47" s="3"/>
+      <c r="DS47" s="1"/>
+      <c r="DT47" s="1"/>
+      <c r="DU47" s="1"/>
+      <c r="DV47" s="1"/>
+      <c r="DW47" s="1"/>
+      <c r="DX47" s="1"/>
+      <c r="DY47" s="1"/>
+      <c r="DZ47" s="1"/>
+      <c r="EA47" s="1"/>
+      <c r="EB47" s="3"/>
+      <c r="EC47" s="1"/>
+      <c r="ED47" s="1"/>
+      <c r="EE47" s="1"/>
+      <c r="EF47" s="1"/>
+      <c r="EG47" s="1"/>
+      <c r="EH47" s="1"/>
+      <c r="EI47" s="1"/>
+      <c r="EJ47" s="1"/>
+      <c r="EK47" s="1"/>
+      <c r="EL47" s="3"/>
+      <c r="EM47" s="1"/>
+      <c r="EN47" s="1"/>
+      <c r="EO47" s="1"/>
+      <c r="EP47" s="1"/>
+      <c r="EQ47" s="1"/>
+      <c r="ER47" s="1"/>
+      <c r="ES47" s="1"/>
+      <c r="ET47" s="1"/>
+      <c r="EU47" s="1"/>
+      <c r="EV47" s="61"/>
+      <c r="EW47" s="1"/>
+      <c r="EX47" s="1"/>
+      <c r="EY47" s="163"/>
+      <c r="EZ47" s="163"/>
+      <c r="FA47" s="163"/>
+      <c r="FB47" s="163"/>
+      <c r="FC47" s="163"/>
+      <c r="FD47" s="1"/>
+      <c r="FE47" s="1"/>
+      <c r="FF47" s="3"/>
+      <c r="FG47" s="1"/>
+      <c r="FH47" s="1"/>
+      <c r="FI47" s="1"/>
+      <c r="FJ47" s="1"/>
+      <c r="FK47" s="1"/>
+      <c r="FL47" s="1"/>
+      <c r="FM47" s="1"/>
+      <c r="FN47" s="1"/>
+      <c r="FO47" s="1"/>
+      <c r="FP47" s="27"/>
+    </row>
+    <row r="48" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="BT48" s="133"/>
+      <c r="CD48" s="2"/>
+      <c r="CN48" s="134"/>
+      <c r="CX48" s="26"/>
+      <c r="DH48" s="2"/>
+      <c r="DR48" s="2"/>
+      <c r="EB48" s="2"/>
+      <c r="EL48" s="2"/>
+      <c r="EV48" s="2"/>
+      <c r="EX48" s="26"/>
+      <c r="FA48" s="109"/>
+      <c r="FC48" s="22"/>
+      <c r="FF48" s="22"/>
+    </row>
+    <row r="49" spans="72:162" x14ac:dyDescent="0.3">
+      <c r="BT49" s="134"/>
+      <c r="CD49" s="2"/>
+      <c r="CN49" s="134"/>
+      <c r="CX49" s="22"/>
+      <c r="DH49" s="2"/>
+      <c r="DR49" s="2"/>
+      <c r="EB49" s="2"/>
+      <c r="EL49" s="2"/>
+      <c r="EV49" s="2"/>
+      <c r="EX49" s="22"/>
+      <c r="FA49" s="109"/>
+      <c r="FC49" s="22"/>
+      <c r="FF49" s="22"/>
+    </row>
+    <row r="50" spans="72:162" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BT50" s="134"/>
+      <c r="BU50" s="1"/>
+      <c r="BV50" s="1"/>
+      <c r="BW50" s="1"/>
+      <c r="BX50" s="1"/>
+      <c r="BY50" s="1"/>
+      <c r="BZ50" s="1"/>
+      <c r="CA50" s="1"/>
+      <c r="CB50" s="1"/>
+      <c r="CC50" s="1"/>
+      <c r="CD50" s="3"/>
+      <c r="CE50" s="1"/>
+      <c r="CF50" s="1"/>
+      <c r="CG50" s="1"/>
+      <c r="CH50" s="1"/>
+      <c r="CI50" s="1"/>
+      <c r="CJ50" s="1"/>
+      <c r="CK50" s="1"/>
+      <c r="CL50" s="1"/>
+      <c r="CM50" s="1"/>
+      <c r="CN50" s="135"/>
+      <c r="CX50" s="22"/>
+      <c r="CY50" s="1"/>
+      <c r="CZ50" s="1"/>
+      <c r="DA50" s="1"/>
+      <c r="DB50" s="1"/>
+      <c r="DC50" s="1"/>
+      <c r="DD50" s="1"/>
+      <c r="DE50" s="1"/>
+      <c r="DF50" s="1"/>
+      <c r="DG50" s="1"/>
+      <c r="DH50" s="3"/>
+      <c r="DI50" s="1"/>
+      <c r="DJ50" s="1"/>
+      <c r="DK50" s="1"/>
+      <c r="DL50" s="1"/>
+      <c r="DM50" s="1"/>
+      <c r="DN50" s="1"/>
+      <c r="DO50" s="1"/>
+      <c r="DP50" s="1"/>
+      <c r="DQ50" s="1"/>
+      <c r="DR50" s="3"/>
+      <c r="DS50" s="1"/>
+      <c r="DT50" s="1"/>
+      <c r="DU50" s="1"/>
+      <c r="DV50" s="1"/>
+      <c r="DW50" s="1"/>
+      <c r="DX50" s="1"/>
+      <c r="DY50" s="1"/>
+      <c r="DZ50" s="1"/>
+      <c r="EA50" s="1"/>
+      <c r="EB50" s="3"/>
+      <c r="EC50" s="1"/>
+      <c r="ED50" s="1"/>
+      <c r="EE50" s="1"/>
+      <c r="EF50" s="1"/>
+      <c r="EG50" s="1"/>
+      <c r="EH50" s="1"/>
+      <c r="EI50" s="1"/>
+      <c r="EJ50" s="1"/>
+      <c r="EK50" s="1"/>
+      <c r="EL50" s="3"/>
+      <c r="EM50" s="1"/>
+      <c r="EN50" s="1"/>
+      <c r="EO50" s="1"/>
+      <c r="EP50" s="1"/>
+      <c r="EQ50" s="1"/>
+      <c r="ER50" s="1"/>
+      <c r="ES50" s="1"/>
+      <c r="ET50" s="1"/>
+      <c r="EU50" s="1"/>
+      <c r="EV50" s="3"/>
+      <c r="EW50" s="1"/>
+      <c r="EX50" s="27"/>
+      <c r="EY50" s="109"/>
+      <c r="EZ50" s="109"/>
+      <c r="FA50" s="109"/>
+      <c r="FB50" s="109"/>
+      <c r="FC50" s="22"/>
+      <c r="FD50" s="1"/>
+      <c r="FE50" s="1"/>
+      <c r="FF50" s="27"/>
+    </row>
+    <row r="51" spans="72:162" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="BT51" s="134"/>
+      <c r="CD51" s="2"/>
+      <c r="CN51" s="134"/>
+      <c r="CX51" s="22"/>
+      <c r="DH51" s="2"/>
+      <c r="DR51" s="2"/>
+      <c r="EB51" s="2"/>
+      <c r="EL51" s="2"/>
+      <c r="EV51" s="2"/>
+      <c r="FD51" s="15"/>
+      <c r="FE51" s="15"/>
+      <c r="FF51" s="112"/>
+    </row>
+    <row r="52" spans="72:162" x14ac:dyDescent="0.3">
+      <c r="BT52" s="134"/>
+      <c r="CD52" s="2"/>
+      <c r="CN52" s="134"/>
+      <c r="CU52" t="s">
+        <v>53</v>
+      </c>
+      <c r="CX52" s="60"/>
+      <c r="DH52" s="2"/>
+      <c r="DR52" s="2"/>
+      <c r="EB52" s="2"/>
+      <c r="EL52" s="2"/>
+      <c r="EV52" s="2"/>
+      <c r="FD52" s="15"/>
+      <c r="FE52" s="15"/>
+      <c r="FF52" s="112"/>
+    </row>
+    <row r="53" spans="72:162" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BT53" s="134"/>
+      <c r="BU53" s="1"/>
+      <c r="BV53" s="1"/>
+      <c r="BW53" s="1"/>
+      <c r="BX53" s="1"/>
+      <c r="BY53" s="1"/>
+      <c r="BZ53" s="1"/>
+      <c r="CA53" s="1"/>
+      <c r="CB53" s="1"/>
+      <c r="CC53" s="1"/>
+      <c r="CD53" s="3"/>
+      <c r="CE53" s="1"/>
+      <c r="CF53" s="1"/>
+      <c r="CG53" s="1"/>
+      <c r="CH53" s="1"/>
+      <c r="CI53" s="1"/>
+      <c r="CJ53" s="1"/>
+      <c r="CK53" s="1"/>
+      <c r="CL53" s="1"/>
+      <c r="CM53" s="1"/>
+      <c r="CN53" s="135"/>
+      <c r="CW53" s="95" t="s">
+        <v>51</v>
+      </c>
+      <c r="CX53" s="60"/>
+      <c r="CY53" s="1"/>
+      <c r="CZ53" s="1"/>
+      <c r="DA53" s="1"/>
+      <c r="DB53" s="1"/>
+      <c r="DC53" s="1"/>
+      <c r="DD53" s="1"/>
+      <c r="DE53" s="1"/>
+      <c r="DF53" s="1"/>
+      <c r="DG53" s="1"/>
+      <c r="DH53" s="3"/>
+      <c r="DI53" s="1"/>
+      <c r="DJ53" s="1"/>
+      <c r="DK53" s="1"/>
+      <c r="DL53" s="1"/>
+      <c r="DM53" s="1"/>
+      <c r="DN53" s="1"/>
+      <c r="DO53" s="1"/>
+      <c r="DP53" s="1"/>
+      <c r="DQ53" s="1"/>
+      <c r="DR53" s="3"/>
+      <c r="DS53" s="1"/>
+      <c r="DT53" s="1"/>
+      <c r="DU53" s="1"/>
+      <c r="DV53" s="1"/>
+      <c r="DW53" s="1"/>
+      <c r="DX53" s="1"/>
+      <c r="DY53" s="1"/>
+      <c r="DZ53" s="1"/>
+      <c r="EA53" s="1"/>
+      <c r="EB53" s="3"/>
+      <c r="EC53" s="1"/>
+      <c r="ED53" s="1"/>
+      <c r="EE53" s="1"/>
+      <c r="EF53" s="1"/>
+      <c r="EG53" s="1"/>
+      <c r="EH53" s="1"/>
+      <c r="EI53" s="1"/>
+      <c r="EJ53" s="1"/>
+      <c r="EK53" s="1"/>
+      <c r="EL53" s="3"/>
+      <c r="EM53" s="1"/>
+      <c r="EN53" s="1"/>
+      <c r="EO53" s="1"/>
+      <c r="EP53" s="1"/>
+      <c r="EQ53" s="1"/>
+      <c r="ER53" s="1"/>
+      <c r="ES53" s="1"/>
+      <c r="ET53" s="1"/>
+      <c r="EU53" s="1"/>
+      <c r="EV53" s="3"/>
+      <c r="EW53" s="1"/>
+      <c r="EX53" s="1"/>
+      <c r="EY53" s="1"/>
+      <c r="EZ53" s="1"/>
+      <c r="FA53" s="1"/>
+      <c r="FB53" s="1"/>
+      <c r="FC53" s="1"/>
+      <c r="FD53" s="90"/>
+      <c r="FE53" s="164"/>
+      <c r="FF53" s="113"/>
+    </row>
+    <row r="54" spans="72:162" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="BT54" s="134"/>
+      <c r="CD54" s="26"/>
+      <c r="CN54" s="134"/>
+      <c r="CU54" t="s">
+        <v>52</v>
+      </c>
+      <c r="CX54" s="22"/>
+      <c r="DH54" s="2"/>
+      <c r="DR54" s="2"/>
+      <c r="EB54" s="2"/>
+      <c r="EL54" s="2"/>
+      <c r="EV54" s="2"/>
+      <c r="FF54" s="22"/>
+    </row>
+    <row r="55" spans="72:162" x14ac:dyDescent="0.3">
+      <c r="BT55" s="134"/>
+      <c r="CD55" s="22"/>
+      <c r="CN55" s="134"/>
+      <c r="CX55" s="22"/>
+      <c r="DH55" s="2"/>
+      <c r="DR55" s="2"/>
+      <c r="EB55" s="2"/>
+      <c r="EL55" s="2"/>
+      <c r="EV55" s="2"/>
+      <c r="FF55" s="22"/>
+    </row>
+    <row r="56" spans="72:162" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BT56" s="134"/>
+      <c r="BU56" s="137"/>
+      <c r="BV56" s="132"/>
+      <c r="BW56" s="132"/>
+      <c r="BX56" s="132"/>
+      <c r="BY56" s="132"/>
+      <c r="BZ56" s="132"/>
+      <c r="CA56" s="132"/>
+      <c r="CB56" s="132"/>
+      <c r="CC56" s="132"/>
+      <c r="CD56" s="145"/>
+      <c r="CE56" s="132"/>
+      <c r="CF56" s="132"/>
+      <c r="CG56" s="132"/>
+      <c r="CH56" s="132"/>
+      <c r="CI56" s="132"/>
+      <c r="CJ56" s="149" t="s">
+        <v>21</v>
+      </c>
+      <c r="CK56" s="132"/>
+      <c r="CL56" s="132"/>
+      <c r="CM56" s="132"/>
+      <c r="CN56" s="144"/>
+      <c r="CX56" s="22"/>
+      <c r="CY56" s="1"/>
+      <c r="CZ56" s="1"/>
+      <c r="DA56" s="1"/>
+      <c r="DB56" s="1"/>
+      <c r="DC56" s="1"/>
+      <c r="DD56" s="1"/>
+      <c r="DE56" s="1"/>
+      <c r="DF56" s="1"/>
+      <c r="DG56" s="1"/>
+      <c r="DH56" s="3"/>
+      <c r="DI56" s="1"/>
+      <c r="DJ56" s="1"/>
+      <c r="DK56" s="1"/>
+      <c r="DL56" s="1"/>
+      <c r="DM56" s="1"/>
+      <c r="DN56" s="1"/>
+      <c r="DO56" s="1"/>
+      <c r="DP56" s="1"/>
+      <c r="DQ56" s="1"/>
+      <c r="DR56" s="3"/>
+      <c r="DS56" s="1"/>
+      <c r="DT56" s="1"/>
+      <c r="DU56" s="1"/>
+      <c r="DV56" s="1"/>
+      <c r="DW56" s="1"/>
+      <c r="DX56" s="1"/>
+      <c r="DY56" s="1"/>
+      <c r="DZ56" s="1"/>
+      <c r="EA56" s="1"/>
+      <c r="EB56" s="3"/>
+      <c r="EC56" s="1"/>
+      <c r="ED56" s="1"/>
+      <c r="EE56" s="1"/>
+      <c r="EF56" s="1"/>
+      <c r="EG56" s="1"/>
+      <c r="EH56" s="1"/>
+      <c r="EI56" s="1"/>
+      <c r="EJ56" s="1"/>
+      <c r="EK56" s="1"/>
+      <c r="EL56" s="3"/>
+      <c r="EM56" s="1"/>
+      <c r="EN56" s="1"/>
+      <c r="EO56" s="1"/>
+      <c r="EP56" s="1"/>
+      <c r="EQ56" s="1"/>
+      <c r="ER56" s="1"/>
+      <c r="ES56" s="1"/>
+      <c r="ET56" s="1"/>
+      <c r="EU56" s="1"/>
+      <c r="EV56" s="3"/>
+      <c r="EW56" s="1"/>
+      <c r="EX56" s="1"/>
+      <c r="EY56" s="1"/>
+      <c r="EZ56" s="1"/>
+      <c r="FA56" s="1"/>
+      <c r="FB56" s="1"/>
+      <c r="FC56" s="1"/>
+      <c r="FD56" s="1"/>
+      <c r="FE56" s="1"/>
+      <c r="FF56" s="27"/>
+    </row>
+    <row r="57" spans="72:162" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Did more level design
Both drafting and trying to figure out how to Unity
</commit_message>
<xml_diff>
--- a/Game Design Documentation/Demo Level Map Draft.xlsx
+++ b/Game Design Documentation/Demo Level Map Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://osekk-my.sharepoint.com/personal/s4voto00_students_osao_fi/Documents/Tiedostot/Github/CartoonViolence/Game Design Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1530" documentId="11_F25DC773A252ABDACC1048BB699D52725ADE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98A30EB2-707E-4F87-8B79-549D2AF35D3D}"/>
+  <xr:revisionPtr revIDLastSave="1558" documentId="11_F25DC773A252ABDACC1048BB699D52725ADE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6BF2B87-F668-448D-AEA7-599F7BB7EBA3}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="9960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1222,6 +1222,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="DN47" authorId="0" shapeId="0" xr:uid="{30BDDE8C-F986-4CBA-AE39-6FA9E461CCEF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ducker
+Unloaded, Stationary.
+You can run past him and into the other screen before he shoots, prompting him to chase after you.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="FA47" authorId="0" shapeId="0" xr:uid="{6E66CF02-2305-461D-8F46-705A678F6DBE}">
       <text>
         <r>
@@ -1301,7 +1327,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>Screen Template</t>
   </si>
@@ -1481,6 +1507,15 @@
   <si>
     <t>END OF DEMO</t>
   </si>
+  <si>
+    <t>RUN BRUV, RUN!</t>
+  </si>
+  <si>
+    <t>Key Dispenser</t>
+  </si>
+  <si>
+    <t>←IN CASE OF LOCKS, SMACK THIS</t>
+  </si>
 </sst>
 </file>
 
@@ -1546,7 +1581,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1607,6 +1642,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="114">
     <border>
@@ -2959,7 +3000,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -3109,12 +3150,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="78" xfId="0" applyBorder="1"/>
@@ -3132,10 +3171,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1"/>
@@ -3194,6 +3229,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="111" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="112" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="113" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -3480,8 +3518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="B2:K10"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3643,7 +3681,7 @@
       </c>
     </row>
     <row r="17" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M17" s="129"/>
+      <c r="M17" s="125"/>
     </row>
     <row r="18" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="18">
@@ -3656,8 +3694,8 @@
       <c r="I18" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="128"/>
-      <c r="M18" s="130"/>
+      <c r="L18" s="124"/>
+      <c r="M18" s="126"/>
       <c r="N18" t="s">
         <v>48</v>
       </c>
@@ -3669,6 +3707,10 @@
       </c>
       <c r="C20" t="s">
         <v>22</v>
+      </c>
+      <c r="H20" s="165"/>
+      <c r="I20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
@@ -3921,7 +3963,7 @@
       <c r="C24" s="22"/>
       <c r="M24" s="2"/>
       <c r="R24" s="26"/>
-      <c r="V24" s="111"/>
+      <c r="V24" s="110"/>
       <c r="W24" s="2"/>
       <c r="X24" s="39"/>
       <c r="Z24" s="41"/>
@@ -3940,7 +3982,7 @@
       <c r="C25" s="22"/>
       <c r="M25" s="2"/>
       <c r="R25" s="22"/>
-      <c r="V25" s="112"/>
+      <c r="V25" s="111"/>
       <c r="W25" s="38"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="40"/>
@@ -4222,7 +4264,7 @@
       <c r="M37" s="22"/>
       <c r="N37" s="11"/>
       <c r="O37" s="22"/>
-      <c r="P37" s="152" t="s">
+      <c r="P37" s="148" t="s">
         <v>44</v>
       </c>
       <c r="Q37" s="86"/>
@@ -4315,8 +4357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A88EDC-4468-4B92-BB23-9A52F08C9D3C}">
   <dimension ref="A1:FP57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DE35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DW40" sqref="DW40"/>
+    <sheetView tabSelected="1" topLeftCell="CW35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DW41" sqref="DW41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4325,83 +4367,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:152" x14ac:dyDescent="0.3">
-      <c r="DR1" s="109"/>
-      <c r="DT1" s="167"/>
-      <c r="EV1" s="134"/>
+      <c r="DT1" s="163"/>
+      <c r="EV1" s="130"/>
     </row>
     <row r="2" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="132"/>
-      <c r="L2" s="132"/>
-      <c r="M2" s="132"/>
-      <c r="N2" s="132"/>
-      <c r="O2" s="132"/>
-      <c r="P2" s="132"/>
-      <c r="Q2" s="132"/>
-      <c r="R2" s="132"/>
-      <c r="S2" s="132"/>
-      <c r="T2" s="132"/>
-      <c r="U2" s="132"/>
-      <c r="V2" s="132"/>
-      <c r="DR2" s="109"/>
-      <c r="DS2" s="166"/>
-      <c r="DT2" s="165"/>
-      <c r="DU2" s="132"/>
-      <c r="DV2" s="132"/>
-      <c r="DW2" s="132"/>
-      <c r="DX2" s="132"/>
-      <c r="DY2" s="132"/>
-      <c r="DZ2" s="132"/>
-      <c r="EA2" s="132"/>
-      <c r="EB2" s="132"/>
-      <c r="EC2" s="132"/>
-      <c r="ED2" s="132"/>
-      <c r="EE2" s="132"/>
-      <c r="EF2" s="132"/>
-      <c r="EG2" s="132"/>
-      <c r="EH2" s="132"/>
-      <c r="EI2" s="132"/>
-      <c r="EJ2" s="132"/>
-      <c r="EK2" s="132"/>
-      <c r="EL2" s="132"/>
-      <c r="EM2" s="132"/>
-      <c r="EN2" s="132"/>
-      <c r="EO2" s="132"/>
-      <c r="EP2" s="132"/>
-      <c r="EQ2" s="132"/>
-      <c r="ER2" s="132"/>
-      <c r="ES2" s="132"/>
-      <c r="ET2" s="132"/>
-      <c r="EU2" s="149" t="s">
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="128"/>
+      <c r="N2" s="128"/>
+      <c r="O2" s="128"/>
+      <c r="P2" s="128"/>
+      <c r="Q2" s="128"/>
+      <c r="R2" s="128"/>
+      <c r="S2" s="128"/>
+      <c r="T2" s="128"/>
+      <c r="U2" s="128"/>
+      <c r="V2" s="128"/>
+      <c r="DS2" s="162"/>
+      <c r="DT2" s="161"/>
+      <c r="DU2" s="128"/>
+      <c r="DV2" s="128"/>
+      <c r="DW2" s="128"/>
+      <c r="DX2" s="128"/>
+      <c r="DY2" s="128"/>
+      <c r="DZ2" s="128"/>
+      <c r="EA2" s="128"/>
+      <c r="EB2" s="128"/>
+      <c r="EC2" s="128"/>
+      <c r="ED2" s="128"/>
+      <c r="EE2" s="128"/>
+      <c r="EF2" s="128"/>
+      <c r="EG2" s="128"/>
+      <c r="EH2" s="128"/>
+      <c r="EI2" s="128"/>
+      <c r="EJ2" s="128"/>
+      <c r="EK2" s="128"/>
+      <c r="EL2" s="128"/>
+      <c r="EM2" s="128"/>
+      <c r="EN2" s="128"/>
+      <c r="EO2" s="128"/>
+      <c r="EP2" s="128"/>
+      <c r="EQ2" s="128"/>
+      <c r="ER2" s="128"/>
+      <c r="ES2" s="128"/>
+      <c r="ET2" s="128"/>
+      <c r="EU2" s="145" t="s">
         <v>21</v>
       </c>
-      <c r="EV2" s="144"/>
+      <c r="EV2" s="140"/>
     </row>
     <row r="3" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="134"/>
+      <c r="B3" s="130"/>
       <c r="L3" s="2"/>
-      <c r="V3" s="133"/>
-      <c r="DR3" s="134"/>
+      <c r="V3" s="129"/>
+      <c r="DR3" s="130"/>
       <c r="EB3" s="2"/>
       <c r="EV3" s="22"/>
     </row>
     <row r="4" spans="1:152" x14ac:dyDescent="0.3">
-      <c r="B4" s="134"/>
+      <c r="B4" s="130"/>
       <c r="L4" s="2"/>
-      <c r="V4" s="134"/>
-      <c r="DR4" s="134"/>
+      <c r="V4" s="130"/>
+      <c r="DR4" s="130"/>
       <c r="EB4" s="2"/>
       <c r="EV4" s="22"/>
     </row>
     <row r="5" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="134"/>
+      <c r="B5" s="130"/>
       <c r="C5" s="1"/>
       <c r="D5" s="30" t="s">
         <v>21</v>
@@ -4423,8 +4463,8 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="135"/>
-      <c r="DR5" s="134"/>
+      <c r="V5" s="131"/>
+      <c r="DR5" s="130"/>
       <c r="DS5" s="1"/>
       <c r="DT5" s="1"/>
       <c r="DU5" s="1"/>
@@ -4438,23 +4478,23 @@
       <c r="EV5" s="22"/>
     </row>
     <row r="6" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="134"/>
+      <c r="B6" s="130"/>
       <c r="L6" s="2"/>
-      <c r="V6" s="134"/>
-      <c r="DR6" s="134"/>
+      <c r="V6" s="130"/>
+      <c r="DR6" s="130"/>
       <c r="EB6" s="2"/>
       <c r="EV6" s="22"/>
     </row>
     <row r="7" spans="1:152" x14ac:dyDescent="0.3">
-      <c r="B7" s="134"/>
+      <c r="B7" s="130"/>
       <c r="L7" s="2"/>
-      <c r="V7" s="134"/>
-      <c r="DR7" s="134"/>
+      <c r="V7" s="130"/>
+      <c r="DR7" s="130"/>
       <c r="EB7" s="2"/>
       <c r="EV7" s="22"/>
     </row>
     <row r="8" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="134"/>
+      <c r="B8" s="130"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -4474,8 +4514,8 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="135"/>
-      <c r="DR8" s="134"/>
+      <c r="V8" s="131"/>
+      <c r="DR8" s="130"/>
       <c r="DS8" s="1"/>
       <c r="DT8" s="1"/>
       <c r="DU8" s="1"/>
@@ -4489,23 +4529,23 @@
       <c r="EV8" s="22"/>
     </row>
     <row r="9" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="134"/>
+      <c r="B9" s="130"/>
       <c r="L9" s="2"/>
-      <c r="V9" s="134"/>
-      <c r="DR9" s="134"/>
+      <c r="V9" s="130"/>
+      <c r="DR9" s="130"/>
       <c r="EB9" s="2"/>
       <c r="EV9" s="22"/>
     </row>
     <row r="10" spans="1:152" x14ac:dyDescent="0.3">
-      <c r="B10" s="134"/>
+      <c r="B10" s="130"/>
       <c r="L10" s="2"/>
-      <c r="V10" s="134"/>
-      <c r="DR10" s="134"/>
+      <c r="V10" s="130"/>
+      <c r="DR10" s="130"/>
       <c r="EB10" s="2"/>
       <c r="EV10" s="22"/>
     </row>
     <row r="11" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="134"/>
+      <c r="B11" s="130"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -4525,17 +4565,17 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="135"/>
-      <c r="W11" s="137"/>
-      <c r="X11" s="132"/>
-      <c r="Y11" s="132"/>
-      <c r="Z11" s="132"/>
-      <c r="AA11" s="132"/>
-      <c r="AB11" s="132"/>
-      <c r="AC11" s="132"/>
-      <c r="AD11" s="132"/>
-      <c r="AE11" s="132"/>
-      <c r="AF11" s="132"/>
+      <c r="V11" s="131"/>
+      <c r="W11" s="133"/>
+      <c r="X11" s="128"/>
+      <c r="Y11" s="128"/>
+      <c r="Z11" s="128"/>
+      <c r="AA11" s="128"/>
+      <c r="AB11" s="128"/>
+      <c r="AC11" s="128"/>
+      <c r="AD11" s="128"/>
+      <c r="AE11" s="128"/>
+      <c r="AF11" s="128"/>
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
@@ -4566,7 +4606,7 @@
       <c r="BH11" s="1"/>
       <c r="BI11" s="1"/>
       <c r="BJ11" s="1"/>
-      <c r="DR11" s="134"/>
+      <c r="DR11" s="130"/>
       <c r="DS11" s="1"/>
       <c r="DT11" s="1"/>
       <c r="DU11" s="1"/>
@@ -4580,26 +4620,26 @@
       <c r="EV11" s="22"/>
     </row>
     <row r="12" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="134"/>
+      <c r="B12" s="130"/>
       <c r="L12" s="2"/>
       <c r="V12" s="26"/>
-      <c r="AF12" s="133"/>
+      <c r="AF12" s="129"/>
       <c r="AI12" s="41"/>
       <c r="AK12" s="41"/>
       <c r="AM12" s="41"/>
       <c r="AO12" s="41"/>
       <c r="AP12" s="26"/>
-      <c r="AZ12" s="115"/>
+      <c r="AZ12" s="113"/>
       <c r="BJ12" s="26"/>
-      <c r="DR12" s="134"/>
+      <c r="DR12" s="130"/>
       <c r="EB12" s="2"/>
       <c r="EV12" s="22"/>
     </row>
     <row r="13" spans="1:152" x14ac:dyDescent="0.3">
-      <c r="B13" s="134"/>
+      <c r="B13" s="130"/>
       <c r="L13" s="2"/>
       <c r="V13" s="22"/>
-      <c r="AF13" s="134"/>
+      <c r="AF13" s="130"/>
       <c r="AH13" s="49"/>
       <c r="AJ13" s="49"/>
       <c r="AL13" s="49"/>
@@ -4610,12 +4650,12 @@
       </c>
       <c r="AZ13" s="2"/>
       <c r="BJ13" s="22"/>
-      <c r="DR13" s="134"/>
+      <c r="DR13" s="130"/>
       <c r="EB13" s="2"/>
       <c r="EV13" s="22"/>
     </row>
     <row r="14" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="134"/>
+      <c r="B14" s="130"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -4645,7 +4685,7 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
-      <c r="AF14" s="135"/>
+      <c r="AF14" s="131"/>
       <c r="AG14" s="40"/>
       <c r="AH14" s="1"/>
       <c r="AI14" s="40"/>
@@ -4657,26 +4697,15 @@
       <c r="AO14" s="40"/>
       <c r="AP14" s="27"/>
       <c r="AQ14" s="23"/>
-      <c r="AR14" s="109"/>
       <c r="AS14" s="1"/>
       <c r="AT14" s="1"/>
-      <c r="AU14" s="109"/>
-      <c r="AV14" s="109"/>
-      <c r="AW14" s="109"/>
-      <c r="AX14" s="109"/>
-      <c r="AY14" s="109"/>
       <c r="AZ14" s="2"/>
-      <c r="BA14" s="109"/>
-      <c r="BB14" s="109"/>
-      <c r="BC14" s="109"/>
       <c r="BD14" s="1"/>
       <c r="BE14" s="1"/>
-      <c r="BF14" s="109"/>
-      <c r="BG14" s="109"/>
       <c r="BH14" s="1"/>
       <c r="BI14" s="1"/>
       <c r="BJ14" s="22"/>
-      <c r="DR14" s="134"/>
+      <c r="DR14" s="130"/>
       <c r="DS14" s="1"/>
       <c r="DT14" s="1"/>
       <c r="DU14" s="1"/>
@@ -4690,7 +4719,7 @@
       <c r="EV14" s="22"/>
     </row>
     <row r="15" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="134"/>
+      <c r="B15" s="130"/>
       <c r="L15" s="2"/>
       <c r="V15" s="22"/>
       <c r="W15" s="87"/>
@@ -4698,26 +4727,26 @@
       <c r="AA15" s="41"/>
       <c r="AC15" s="41"/>
       <c r="AE15" s="41"/>
-      <c r="AF15" s="134"/>
+      <c r="AF15" s="130"/>
       <c r="AP15" s="22"/>
       <c r="AS15" s="26"/>
       <c r="AT15" s="81"/>
       <c r="AZ15" s="2"/>
       <c r="BD15" s="26"/>
       <c r="BJ15" s="22"/>
-      <c r="DR15" s="134"/>
+      <c r="DR15" s="130"/>
       <c r="EB15" s="2"/>
       <c r="EV15" s="22"/>
     </row>
     <row r="16" spans="1:152" x14ac:dyDescent="0.3">
-      <c r="B16" s="134"/>
+      <c r="B16" s="130"/>
       <c r="L16" s="2"/>
       <c r="V16" s="22"/>
       <c r="X16" s="49"/>
       <c r="Z16" s="49"/>
       <c r="AB16" s="49"/>
       <c r="AD16" s="49"/>
-      <c r="AF16" s="138"/>
+      <c r="AF16" s="134"/>
       <c r="AP16" s="22"/>
       <c r="AS16" s="22"/>
       <c r="AT16" s="12"/>
@@ -4727,12 +4756,12 @@
       <c r="AZ16" s="2"/>
       <c r="BD16" s="22"/>
       <c r="BJ16" s="22"/>
-      <c r="DR16" s="134"/>
+      <c r="DR16" s="130"/>
       <c r="EB16" s="2"/>
       <c r="EV16" s="22"/>
     </row>
     <row r="17" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="134"/>
+      <c r="B17" s="130"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -4762,21 +4791,11 @@
       <c r="AC17" s="40"/>
       <c r="AD17" s="1"/>
       <c r="AE17" s="40"/>
-      <c r="AF17" s="135"/>
-      <c r="AG17" s="109"/>
-      <c r="AH17" s="109"/>
-      <c r="AI17" s="109"/>
-      <c r="AJ17" s="109"/>
-      <c r="AK17" s="109"/>
-      <c r="AL17" s="109"/>
-      <c r="AM17" s="109"/>
-      <c r="AN17" s="109"/>
-      <c r="AO17" s="109"/>
+      <c r="AF17" s="131"/>
       <c r="AP17" s="22"/>
       <c r="AQ17" s="23"/>
-      <c r="AR17" s="109"/>
       <c r="AS17" s="27"/>
-      <c r="AT17" s="116"/>
+      <c r="AT17" s="114"/>
       <c r="AU17" s="1"/>
       <c r="AV17" s="1"/>
       <c r="AW17" s="1"/>
@@ -4788,12 +4807,9 @@
       <c r="BC17" s="1"/>
       <c r="BD17" s="27"/>
       <c r="BE17" s="23"/>
-      <c r="BF17" s="109"/>
-      <c r="BG17" s="109"/>
-      <c r="BH17" s="109"/>
       <c r="BI17" s="1"/>
       <c r="BJ17" s="27"/>
-      <c r="DR17" s="134"/>
+      <c r="DR17" s="130"/>
       <c r="DS17" s="1"/>
       <c r="DT17" s="1"/>
       <c r="DU17" s="1"/>
@@ -4807,11 +4823,11 @@
       <c r="EV17" s="22"/>
     </row>
     <row r="18" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="134"/>
+      <c r="B18" s="130"/>
       <c r="L18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="107"/>
-      <c r="AF18" s="136"/>
+      <c r="AF18" s="132"/>
       <c r="AP18" s="22"/>
       <c r="AZ18" s="26"/>
       <c r="BA18" s="87"/>
@@ -4820,12 +4836,12 @@
       <c r="BH18" s="22"/>
       <c r="BI18" s="87"/>
       <c r="BJ18" s="26"/>
-      <c r="DR18" s="134"/>
+      <c r="DR18" s="130"/>
       <c r="EB18" s="2"/>
       <c r="EV18" s="22"/>
     </row>
     <row r="19" spans="1:152" x14ac:dyDescent="0.3">
-      <c r="B19" s="134"/>
+      <c r="B19" s="130"/>
       <c r="L19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="108"/>
@@ -4839,42 +4855,42 @@
       <c r="BD19" s="37"/>
       <c r="BH19" s="22"/>
       <c r="BJ19" s="37"/>
-      <c r="DR19" s="134"/>
+      <c r="DR19" s="130"/>
       <c r="EB19" s="2"/>
       <c r="EV19" s="22"/>
     </row>
     <row r="20" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="134"/>
-      <c r="C20" s="132"/>
-      <c r="D20" s="132"/>
-      <c r="E20" s="132"/>
-      <c r="F20" s="132"/>
-      <c r="G20" s="132"/>
-      <c r="H20" s="132"/>
-      <c r="I20" s="132"/>
-      <c r="J20" s="132"/>
-      <c r="K20" s="132"/>
-      <c r="L20" s="140"/>
-      <c r="M20" s="139"/>
-      <c r="N20" s="132"/>
-      <c r="O20" s="132"/>
-      <c r="P20" s="132"/>
-      <c r="Q20" s="132"/>
-      <c r="R20" s="132"/>
-      <c r="S20" s="132"/>
-      <c r="T20" s="132"/>
-      <c r="U20" s="132"/>
-      <c r="V20" s="140"/>
-      <c r="W20" s="141"/>
-      <c r="X20" s="132"/>
-      <c r="Y20" s="132"/>
-      <c r="Z20" s="132"/>
-      <c r="AA20" s="132"/>
-      <c r="AB20" s="132"/>
-      <c r="AC20" s="132"/>
-      <c r="AD20" s="132"/>
-      <c r="AE20" s="132"/>
-      <c r="AF20" s="142"/>
+      <c r="B20" s="130"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="128"/>
+      <c r="F20" s="128"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="128"/>
+      <c r="I20" s="128"/>
+      <c r="J20" s="128"/>
+      <c r="K20" s="128"/>
+      <c r="L20" s="136"/>
+      <c r="M20" s="135"/>
+      <c r="N20" s="128"/>
+      <c r="O20" s="128"/>
+      <c r="P20" s="128"/>
+      <c r="Q20" s="128"/>
+      <c r="R20" s="128"/>
+      <c r="S20" s="128"/>
+      <c r="T20" s="128"/>
+      <c r="U20" s="128"/>
+      <c r="V20" s="136"/>
+      <c r="W20" s="137"/>
+      <c r="X20" s="128"/>
+      <c r="Y20" s="128"/>
+      <c r="Z20" s="128"/>
+      <c r="AA20" s="128"/>
+      <c r="AB20" s="128"/>
+      <c r="AC20" s="128"/>
+      <c r="AD20" s="128"/>
+      <c r="AE20" s="128"/>
+      <c r="AF20" s="138"/>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
@@ -4899,9 +4915,9 @@
       <c r="BB20" s="1"/>
       <c r="BC20" s="40"/>
       <c r="BD20" s="27"/>
-      <c r="BE20" s="118"/>
-      <c r="BF20" s="119"/>
-      <c r="BG20" s="117"/>
+      <c r="BE20" s="116"/>
+      <c r="BF20" s="117"/>
+      <c r="BG20" s="115"/>
       <c r="BH20" s="27"/>
       <c r="BI20" s="48"/>
       <c r="BJ20" s="27"/>
@@ -4945,7 +4961,7 @@
       <c r="CV20" s="1"/>
       <c r="CW20" s="1"/>
       <c r="CX20" s="1"/>
-      <c r="DR20" s="134"/>
+      <c r="DR20" s="130"/>
       <c r="DS20" s="1"/>
       <c r="DT20" s="1"/>
       <c r="DU20" s="1"/>
@@ -4967,7 +4983,6 @@
       <c r="V21" s="2"/>
       <c r="Y21" s="53"/>
       <c r="Z21" s="49"/>
-      <c r="AA21" s="109"/>
       <c r="AB21" s="49"/>
       <c r="AC21" s="22"/>
       <c r="AD21" s="48"/>
@@ -4999,7 +5014,7 @@
       <c r="CF21" s="26"/>
       <c r="CN21" s="2"/>
       <c r="CX21" s="22"/>
-      <c r="DR21" s="134"/>
+      <c r="DR21" s="130"/>
       <c r="EB21" s="2"/>
       <c r="EV21" s="22"/>
     </row>
@@ -5014,13 +5029,13 @@
       <c r="AA22" s="40"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="94"/>
-      <c r="AD22" s="150" t="s">
+      <c r="AD22" s="146" t="s">
         <v>25</v>
       </c>
-      <c r="AE22" s="150" t="s">
+      <c r="AE22" s="146" t="s">
         <v>25</v>
       </c>
-      <c r="AF22" s="151" t="s">
+      <c r="AF22" s="147" t="s">
         <v>25</v>
       </c>
       <c r="AG22" s="48"/>
@@ -5047,7 +5062,7 @@
       <c r="CF22" s="37"/>
       <c r="CN22" s="2"/>
       <c r="CX22" s="22"/>
-      <c r="DR22" s="134"/>
+      <c r="DR22" s="130"/>
       <c r="EB22" s="2"/>
       <c r="EV22" s="22"/>
     </row>
@@ -5060,7 +5075,7 @@
       <c r="M23" s="44"/>
       <c r="V23" s="2"/>
       <c r="W23" s="28"/>
-      <c r="AA23" s="150" t="s">
+      <c r="AA23" s="146" t="s">
         <v>25</v>
       </c>
       <c r="AC23" s="22"/>
@@ -5073,9 +5088,6 @@
       <c r="AP23" s="94"/>
       <c r="AQ23" s="1"/>
       <c r="AR23" s="1"/>
-      <c r="AS23" s="109"/>
-      <c r="AT23" s="109"/>
-      <c r="AU23" s="109"/>
       <c r="AV23" s="1"/>
       <c r="AW23" s="1"/>
       <c r="AX23" s="1"/>
@@ -5083,22 +5095,15 @@
       <c r="AZ23" s="27"/>
       <c r="BA23" s="23"/>
       <c r="BB23" s="49"/>
-      <c r="BC23" s="109"/>
       <c r="BD23" s="94"/>
-      <c r="BE23" s="109"/>
-      <c r="BF23" s="109"/>
       <c r="BG23" s="1"/>
       <c r="BH23" s="1"/>
       <c r="BI23" s="1"/>
       <c r="BJ23" s="27"/>
       <c r="BK23" s="93"/>
-      <c r="BL23" s="109"/>
       <c r="BM23" s="49"/>
-      <c r="BN23" s="109"/>
       <c r="BO23" s="49"/>
-      <c r="BP23" s="109"/>
       <c r="BQ23" s="49"/>
-      <c r="BR23" s="109"/>
       <c r="BS23" s="49"/>
       <c r="BT23" s="22"/>
       <c r="BU23" s="48"/>
@@ -5113,8 +5118,6 @@
       <c r="CD23" s="27"/>
       <c r="CE23" s="48"/>
       <c r="CF23" s="27"/>
-      <c r="CG23" s="109"/>
-      <c r="CH23" s="109"/>
       <c r="CI23" s="1"/>
       <c r="CJ23" s="1"/>
       <c r="CK23" s="1"/>
@@ -5126,14 +5129,8 @@
       <c r="CQ23" s="14">
         <v>2</v>
       </c>
-      <c r="CR23" s="109"/>
-      <c r="CS23" s="109"/>
-      <c r="CT23" s="109"/>
-      <c r="CU23" s="109"/>
-      <c r="CV23" s="109"/>
-      <c r="CW23" s="109"/>
       <c r="CX23" s="22"/>
-      <c r="DR23" s="134"/>
+      <c r="DR23" s="130"/>
       <c r="DS23" s="1"/>
       <c r="DT23" s="1"/>
       <c r="DU23" s="1"/>
@@ -5181,7 +5178,7 @@
       <c r="CO24" s="87"/>
       <c r="CQ24" s="42"/>
       <c r="CX24" s="22"/>
-      <c r="DR24" s="134"/>
+      <c r="DR24" s="130"/>
       <c r="EB24" s="2"/>
       <c r="EV24" s="22"/>
     </row>
@@ -5216,7 +5213,7 @@
       <c r="CP25" s="49"/>
       <c r="CQ25" s="22"/>
       <c r="CX25" s="22"/>
-      <c r="DR25" s="134"/>
+      <c r="DR25" s="130"/>
       <c r="EB25" s="2"/>
       <c r="EV25" s="22"/>
     </row>
@@ -5260,12 +5257,6 @@
       <c r="BA26" s="48"/>
       <c r="BB26" s="1"/>
       <c r="BC26" s="94"/>
-      <c r="BD26" s="109"/>
-      <c r="BE26" s="109"/>
-      <c r="BF26" s="109"/>
-      <c r="BG26" s="109"/>
-      <c r="BH26" s="109"/>
-      <c r="BI26" s="109"/>
       <c r="BJ26" s="22"/>
       <c r="BK26" s="1"/>
       <c r="BL26" s="40"/>
@@ -5279,17 +5270,17 @@
       <c r="BT26" s="94"/>
       <c r="BU26" s="1"/>
       <c r="BW26" s="1"/>
-      <c r="BX26" s="120"/>
-      <c r="BY26" s="123" t="s">
+      <c r="BX26" s="118"/>
+      <c r="BY26" s="121" t="s">
         <v>47</v>
       </c>
-      <c r="BZ26" s="121" t="s">
+      <c r="BZ26" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="CA26" s="121" t="s">
+      <c r="CA26" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="CB26" s="122" t="s">
+      <c r="CB26" s="120" t="s">
         <v>47</v>
       </c>
       <c r="CC26" s="90"/>
@@ -5299,36 +5290,33 @@
       <c r="CG26" s="1"/>
       <c r="CH26" s="27"/>
       <c r="CI26" s="93"/>
-      <c r="CJ26" s="109"/>
       <c r="CK26" s="49"/>
-      <c r="CL26" s="109"/>
       <c r="CM26" s="49"/>
       <c r="CN26" s="22"/>
       <c r="CO26" s="93"/>
-      <c r="CP26" s="109"/>
       <c r="CQ26" s="37"/>
-      <c r="CR26" s="153" t="s">
+      <c r="CR26" s="149" t="s">
         <v>47</v>
       </c>
-      <c r="CS26" s="121" t="s">
+      <c r="CS26" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="CT26" s="121" t="s">
+      <c r="CT26" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="CU26" s="121" t="s">
+      <c r="CU26" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="CV26" s="154" t="s">
+      <c r="CV26" s="150" t="s">
         <v>47</v>
       </c>
-      <c r="CW26" s="154" t="s">
+      <c r="CW26" s="150" t="s">
         <v>47</v>
       </c>
-      <c r="CX26" s="155" t="s">
+      <c r="CX26" s="151" t="s">
         <v>47</v>
       </c>
-      <c r="DR26" s="134"/>
+      <c r="DR26" s="130"/>
       <c r="DS26" s="1"/>
       <c r="DT26" s="1"/>
       <c r="DU26" s="1"/>
@@ -5381,7 +5369,7 @@
       <c r="BJ27" s="22"/>
       <c r="BT27" s="2"/>
       <c r="BW27" s="26"/>
-      <c r="BY27" s="124"/>
+      <c r="BY27" s="122"/>
       <c r="BZ27" s="87"/>
       <c r="CA27" s="29"/>
       <c r="CB27" s="41"/>
@@ -5397,7 +5385,7 @@
         <v>2</v>
       </c>
       <c r="CX27" s="22"/>
-      <c r="DR27" s="134"/>
+      <c r="DR27" s="130"/>
       <c r="EB27" s="2"/>
       <c r="EV27" s="22"/>
     </row>
@@ -5426,7 +5414,7 @@
       <c r="AP28" s="99"/>
       <c r="AQ28" s="15"/>
       <c r="AR28" s="15"/>
-      <c r="AS28" s="114"/>
+      <c r="AS28" s="15"/>
       <c r="AT28" s="15"/>
       <c r="AU28" s="15"/>
       <c r="AV28" s="15"/>
@@ -5455,7 +5443,7 @@
       <c r="CQ28" s="40"/>
       <c r="CR28" s="27"/>
       <c r="CX28" s="22"/>
-      <c r="DR28" s="134"/>
+      <c r="DR28" s="130"/>
       <c r="EB28" s="2"/>
       <c r="EV28" s="22"/>
     </row>
@@ -5523,20 +5511,20 @@
       <c r="BH29" s="1"/>
       <c r="BI29" s="1"/>
       <c r="BJ29" s="61"/>
-      <c r="BK29" s="146"/>
-      <c r="BL29" s="132"/>
-      <c r="BM29" s="132"/>
-      <c r="BN29" s="132"/>
-      <c r="BO29" s="132"/>
-      <c r="BP29" s="147"/>
-      <c r="BQ29" s="132"/>
-      <c r="BR29" s="132"/>
-      <c r="BS29" s="132"/>
-      <c r="BT29" s="140"/>
+      <c r="BK29" s="142"/>
+      <c r="BL29" s="128"/>
+      <c r="BM29" s="128"/>
+      <c r="BN29" s="128"/>
+      <c r="BO29" s="128"/>
+      <c r="BP29" s="143"/>
+      <c r="BQ29" s="128"/>
+      <c r="BR29" s="128"/>
+      <c r="BS29" s="128"/>
+      <c r="BT29" s="136"/>
       <c r="BU29" s="1"/>
       <c r="BV29" s="1"/>
       <c r="BW29" s="27"/>
-      <c r="BX29" s="125"/>
+      <c r="BX29" s="123"/>
       <c r="BY29" s="35"/>
       <c r="BZ29" s="48"/>
       <c r="CA29" s="1"/>
@@ -5553,7 +5541,7 @@
       <c r="CL29" s="40"/>
       <c r="CM29" s="1"/>
       <c r="CN29" s="94"/>
-      <c r="CO29" s="156"/>
+      <c r="CO29" s="152"/>
       <c r="CP29" s="4"/>
       <c r="CQ29" s="1"/>
       <c r="CR29" s="1"/>
@@ -5563,7 +5551,7 @@
       <c r="CV29" s="1"/>
       <c r="CW29" s="54"/>
       <c r="CX29" s="89"/>
-      <c r="DR29" s="134"/>
+      <c r="DR29" s="130"/>
       <c r="DS29" s="1"/>
       <c r="DT29" s="1"/>
       <c r="DU29" s="1"/>
@@ -5577,13 +5565,13 @@
       <c r="EV29" s="22"/>
     </row>
     <row r="30" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="BJ30" s="136"/>
+      <c r="BJ30" s="132"/>
       <c r="BK30" s="49"/>
       <c r="BM30" s="49"/>
       <c r="BO30" s="49"/>
       <c r="BQ30" s="49"/>
       <c r="BS30" s="49"/>
-      <c r="BT30" s="133"/>
+      <c r="BT30" s="129"/>
       <c r="CA30" s="22"/>
       <c r="CC30" s="41"/>
       <c r="CD30" s="26"/>
@@ -5595,18 +5583,18 @@
       <c r="CS30" s="41"/>
       <c r="CU30" s="41"/>
       <c r="CV30" s="26"/>
-      <c r="CX30" s="157"/>
-      <c r="DR30" s="134"/>
+      <c r="CX30" s="153"/>
+      <c r="DR30" s="130"/>
       <c r="EB30" s="2"/>
       <c r="EV30" s="22"/>
     </row>
     <row r="31" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BJ31" s="134"/>
+      <c r="BJ31" s="130"/>
       <c r="BL31" s="49"/>
       <c r="BN31" s="49"/>
       <c r="BP31" s="49"/>
       <c r="BR31" s="49"/>
-      <c r="BT31" s="138"/>
+      <c r="BT31" s="134"/>
       <c r="CA31" s="22"/>
       <c r="CB31" s="93"/>
       <c r="CD31" s="37"/>
@@ -5618,12 +5606,12 @@
       <c r="CT31" s="49"/>
       <c r="CV31" s="37"/>
       <c r="CX31" s="22"/>
-      <c r="DR31" s="134"/>
+      <c r="DR31" s="130"/>
       <c r="EB31" s="2"/>
       <c r="EV31" s="22"/>
     </row>
     <row r="32" spans="1:152" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BJ32" s="134"/>
+      <c r="BJ32" s="130"/>
       <c r="BK32" s="40"/>
       <c r="BL32" s="1"/>
       <c r="BM32" s="40"/>
@@ -5633,10 +5621,7 @@
       <c r="BQ32" s="40"/>
       <c r="BR32" s="1"/>
       <c r="BS32" s="40"/>
-      <c r="BT32" s="135"/>
-      <c r="BU32" s="109"/>
-      <c r="BV32" s="109"/>
-      <c r="BW32" s="109"/>
+      <c r="BT32" s="131"/>
       <c r="BX32" s="1"/>
       <c r="BY32" s="1"/>
       <c r="BZ32" s="1"/>
@@ -5645,16 +5630,13 @@
       <c r="CC32" s="49"/>
       <c r="CD32" s="22"/>
       <c r="CE32" s="23"/>
-      <c r="CF32" s="109"/>
-      <c r="CG32" s="109"/>
-      <c r="CH32" s="109"/>
       <c r="CI32" s="1"/>
       <c r="CJ32" s="1"/>
       <c r="CK32" s="1"/>
       <c r="CL32" s="1"/>
       <c r="CM32" s="1"/>
       <c r="CN32" s="3"/>
-      <c r="CO32" s="110"/>
+      <c r="CO32" s="109"/>
       <c r="CP32" s="27"/>
       <c r="CQ32" s="48"/>
       <c r="CR32" s="1"/>
@@ -5664,7 +5646,7 @@
       <c r="CV32" s="27"/>
       <c r="CW32" s="1"/>
       <c r="CX32" s="27"/>
-      <c r="DR32" s="134"/>
+      <c r="DR32" s="130"/>
       <c r="DS32" s="1"/>
       <c r="DT32" s="1"/>
       <c r="DU32" s="1"/>
@@ -5678,25 +5660,23 @@
       <c r="EV32" s="22"/>
     </row>
     <row r="33" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="BJ33" s="134"/>
-      <c r="BT33" s="134"/>
+      <c r="BJ33" s="130"/>
+      <c r="BT33" s="130"/>
       <c r="BW33" s="22"/>
       <c r="BX33" s="87"/>
       <c r="BZ33" s="41"/>
       <c r="CB33" s="49"/>
       <c r="CD33" s="37"/>
       <c r="CL33" s="64"/>
-      <c r="CN33" s="115"/>
-      <c r="CV33" s="109"/>
-      <c r="CW33" s="109"/>
+      <c r="CN33" s="113"/>
       <c r="CX33" s="22"/>
-      <c r="DR33" s="134"/>
+      <c r="DR33" s="130"/>
       <c r="EB33" s="2"/>
       <c r="EV33" s="22"/>
     </row>
     <row r="34" spans="62:172" x14ac:dyDescent="0.3">
-      <c r="BJ34" s="134"/>
-      <c r="BT34" s="134"/>
+      <c r="BJ34" s="130"/>
+      <c r="BT34" s="130"/>
       <c r="BW34" s="22"/>
       <c r="BX34" s="23"/>
       <c r="BY34" s="49"/>
@@ -5704,47 +5684,32 @@
       <c r="CC34" s="49"/>
       <c r="CD34" s="22"/>
       <c r="CL34" s="65"/>
-      <c r="CM34" s="161">
+      <c r="CM34" s="157">
         <v>3</v>
       </c>
       <c r="CN34" s="2"/>
-      <c r="CV34" s="109"/>
-      <c r="CW34" s="109"/>
       <c r="CX34" s="22"/>
-      <c r="DR34" s="134"/>
+      <c r="DR34" s="130"/>
       <c r="EB34" s="2"/>
       <c r="EV34" s="22"/>
     </row>
     <row r="35" spans="62:172" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BJ35" s="134"/>
-      <c r="BK35" s="109"/>
-      <c r="BL35" s="109"/>
-      <c r="BM35" s="109"/>
-      <c r="BN35" s="109"/>
-      <c r="BO35" s="109"/>
-      <c r="BP35" s="109"/>
-      <c r="BQ35" s="127" t="s">
+      <c r="BJ35" s="130"/>
+      <c r="BQ35" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="BR35" s="109"/>
-      <c r="BS35" s="109"/>
-      <c r="BT35" s="134"/>
-      <c r="BU35" s="109"/>
-      <c r="BV35" s="109"/>
+      <c r="BT35" s="130"/>
       <c r="BW35" s="22"/>
       <c r="BX35" s="93"/>
-      <c r="BY35" s="109"/>
       <c r="BZ35" s="49"/>
-      <c r="CA35" s="109"/>
       <c r="CB35" s="49"/>
-      <c r="CC35" s="109"/>
       <c r="CD35" s="37"/>
       <c r="CE35" s="1"/>
       <c r="CF35" s="77">
         <v>3</v>
       </c>
       <c r="CG35" s="1"/>
-      <c r="CH35" s="158"/>
+      <c r="CH35" s="154"/>
       <c r="CI35" s="1"/>
       <c r="CJ35" s="1"/>
       <c r="CK35" s="1"/>
@@ -5753,15 +5718,11 @@
       <c r="CN35" s="3"/>
       <c r="CO35" s="1"/>
       <c r="CP35" s="1"/>
-      <c r="CQ35" s="109"/>
-      <c r="CR35" s="109"/>
       <c r="CS35" s="1"/>
       <c r="CT35" s="1"/>
       <c r="CU35" s="1"/>
-      <c r="CV35" s="109"/>
-      <c r="CW35" s="109"/>
       <c r="CX35" s="27"/>
-      <c r="DR35" s="134"/>
+      <c r="DR35" s="130"/>
       <c r="DS35" s="1"/>
       <c r="DT35" s="1"/>
       <c r="DU35" s="1"/>
@@ -5775,8 +5736,8 @@
       <c r="EV35" s="22"/>
     </row>
     <row r="36" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="BJ36" s="134"/>
-      <c r="BT36" s="134"/>
+      <c r="BJ36" s="130"/>
+      <c r="BT36" s="130"/>
       <c r="BW36" s="22"/>
       <c r="BX36" s="23"/>
       <c r="BY36" s="49"/>
@@ -5784,17 +5745,15 @@
       <c r="CC36" s="49"/>
       <c r="CD36" s="22"/>
       <c r="CN36" s="2"/>
-      <c r="CR36" s="109"/>
-      <c r="CS36" s="109"/>
       <c r="CU36" s="26"/>
       <c r="CW36" s="22"/>
       <c r="CX36" s="45"/>
-      <c r="DR36" s="134"/>
+      <c r="DR36" s="130"/>
       <c r="EB36" s="2"/>
       <c r="EV36" s="22"/>
     </row>
     <row r="37" spans="62:172" x14ac:dyDescent="0.3">
-      <c r="BJ37" s="134"/>
+      <c r="BJ37" s="130"/>
       <c r="BT37" s="60"/>
       <c r="BW37" s="22"/>
       <c r="BX37" s="93"/>
@@ -5802,13 +5761,10 @@
       <c r="CB37" s="49"/>
       <c r="CD37" s="37"/>
       <c r="CN37" s="2"/>
-      <c r="CR37" s="109"/>
-      <c r="CS37" s="109"/>
-      <c r="CT37" s="109"/>
       <c r="CU37" s="22"/>
       <c r="CW37" s="22"/>
       <c r="CX37" s="22"/>
-      <c r="DR37" s="134"/>
+      <c r="DR37" s="130"/>
       <c r="DX37" s="50" t="s">
         <v>32</v>
       </c>
@@ -5816,10 +5772,10 @@
       <c r="EV37" s="22"/>
     </row>
     <row r="38" spans="62:172" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BJ38" s="134"/>
+      <c r="BJ38" s="130"/>
       <c r="BK38" s="1"/>
-      <c r="BL38" s="131"/>
-      <c r="BM38" s="131"/>
+      <c r="BL38" s="127"/>
+      <c r="BM38" s="127"/>
       <c r="BN38" s="1"/>
       <c r="BO38" s="1"/>
       <c r="BP38" s="1"/>
@@ -5827,30 +5783,30 @@
       <c r="BR38" s="57"/>
       <c r="BS38" s="1"/>
       <c r="BT38" s="61"/>
-      <c r="BU38" s="132"/>
-      <c r="BV38" s="132"/>
-      <c r="BW38" s="145"/>
-      <c r="BX38" s="143"/>
-      <c r="BY38" s="148"/>
-      <c r="BZ38" s="132"/>
-      <c r="CA38" s="148"/>
-      <c r="CB38" s="132"/>
-      <c r="CC38" s="148"/>
-      <c r="CD38" s="145"/>
-      <c r="CE38" s="143"/>
+      <c r="BU38" s="128"/>
+      <c r="BV38" s="128"/>
+      <c r="BW38" s="141"/>
+      <c r="BX38" s="139"/>
+      <c r="BY38" s="144"/>
+      <c r="BZ38" s="128"/>
+      <c r="CA38" s="144"/>
+      <c r="CB38" s="128"/>
+      <c r="CC38" s="144"/>
+      <c r="CD38" s="141"/>
+      <c r="CE38" s="139"/>
       <c r="CF38" s="84"/>
-      <c r="CG38" s="132"/>
-      <c r="CH38" s="132"/>
-      <c r="CI38" s="132"/>
-      <c r="CJ38" s="132"/>
-      <c r="CK38" s="158"/>
-      <c r="CL38" s="132"/>
-      <c r="CM38" s="132"/>
-      <c r="CN38" s="140"/>
-      <c r="CO38" s="110"/>
+      <c r="CG38" s="128"/>
+      <c r="CH38" s="128"/>
+      <c r="CI38" s="128"/>
+      <c r="CJ38" s="128"/>
+      <c r="CK38" s="154"/>
+      <c r="CL38" s="128"/>
+      <c r="CM38" s="128"/>
+      <c r="CN38" s="136"/>
+      <c r="CO38" s="109"/>
       <c r="CP38" s="1"/>
       <c r="CQ38" s="85"/>
-      <c r="CR38" s="162">
+      <c r="CR38" s="158">
         <v>4</v>
       </c>
       <c r="CS38" s="1"/>
@@ -5878,17 +5834,17 @@
       <c r="DO38" s="1"/>
       <c r="DP38" s="1"/>
       <c r="DQ38" s="1"/>
-      <c r="DR38" s="135"/>
-      <c r="DS38" s="137"/>
-      <c r="DT38" s="132"/>
-      <c r="DU38" s="132"/>
-      <c r="DV38" s="132"/>
-      <c r="DW38" s="132"/>
-      <c r="DX38" s="132"/>
-      <c r="DY38" s="132"/>
-      <c r="DZ38" s="132"/>
-      <c r="EA38" s="132"/>
-      <c r="EB38" s="140"/>
+      <c r="DR38" s="131"/>
+      <c r="DS38" s="133"/>
+      <c r="DT38" s="128"/>
+      <c r="DU38" s="128"/>
+      <c r="DV38" s="128"/>
+      <c r="DW38" s="128"/>
+      <c r="DX38" s="128"/>
+      <c r="DY38" s="128"/>
+      <c r="DZ38" s="128"/>
+      <c r="EA38" s="128"/>
+      <c r="EB38" s="136"/>
       <c r="EC38" s="1"/>
       <c r="ED38" s="1"/>
       <c r="EE38" s="1"/>
@@ -5931,10 +5887,10 @@
       <c r="FP38" s="1"/>
     </row>
     <row r="39" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="BJ39" s="134"/>
+      <c r="BJ39" s="130"/>
       <c r="BT39" s="2"/>
       <c r="CD39" s="2"/>
-      <c r="CN39" s="134"/>
+      <c r="CN39" s="130"/>
       <c r="CO39" s="15"/>
       <c r="CP39" s="45"/>
       <c r="CW39" s="22"/>
@@ -5948,15 +5904,18 @@
       <c r="FP39" s="26"/>
     </row>
     <row r="40" spans="62:172" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BJ40" s="134"/>
+      <c r="BJ40" s="130"/>
       <c r="BT40" s="2"/>
       <c r="CD40" s="2"/>
       <c r="CN40" s="60"/>
       <c r="CO40" s="15"/>
-      <c r="CP40" s="156"/>
+      <c r="CP40" s="152"/>
       <c r="CW40" s="22"/>
       <c r="CX40" s="44"/>
       <c r="DH40" s="22"/>
+      <c r="DL40" s="47" t="s">
+        <v>56</v>
+      </c>
       <c r="DR40" s="2"/>
       <c r="EB40" s="2"/>
       <c r="EL40" s="2"/>
@@ -5965,7 +5924,7 @@
       <c r="FP40" s="22"/>
     </row>
     <row r="41" spans="62:172" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BJ41" s="134"/>
+      <c r="BJ41" s="130"/>
       <c r="BK41" s="1"/>
       <c r="BL41" s="1"/>
       <c r="BM41" s="1"/>
@@ -5998,25 +5957,15 @@
       <c r="CN41" s="61"/>
       <c r="CO41" s="90"/>
       <c r="CP41" s="90"/>
-      <c r="CQ41" s="109"/>
-      <c r="CR41" s="109"/>
       <c r="CT41" s="1"/>
       <c r="CU41" s="1"/>
       <c r="CV41" s="1"/>
       <c r="CW41" s="27"/>
       <c r="CX41" s="27"/>
       <c r="CY41" s="23"/>
-      <c r="CZ41" s="109"/>
-      <c r="DA41" s="109"/>
-      <c r="DB41" s="109"/>
-      <c r="DC41" s="109"/>
-      <c r="DD41" s="109"/>
-      <c r="DE41" s="109"/>
-      <c r="DF41" s="109"/>
-      <c r="DG41" s="109"/>
       <c r="DH41" s="22"/>
       <c r="DI41" s="1"/>
-      <c r="DJ41" s="1"/>
+      <c r="DJ41" s="166"/>
       <c r="DK41" s="1"/>
       <c r="DL41" s="1"/>
       <c r="DM41" s="1"/>
@@ -6055,37 +6004,25 @@
       <c r="ET41" s="1"/>
       <c r="EU41" s="1"/>
       <c r="EV41" s="27"/>
-      <c r="EW41" s="109"/>
-      <c r="EX41" s="109"/>
-      <c r="EY41" s="109"/>
-      <c r="EZ41" s="109"/>
-      <c r="FA41" s="109"/>
-      <c r="FB41" s="109"/>
-      <c r="FC41" s="109"/>
-      <c r="FD41" s="109"/>
-      <c r="FE41" s="109"/>
       <c r="FF41" s="22"/>
       <c r="FG41" s="23"/>
-      <c r="FH41" s="109"/>
-      <c r="FI41" s="109"/>
-      <c r="FJ41" s="109"/>
-      <c r="FK41" s="109"/>
-      <c r="FL41" s="109"/>
-      <c r="FM41" s="109"/>
-      <c r="FN41" s="109"/>
-      <c r="FO41" s="109"/>
       <c r="FP41" s="22"/>
     </row>
     <row r="42" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="BJ42" s="134"/>
+      <c r="BJ42" s="130"/>
       <c r="BT42" s="2"/>
       <c r="CD42" s="2"/>
-      <c r="CN42" s="134"/>
-      <c r="CO42" s="159"/>
+      <c r="CN42" s="130"/>
+      <c r="CO42" s="155"/>
       <c r="CP42" s="26"/>
       <c r="CX42" s="26"/>
       <c r="DH42" s="22"/>
-      <c r="DR42" s="2"/>
+      <c r="DI42" s="87"/>
+      <c r="DK42" s="41"/>
+      <c r="DM42" s="41"/>
+      <c r="DO42" s="41"/>
+      <c r="DQ42" s="41"/>
+      <c r="DR42" s="26"/>
       <c r="EB42" s="2"/>
       <c r="EL42" s="2"/>
       <c r="EV42" s="22"/>
@@ -6096,14 +6033,18 @@
       <c r="FP42" s="22"/>
     </row>
     <row r="43" spans="62:172" x14ac:dyDescent="0.3">
-      <c r="BJ43" s="134"/>
+      <c r="BJ43" s="130"/>
       <c r="BT43" s="2"/>
       <c r="CD43" s="2"/>
-      <c r="CN43" s="134"/>
+      <c r="CN43" s="130"/>
       <c r="CP43" s="37"/>
       <c r="CX43" s="60"/>
       <c r="DH43" s="22"/>
-      <c r="DR43" s="2"/>
+      <c r="DJ43" s="49"/>
+      <c r="DL43" s="49"/>
+      <c r="DN43" s="49"/>
+      <c r="DP43" s="49"/>
+      <c r="DR43" s="37"/>
       <c r="EB43" s="2"/>
       <c r="EL43" s="2"/>
       <c r="EV43" s="22"/>
@@ -6111,7 +6052,7 @@
       <c r="FP43" s="22"/>
     </row>
     <row r="44" spans="62:172" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BJ44" s="134"/>
+      <c r="BJ44" s="130"/>
       <c r="BK44" s="1"/>
       <c r="BL44" s="1"/>
       <c r="BM44" s="1"/>
@@ -6141,8 +6082,8 @@
       <c r="CK44" s="1"/>
       <c r="CL44" s="1"/>
       <c r="CM44" s="1"/>
-      <c r="CN44" s="135"/>
-      <c r="CO44" s="160"/>
+      <c r="CN44" s="131"/>
+      <c r="CO44" s="156"/>
       <c r="CP44" s="22"/>
       <c r="CQ44" s="18">
         <v>4</v>
@@ -6160,23 +6101,19 @@
       <c r="CX44" s="61"/>
       <c r="CY44" s="1"/>
       <c r="CZ44" s="1"/>
-      <c r="DA44" s="147"/>
+      <c r="DA44" s="143"/>
       <c r="DB44" s="1"/>
-      <c r="DD44" s="109"/>
-      <c r="DE44" s="109"/>
-      <c r="DF44" s="109"/>
-      <c r="DG44" s="109"/>
       <c r="DH44" s="22"/>
-      <c r="DI44" s="1"/>
+      <c r="DI44" s="48"/>
       <c r="DJ44" s="1"/>
-      <c r="DK44" s="1"/>
+      <c r="DK44" s="40"/>
       <c r="DL44" s="1"/>
-      <c r="DM44" s="1"/>
+      <c r="DM44" s="40"/>
       <c r="DN44" s="1"/>
-      <c r="DO44" s="1"/>
+      <c r="DO44" s="40"/>
       <c r="DP44" s="1"/>
-      <c r="DQ44" s="1"/>
-      <c r="DR44" s="3"/>
+      <c r="DQ44" s="40"/>
+      <c r="DR44" s="27"/>
       <c r="DS44" s="1"/>
       <c r="DT44" s="1"/>
       <c r="DU44" s="1"/>
@@ -6207,34 +6144,18 @@
       <c r="ET44" s="1"/>
       <c r="EU44" s="1"/>
       <c r="EV44" s="27"/>
-      <c r="EW44" s="109"/>
-      <c r="EX44" s="109"/>
-      <c r="EY44" s="109"/>
-      <c r="EZ44" s="109"/>
-      <c r="FA44" s="109"/>
-      <c r="FB44" s="109"/>
-      <c r="FC44" s="109"/>
-      <c r="FD44" s="109"/>
-      <c r="FE44" s="109"/>
       <c r="FF44" s="22"/>
       <c r="FG44" s="23"/>
-      <c r="FH44" s="109"/>
-      <c r="FI44" s="109"/>
-      <c r="FJ44" s="109"/>
-      <c r="FK44" s="109"/>
-      <c r="FL44" s="126" t="s">
+      <c r="FL44" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="FM44" s="109"/>
-      <c r="FN44" s="109"/>
-      <c r="FO44" s="109"/>
       <c r="FP44" s="22"/>
     </row>
     <row r="45" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="BJ45" s="134"/>
+      <c r="BJ45" s="130"/>
       <c r="BT45" s="2"/>
       <c r="CD45" s="2"/>
-      <c r="CN45" s="134"/>
+      <c r="CN45" s="130"/>
       <c r="CP45" s="49"/>
       <c r="CR45" s="49"/>
       <c r="CT45" s="41"/>
@@ -6242,7 +6163,11 @@
       <c r="CX45" s="42"/>
       <c r="CZ45" s="41"/>
       <c r="DB45" s="42"/>
-      <c r="DH45" s="2"/>
+      <c r="DH45" s="99"/>
+      <c r="DI45" s="15"/>
+      <c r="DJ45" s="15"/>
+      <c r="DK45" s="15"/>
+      <c r="DL45" s="15"/>
       <c r="DR45" s="2"/>
       <c r="EB45" s="2"/>
       <c r="EL45" s="2"/>
@@ -6251,12 +6176,11 @@
       <c r="FP45" s="22"/>
     </row>
     <row r="46" spans="62:172" x14ac:dyDescent="0.3">
-      <c r="BJ46" s="134"/>
+      <c r="BJ46" s="130"/>
       <c r="BT46" s="2"/>
       <c r="CD46" s="2"/>
-      <c r="CN46" s="134"/>
-      <c r="CO46" s="160"/>
-      <c r="CP46" s="109"/>
+      <c r="CN46" s="130"/>
+      <c r="CO46" s="156"/>
       <c r="CQ46" s="49"/>
       <c r="CS46" s="49"/>
       <c r="CU46" s="49"/>
@@ -6265,8 +6189,15 @@
       <c r="CY46" s="93"/>
       <c r="DA46" s="49"/>
       <c r="DB46" s="22"/>
-      <c r="DH46" s="2"/>
+      <c r="DH46" s="99"/>
+      <c r="DI46" s="15"/>
+      <c r="DJ46" s="15"/>
+      <c r="DK46" s="15"/>
+      <c r="DL46" s="15"/>
       <c r="DR46" s="2"/>
+      <c r="DU46" s="31" t="s">
+        <v>54</v>
+      </c>
       <c r="EB46" s="2"/>
       <c r="EL46" s="2"/>
       <c r="EV46" s="60"/>
@@ -6274,18 +6205,18 @@
       <c r="FP46" s="22"/>
     </row>
     <row r="47" spans="62:172" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BJ47" s="134"/>
-      <c r="BK47" s="137"/>
-      <c r="BL47" s="132"/>
-      <c r="BM47" s="132"/>
-      <c r="BN47" s="132"/>
-      <c r="BO47" s="132"/>
-      <c r="BP47" s="132"/>
-      <c r="BQ47" s="132"/>
-      <c r="BR47" s="132"/>
-      <c r="BS47" s="132"/>
-      <c r="BT47" s="140"/>
-      <c r="BU47" s="110"/>
+      <c r="BJ47" s="130"/>
+      <c r="BK47" s="133"/>
+      <c r="BL47" s="128"/>
+      <c r="BM47" s="128"/>
+      <c r="BN47" s="128"/>
+      <c r="BO47" s="128"/>
+      <c r="BP47" s="128"/>
+      <c r="BQ47" s="128"/>
+      <c r="BR47" s="128"/>
+      <c r="BS47" s="128"/>
+      <c r="BT47" s="136"/>
+      <c r="BU47" s="109"/>
       <c r="BV47" s="1"/>
       <c r="BW47" s="1"/>
       <c r="BX47" s="1"/>
@@ -6304,7 +6235,7 @@
       <c r="CK47" s="1"/>
       <c r="CL47" s="1"/>
       <c r="CM47" s="1"/>
-      <c r="CN47" s="135"/>
+      <c r="CN47" s="131"/>
       <c r="CO47" s="1"/>
       <c r="CP47" s="40"/>
       <c r="CQ47" s="1"/>
@@ -6324,13 +6255,15 @@
       <c r="DE47" s="1"/>
       <c r="DF47" s="1"/>
       <c r="DG47" s="1"/>
-      <c r="DH47" s="3"/>
-      <c r="DI47" s="1"/>
-      <c r="DJ47" s="1"/>
-      <c r="DK47" s="1"/>
-      <c r="DL47" s="1"/>
+      <c r="DH47" s="92"/>
+      <c r="DI47" s="90"/>
+      <c r="DJ47" s="90"/>
+      <c r="DK47" s="90"/>
+      <c r="DL47" s="90"/>
       <c r="DM47" s="1"/>
-      <c r="DN47" s="1"/>
+      <c r="DN47" s="164" t="s">
+        <v>45</v>
+      </c>
       <c r="DO47" s="1"/>
       <c r="DP47" s="1"/>
       <c r="DQ47" s="1"/>
@@ -6367,11 +6300,11 @@
       <c r="EV47" s="61"/>
       <c r="EW47" s="1"/>
       <c r="EX47" s="1"/>
-      <c r="EY47" s="163"/>
-      <c r="EZ47" s="163"/>
-      <c r="FA47" s="163"/>
-      <c r="FB47" s="163"/>
-      <c r="FC47" s="163"/>
+      <c r="EY47" s="159"/>
+      <c r="EZ47" s="159"/>
+      <c r="FA47" s="159"/>
+      <c r="FB47" s="159"/>
+      <c r="FC47" s="159"/>
       <c r="FD47" s="1"/>
       <c r="FE47" s="1"/>
       <c r="FF47" s="3"/>
@@ -6387,9 +6320,9 @@
       <c r="FP47" s="27"/>
     </row>
     <row r="48" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="BT48" s="133"/>
+      <c r="BT48" s="129"/>
       <c r="CD48" s="2"/>
-      <c r="CN48" s="134"/>
+      <c r="CN48" s="130"/>
       <c r="CX48" s="26"/>
       <c r="DH48" s="2"/>
       <c r="DR48" s="2"/>
@@ -6397,14 +6330,13 @@
       <c r="EL48" s="2"/>
       <c r="EV48" s="2"/>
       <c r="EX48" s="26"/>
-      <c r="FA48" s="109"/>
       <c r="FC48" s="22"/>
       <c r="FF48" s="22"/>
     </row>
     <row r="49" spans="72:162" x14ac:dyDescent="0.3">
-      <c r="BT49" s="134"/>
+      <c r="BT49" s="130"/>
       <c r="CD49" s="2"/>
-      <c r="CN49" s="134"/>
+      <c r="CN49" s="130"/>
       <c r="CX49" s="22"/>
       <c r="DH49" s="2"/>
       <c r="DR49" s="2"/>
@@ -6412,12 +6344,11 @@
       <c r="EL49" s="2"/>
       <c r="EV49" s="2"/>
       <c r="EX49" s="22"/>
-      <c r="FA49" s="109"/>
       <c r="FC49" s="22"/>
       <c r="FF49" s="22"/>
     </row>
     <row r="50" spans="72:162" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BT50" s="134"/>
+      <c r="BT50" s="130"/>
       <c r="BU50" s="1"/>
       <c r="BV50" s="1"/>
       <c r="BW50" s="1"/>
@@ -6437,7 +6368,7 @@
       <c r="CK50" s="1"/>
       <c r="CL50" s="1"/>
       <c r="CM50" s="1"/>
-      <c r="CN50" s="135"/>
+      <c r="CN50" s="131"/>
       <c r="CX50" s="22"/>
       <c r="CY50" s="1"/>
       <c r="CZ50" s="1"/>
@@ -6491,19 +6422,15 @@
       <c r="EV50" s="3"/>
       <c r="EW50" s="1"/>
       <c r="EX50" s="27"/>
-      <c r="EY50" s="109"/>
-      <c r="EZ50" s="109"/>
-      <c r="FA50" s="109"/>
-      <c r="FB50" s="109"/>
       <c r="FC50" s="22"/>
       <c r="FD50" s="1"/>
       <c r="FE50" s="1"/>
       <c r="FF50" s="27"/>
     </row>
     <row r="51" spans="72:162" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="BT51" s="134"/>
+      <c r="BT51" s="130"/>
       <c r="CD51" s="2"/>
-      <c r="CN51" s="134"/>
+      <c r="CN51" s="130"/>
       <c r="CX51" s="22"/>
       <c r="DH51" s="2"/>
       <c r="DR51" s="2"/>
@@ -6512,12 +6439,12 @@
       <c r="EV51" s="2"/>
       <c r="FD51" s="15"/>
       <c r="FE51" s="15"/>
-      <c r="FF51" s="112"/>
+      <c r="FF51" s="111"/>
     </row>
     <row r="52" spans="72:162" x14ac:dyDescent="0.3">
-      <c r="BT52" s="134"/>
+      <c r="BT52" s="130"/>
       <c r="CD52" s="2"/>
-      <c r="CN52" s="134"/>
+      <c r="CN52" s="130"/>
       <c r="CU52" t="s">
         <v>53</v>
       </c>
@@ -6529,10 +6456,10 @@
       <c r="EV52" s="2"/>
       <c r="FD52" s="15"/>
       <c r="FE52" s="15"/>
-      <c r="FF52" s="112"/>
+      <c r="FF52" s="111"/>
     </row>
     <row r="53" spans="72:162" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BT53" s="134"/>
+      <c r="BT53" s="130"/>
       <c r="BU53" s="1"/>
       <c r="BV53" s="1"/>
       <c r="BW53" s="1"/>
@@ -6552,7 +6479,7 @@
       <c r="CK53" s="1"/>
       <c r="CL53" s="1"/>
       <c r="CM53" s="1"/>
-      <c r="CN53" s="135"/>
+      <c r="CN53" s="131"/>
       <c r="CW53" s="95" t="s">
         <v>51</v>
       </c>
@@ -6615,13 +6542,13 @@
       <c r="FB53" s="1"/>
       <c r="FC53" s="1"/>
       <c r="FD53" s="90"/>
-      <c r="FE53" s="164"/>
-      <c r="FF53" s="113"/>
+      <c r="FE53" s="160"/>
+      <c r="FF53" s="112"/>
     </row>
     <row r="54" spans="72:162" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="BT54" s="134"/>
+      <c r="BT54" s="130"/>
       <c r="CD54" s="26"/>
-      <c r="CN54" s="134"/>
+      <c r="CN54" s="130"/>
       <c r="CU54" t="s">
         <v>52</v>
       </c>
@@ -6634,9 +6561,9 @@
       <c r="FF54" s="22"/>
     </row>
     <row r="55" spans="72:162" x14ac:dyDescent="0.3">
-      <c r="BT55" s="134"/>
+      <c r="BT55" s="130"/>
       <c r="CD55" s="22"/>
-      <c r="CN55" s="134"/>
+      <c r="CN55" s="130"/>
       <c r="CX55" s="22"/>
       <c r="DH55" s="2"/>
       <c r="DR55" s="2"/>
@@ -6646,29 +6573,29 @@
       <c r="FF55" s="22"/>
     </row>
     <row r="56" spans="72:162" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BT56" s="134"/>
-      <c r="BU56" s="137"/>
-      <c r="BV56" s="132"/>
-      <c r="BW56" s="132"/>
-      <c r="BX56" s="132"/>
-      <c r="BY56" s="132"/>
-      <c r="BZ56" s="132"/>
-      <c r="CA56" s="132"/>
-      <c r="CB56" s="132"/>
-      <c r="CC56" s="132"/>
-      <c r="CD56" s="145"/>
-      <c r="CE56" s="132"/>
-      <c r="CF56" s="132"/>
-      <c r="CG56" s="132"/>
-      <c r="CH56" s="132"/>
-      <c r="CI56" s="132"/>
-      <c r="CJ56" s="149" t="s">
+      <c r="BT56" s="130"/>
+      <c r="BU56" s="133"/>
+      <c r="BV56" s="128"/>
+      <c r="BW56" s="128"/>
+      <c r="BX56" s="128"/>
+      <c r="BY56" s="128"/>
+      <c r="BZ56" s="128"/>
+      <c r="CA56" s="128"/>
+      <c r="CB56" s="128"/>
+      <c r="CC56" s="128"/>
+      <c r="CD56" s="141"/>
+      <c r="CE56" s="128"/>
+      <c r="CF56" s="128"/>
+      <c r="CG56" s="128"/>
+      <c r="CH56" s="128"/>
+      <c r="CI56" s="128"/>
+      <c r="CJ56" s="145" t="s">
         <v>21</v>
       </c>
-      <c r="CK56" s="132"/>
-      <c r="CL56" s="132"/>
-      <c r="CM56" s="132"/>
-      <c r="CN56" s="144"/>
+      <c r="CK56" s="128"/>
+      <c r="CL56" s="128"/>
+      <c r="CM56" s="128"/>
+      <c r="CN56" s="140"/>
       <c r="CX56" s="22"/>
       <c r="CY56" s="1"/>
       <c r="CZ56" s="1"/>

</xml_diff>

<commit_message>
Made the Intro Storyboard
Also advanced the demo level draft a little bit, only Mr. Phant chase really needs fleshing out.
</commit_message>
<xml_diff>
--- a/Game Design Documentation/Demo Level Map Draft.xlsx
+++ b/Game Design Documentation/Demo Level Map Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://osekk-my.sharepoint.com/personal/s4voto00_students_osao_fi/Documents/Tiedostot/Github/CartoonViolence/Game Design Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1558" documentId="11_F25DC773A252ABDACC1048BB699D52725ADE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6BF2B87-F668-448D-AEA7-599F7BB7EBA3}"/>
+  <xr:revisionPtr revIDLastSave="1679" documentId="11_F25DC773A252ABDACC1048BB699D52725ADE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CC8772E-8C35-4488-9E87-F1D8BB713186}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="9960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,10 +17,21 @@
     <sheet name="TutorialArea" sheetId="2" r:id="rId2"/>
     <sheet name="Offices" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1098,7 +1109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DX37" authorId="0" shapeId="0" xr:uid="{FDD08983-F57B-40F5-B2DD-EBD86D7E79D8}">
+    <comment ref="EG37" authorId="0" shapeId="0" xr:uid="{FDD08983-F57B-40F5-B2DD-EBD86D7E79D8}">
       <text>
         <r>
           <rPr>
@@ -1173,6 +1184,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="DY40" authorId="0" shapeId="0" xr:uid="{42F8EA30-3ACE-4374-9969-8C657620852A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Lipsmack
+If he eats a bomb, the ceiling also breaks, revealing a secret.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="CR44" authorId="0" shapeId="0" xr:uid="{8E969225-FBD9-479A-924B-5F0C6A278995}">
       <text>
         <r>
@@ -1245,6 +1281,30 @@
 Ducker
 Unloaded, Stationary.
 You can run past him and into the other screen before he shoots, prompting him to chase after you.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EI47" authorId="0" shapeId="0" xr:uid="{381856F0-BDFE-4CE7-BBFD-C1C9F052F6FB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Touko Erkki Tapani Vornanen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Opens and closes the shutter.</t>
         </r>
       </text>
     </comment>
@@ -1327,7 +1387,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>Screen Template</t>
   </si>
@@ -1516,6 +1576,27 @@
   <si>
     <t>←IN CASE OF LOCKS, SMACK THIS</t>
   </si>
+  <si>
+    <t>One Screen in Unity Camera Terms:</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>(Y has have .5 added to it)</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Ω</t>
+  </si>
+  <si>
+    <t>Locked Door</t>
+  </si>
 </sst>
 </file>
 
@@ -1649,7 +1730,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="114">
+  <borders count="116">
     <border>
       <left/>
       <right/>
@@ -2996,11 +3077,35 @@
         <color rgb="FF7030A0"/>
       </diagonal>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -3232,6 +3337,12 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="114" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="115" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -3516,10 +3627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3527,7 +3638,7 @@
     <col min="1" max="269" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3542,7 +3653,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="K2" s="2"/>
       <c r="M2" s="6"/>
@@ -3550,11 +3661,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3570,20 +3684,41 @@
       <c r="N4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S4" t="s">
+        <v>58</v>
+      </c>
+      <c r="T4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S5" t="s">
+        <v>59</v>
+      </c>
+      <c r="T5">
+        <v>15</v>
+      </c>
+      <c r="V5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="K6" s="2"/>
       <c r="M6" s="7"/>
       <c r="N6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S6" t="s">
+        <v>61</v>
+      </c>
+      <c r="T6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3596,19 +3731,25 @@
       <c r="J7" s="1"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="K8" s="2"/>
       <c r="M8" s="8"/>
       <c r="N8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q8" s="95" t="s">
+        <v>62</v>
+      </c>
+      <c r="R8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -3625,8 +3766,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="24"/>
       <c r="C12" t="s">
         <v>7</v>
@@ -3646,8 +3787,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12"/>
       <c r="C14" t="s">
         <v>19</v>
@@ -3665,8 +3806,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="16"/>
       <c r="C16" t="s">
         <v>13</v>
@@ -3733,8 +3874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2B2FEB-625D-42F7-933A-9E09CE4A3EF3}">
   <dimension ref="C17:BL45"/>
   <sheetViews>
-    <sheetView topLeftCell="H22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z30" sqref="Z30"/>
+    <sheetView topLeftCell="H27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W41" sqref="W41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4357,8 +4498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A88EDC-4468-4B92-BB23-9A52F08C9D3C}">
   <dimension ref="A1:FP57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CW35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DW41" sqref="DW41"/>
+    <sheetView tabSelected="1" topLeftCell="DQ36" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="EF42" sqref="EF42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4367,7 +4508,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:152" x14ac:dyDescent="0.3">
-      <c r="DT1" s="163"/>
+      <c r="ED1" s="163"/>
       <c r="EV1" s="130"/>
     </row>
     <row r="2" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4391,18 +4532,8 @@
       <c r="T2" s="128"/>
       <c r="U2" s="128"/>
       <c r="V2" s="128"/>
-      <c r="DS2" s="162"/>
-      <c r="DT2" s="161"/>
-      <c r="DU2" s="128"/>
-      <c r="DV2" s="128"/>
-      <c r="DW2" s="128"/>
-      <c r="DX2" s="128"/>
-      <c r="DY2" s="128"/>
-      <c r="DZ2" s="128"/>
-      <c r="EA2" s="128"/>
-      <c r="EB2" s="128"/>
-      <c r="EC2" s="128"/>
-      <c r="ED2" s="128"/>
+      <c r="EC2" s="162"/>
+      <c r="ED2" s="161"/>
       <c r="EE2" s="128"/>
       <c r="EF2" s="128"/>
       <c r="EG2" s="128"/>
@@ -4428,16 +4559,18 @@
       <c r="B3" s="130"/>
       <c r="L3" s="2"/>
       <c r="V3" s="129"/>
-      <c r="DR3" s="130"/>
-      <c r="EB3" s="2"/>
+      <c r="DR3" s="168"/>
+      <c r="EB3" s="130"/>
+      <c r="EL3" s="129"/>
       <c r="EV3" s="22"/>
     </row>
     <row r="4" spans="1:152" x14ac:dyDescent="0.3">
       <c r="B4" s="130"/>
       <c r="L4" s="2"/>
       <c r="V4" s="130"/>
-      <c r="DR4" s="130"/>
-      <c r="EB4" s="2"/>
+      <c r="DR4" s="168"/>
+      <c r="EB4" s="130"/>
+      <c r="EL4" s="130"/>
       <c r="EV4" s="22"/>
     </row>
     <row r="5" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4464,33 +4597,36 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="131"/>
-      <c r="DR5" s="130"/>
-      <c r="DS5" s="1"/>
-      <c r="DT5" s="1"/>
-      <c r="DU5" s="1"/>
-      <c r="DV5" s="1"/>
-      <c r="DW5" s="1"/>
-      <c r="DX5" s="1"/>
-      <c r="DY5" s="1"/>
-      <c r="DZ5" s="1"/>
-      <c r="EA5" s="1"/>
-      <c r="EB5" s="3"/>
+      <c r="DR5" s="168"/>
+      <c r="EB5" s="130"/>
+      <c r="EC5" s="1"/>
+      <c r="ED5" s="1"/>
+      <c r="EE5" s="1"/>
+      <c r="EF5" s="1"/>
+      <c r="EG5" s="1"/>
+      <c r="EH5" s="1"/>
+      <c r="EI5" s="1"/>
+      <c r="EJ5" s="1"/>
+      <c r="EK5" s="1"/>
+      <c r="EL5" s="131"/>
       <c r="EV5" s="22"/>
     </row>
     <row r="6" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="130"/>
       <c r="L6" s="2"/>
       <c r="V6" s="130"/>
-      <c r="DR6" s="130"/>
-      <c r="EB6" s="2"/>
+      <c r="DR6" s="168"/>
+      <c r="EB6" s="130"/>
+      <c r="EL6" s="132"/>
       <c r="EV6" s="22"/>
     </row>
     <row r="7" spans="1:152" x14ac:dyDescent="0.3">
       <c r="B7" s="130"/>
       <c r="L7" s="2"/>
       <c r="V7" s="130"/>
-      <c r="DR7" s="130"/>
-      <c r="EB7" s="2"/>
+      <c r="DR7" s="168"/>
+      <c r="EB7" s="130"/>
+      <c r="EL7" s="130"/>
       <c r="EV7" s="22"/>
     </row>
     <row r="8" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4515,33 +4651,36 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="131"/>
-      <c r="DR8" s="130"/>
-      <c r="DS8" s="1"/>
-      <c r="DT8" s="1"/>
-      <c r="DU8" s="1"/>
-      <c r="DV8" s="1"/>
-      <c r="DW8" s="1"/>
-      <c r="DX8" s="1"/>
-      <c r="DY8" s="1"/>
-      <c r="DZ8" s="1"/>
-      <c r="EA8" s="1"/>
-      <c r="EB8" s="3"/>
+      <c r="DR8" s="168"/>
+      <c r="EB8" s="130"/>
+      <c r="EC8" s="1"/>
+      <c r="ED8" s="1"/>
+      <c r="EE8" s="1"/>
+      <c r="EF8" s="1"/>
+      <c r="EG8" s="1"/>
+      <c r="EH8" s="1"/>
+      <c r="EI8" s="1"/>
+      <c r="EJ8" s="1"/>
+      <c r="EK8" s="1"/>
+      <c r="EL8" s="131"/>
       <c r="EV8" s="22"/>
     </row>
     <row r="9" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B9" s="130"/>
       <c r="L9" s="2"/>
       <c r="V9" s="130"/>
-      <c r="DR9" s="130"/>
-      <c r="EB9" s="2"/>
+      <c r="DR9" s="168"/>
+      <c r="EB9" s="130"/>
+      <c r="EL9" s="130"/>
       <c r="EV9" s="22"/>
     </row>
     <row r="10" spans="1:152" x14ac:dyDescent="0.3">
       <c r="B10" s="130"/>
       <c r="L10" s="2"/>
       <c r="V10" s="130"/>
-      <c r="DR10" s="130"/>
-      <c r="EB10" s="2"/>
+      <c r="DR10" s="168"/>
+      <c r="EB10" s="130"/>
+      <c r="EL10" s="130"/>
       <c r="EV10" s="22"/>
     </row>
     <row r="11" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4606,17 +4745,18 @@
       <c r="BH11" s="1"/>
       <c r="BI11" s="1"/>
       <c r="BJ11" s="1"/>
-      <c r="DR11" s="130"/>
-      <c r="DS11" s="1"/>
-      <c r="DT11" s="1"/>
-      <c r="DU11" s="1"/>
-      <c r="DV11" s="1"/>
-      <c r="DW11" s="1"/>
-      <c r="DX11" s="1"/>
-      <c r="DY11" s="1"/>
-      <c r="DZ11" s="1"/>
-      <c r="EA11" s="1"/>
-      <c r="EB11" s="3"/>
+      <c r="DR11" s="168"/>
+      <c r="EB11" s="130"/>
+      <c r="EC11" s="1"/>
+      <c r="ED11" s="1"/>
+      <c r="EE11" s="1"/>
+      <c r="EF11" s="1"/>
+      <c r="EG11" s="1"/>
+      <c r="EH11" s="1"/>
+      <c r="EI11" s="1"/>
+      <c r="EJ11" s="1"/>
+      <c r="EK11" s="1"/>
+      <c r="EL11" s="131"/>
       <c r="EV11" s="22"/>
     </row>
     <row r="12" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -4631,8 +4771,9 @@
       <c r="AP12" s="26"/>
       <c r="AZ12" s="113"/>
       <c r="BJ12" s="26"/>
-      <c r="DR12" s="130"/>
-      <c r="EB12" s="2"/>
+      <c r="DR12" s="168"/>
+      <c r="EB12" s="130"/>
+      <c r="EL12" s="130"/>
       <c r="EV12" s="22"/>
     </row>
     <row r="13" spans="1:152" x14ac:dyDescent="0.3">
@@ -4650,8 +4791,9 @@
       </c>
       <c r="AZ13" s="2"/>
       <c r="BJ13" s="22"/>
-      <c r="DR13" s="130"/>
-      <c r="EB13" s="2"/>
+      <c r="DR13" s="168"/>
+      <c r="EB13" s="130"/>
+      <c r="EL13" s="130"/>
       <c r="EV13" s="22"/>
     </row>
     <row r="14" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4705,17 +4847,18 @@
       <c r="BH14" s="1"/>
       <c r="BI14" s="1"/>
       <c r="BJ14" s="22"/>
-      <c r="DR14" s="130"/>
-      <c r="DS14" s="1"/>
-      <c r="DT14" s="1"/>
-      <c r="DU14" s="1"/>
-      <c r="DV14" s="1"/>
-      <c r="DW14" s="1"/>
-      <c r="DX14" s="1"/>
-      <c r="DY14" s="1"/>
-      <c r="DZ14" s="1"/>
-      <c r="EA14" s="1"/>
-      <c r="EB14" s="3"/>
+      <c r="DR14" s="168"/>
+      <c r="EB14" s="130"/>
+      <c r="EC14" s="1"/>
+      <c r="ED14" s="1"/>
+      <c r="EE14" s="1"/>
+      <c r="EF14" s="1"/>
+      <c r="EG14" s="1"/>
+      <c r="EH14" s="1"/>
+      <c r="EI14" s="1"/>
+      <c r="EJ14" s="1"/>
+      <c r="EK14" s="1"/>
+      <c r="EL14" s="131"/>
       <c r="EV14" s="22"/>
     </row>
     <row r="15" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -4734,8 +4877,9 @@
       <c r="AZ15" s="2"/>
       <c r="BD15" s="26"/>
       <c r="BJ15" s="22"/>
-      <c r="DR15" s="130"/>
-      <c r="EB15" s="2"/>
+      <c r="DR15" s="168"/>
+      <c r="EB15" s="130"/>
+      <c r="EL15" s="130"/>
       <c r="EV15" s="22"/>
     </row>
     <row r="16" spans="1:152" x14ac:dyDescent="0.3">
@@ -4756,8 +4900,9 @@
       <c r="AZ16" s="2"/>
       <c r="BD16" s="22"/>
       <c r="BJ16" s="22"/>
-      <c r="DR16" s="130"/>
-      <c r="EB16" s="2"/>
+      <c r="DR16" s="168"/>
+      <c r="EB16" s="130"/>
+      <c r="EL16" s="130"/>
       <c r="EV16" s="22"/>
     </row>
     <row r="17" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4809,17 +4954,18 @@
       <c r="BE17" s="23"/>
       <c r="BI17" s="1"/>
       <c r="BJ17" s="27"/>
-      <c r="DR17" s="130"/>
-      <c r="DS17" s="1"/>
-      <c r="DT17" s="1"/>
-      <c r="DU17" s="1"/>
-      <c r="DV17" s="1"/>
-      <c r="DW17" s="1"/>
-      <c r="DX17" s="1"/>
-      <c r="DY17" s="1"/>
-      <c r="DZ17" s="1"/>
-      <c r="EA17" s="1"/>
-      <c r="EB17" s="3"/>
+      <c r="DR17" s="168"/>
+      <c r="EB17" s="130"/>
+      <c r="EC17" s="1"/>
+      <c r="ED17" s="1"/>
+      <c r="EE17" s="1"/>
+      <c r="EF17" s="1"/>
+      <c r="EG17" s="1"/>
+      <c r="EH17" s="1"/>
+      <c r="EI17" s="1"/>
+      <c r="EJ17" s="1"/>
+      <c r="EK17" s="1"/>
+      <c r="EL17" s="131"/>
       <c r="EV17" s="22"/>
     </row>
     <row r="18" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -4836,8 +4982,9 @@
       <c r="BH18" s="22"/>
       <c r="BI18" s="87"/>
       <c r="BJ18" s="26"/>
-      <c r="DR18" s="130"/>
-      <c r="EB18" s="2"/>
+      <c r="DR18" s="168"/>
+      <c r="EB18" s="130"/>
+      <c r="EL18" s="130"/>
       <c r="EV18" s="22"/>
     </row>
     <row r="19" spans="1:152" x14ac:dyDescent="0.3">
@@ -4855,8 +5002,9 @@
       <c r="BD19" s="37"/>
       <c r="BH19" s="22"/>
       <c r="BJ19" s="37"/>
-      <c r="DR19" s="130"/>
-      <c r="EB19" s="2"/>
+      <c r="DR19" s="168"/>
+      <c r="EB19" s="130"/>
+      <c r="EL19" s="130"/>
       <c r="EV19" s="22"/>
     </row>
     <row r="20" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4961,17 +5109,18 @@
       <c r="CV20" s="1"/>
       <c r="CW20" s="1"/>
       <c r="CX20" s="1"/>
-      <c r="DR20" s="130"/>
-      <c r="DS20" s="1"/>
-      <c r="DT20" s="1"/>
-      <c r="DU20" s="1"/>
-      <c r="DV20" s="1"/>
-      <c r="DW20" s="1"/>
-      <c r="DX20" s="1"/>
-      <c r="DY20" s="1"/>
-      <c r="DZ20" s="1"/>
-      <c r="EA20" s="1"/>
-      <c r="EB20" s="3"/>
+      <c r="DR20" s="168"/>
+      <c r="EB20" s="130"/>
+      <c r="EC20" s="1"/>
+      <c r="ED20" s="1"/>
+      <c r="EE20" s="1"/>
+      <c r="EF20" s="1"/>
+      <c r="EG20" s="1"/>
+      <c r="EH20" s="1"/>
+      <c r="EI20" s="1"/>
+      <c r="EJ20" s="1"/>
+      <c r="EK20" s="1"/>
+      <c r="EL20" s="131"/>
       <c r="EV20" s="22"/>
     </row>
     <row r="21" spans="1:152" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5014,8 +5163,9 @@
       <c r="CF21" s="26"/>
       <c r="CN21" s="2"/>
       <c r="CX21" s="22"/>
-      <c r="DR21" s="130"/>
-      <c r="EB21" s="2"/>
+      <c r="DR21" s="168"/>
+      <c r="EB21" s="130"/>
+      <c r="EL21" s="132"/>
       <c r="EV21" s="22"/>
     </row>
     <row r="22" spans="1:152" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5062,8 +5212,9 @@
       <c r="CF22" s="37"/>
       <c r="CN22" s="2"/>
       <c r="CX22" s="22"/>
-      <c r="DR22" s="130"/>
-      <c r="EB22" s="2"/>
+      <c r="DR22" s="168"/>
+      <c r="EB22" s="130"/>
+      <c r="EL22" s="130"/>
       <c r="EV22" s="22"/>
     </row>
     <row r="23" spans="1:152" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5130,17 +5281,18 @@
         <v>2</v>
       </c>
       <c r="CX23" s="22"/>
-      <c r="DR23" s="130"/>
-      <c r="DS23" s="1"/>
-      <c r="DT23" s="1"/>
-      <c r="DU23" s="1"/>
-      <c r="DV23" s="1"/>
-      <c r="DW23" s="1"/>
-      <c r="DX23" s="1"/>
-      <c r="DY23" s="1"/>
-      <c r="DZ23" s="1"/>
-      <c r="EA23" s="1"/>
-      <c r="EB23" s="3"/>
+      <c r="DR23" s="168"/>
+      <c r="EB23" s="130"/>
+      <c r="EC23" s="1"/>
+      <c r="ED23" s="1"/>
+      <c r="EE23" s="1"/>
+      <c r="EF23" s="1"/>
+      <c r="EG23" s="1"/>
+      <c r="EH23" s="1"/>
+      <c r="EI23" s="1"/>
+      <c r="EJ23" s="1"/>
+      <c r="EK23" s="1"/>
+      <c r="EL23" s="131"/>
       <c r="EV23" s="22"/>
     </row>
     <row r="24" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -5178,8 +5330,9 @@
       <c r="CO24" s="87"/>
       <c r="CQ24" s="42"/>
       <c r="CX24" s="22"/>
-      <c r="DR24" s="130"/>
-      <c r="EB24" s="2"/>
+      <c r="DR24" s="168"/>
+      <c r="EB24" s="130"/>
+      <c r="EL24" s="130"/>
       <c r="EV24" s="22"/>
     </row>
     <row r="25" spans="1:152" x14ac:dyDescent="0.3">
@@ -5213,8 +5366,9 @@
       <c r="CP25" s="49"/>
       <c r="CQ25" s="22"/>
       <c r="CX25" s="22"/>
-      <c r="DR25" s="130"/>
-      <c r="EB25" s="2"/>
+      <c r="DR25" s="168"/>
+      <c r="EB25" s="130"/>
+      <c r="EL25" s="130"/>
       <c r="EV25" s="22"/>
     </row>
     <row r="26" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5316,17 +5470,18 @@
       <c r="CX26" s="151" t="s">
         <v>47</v>
       </c>
-      <c r="DR26" s="130"/>
-      <c r="DS26" s="1"/>
-      <c r="DT26" s="1"/>
-      <c r="DU26" s="1"/>
-      <c r="DV26" s="1"/>
-      <c r="DW26" s="1"/>
-      <c r="DX26" s="1"/>
-      <c r="DY26" s="1"/>
-      <c r="DZ26" s="1"/>
-      <c r="EA26" s="1"/>
-      <c r="EB26" s="3"/>
+      <c r="DR26" s="168"/>
+      <c r="EB26" s="130"/>
+      <c r="EC26" s="1"/>
+      <c r="ED26" s="1"/>
+      <c r="EE26" s="1"/>
+      <c r="EF26" s="1"/>
+      <c r="EG26" s="1"/>
+      <c r="EH26" s="1"/>
+      <c r="EI26" s="1"/>
+      <c r="EJ26" s="1"/>
+      <c r="EK26" s="1"/>
+      <c r="EL26" s="131"/>
       <c r="EV26" s="22"/>
     </row>
     <row r="27" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -5385,8 +5540,9 @@
         <v>2</v>
       </c>
       <c r="CX27" s="22"/>
-      <c r="DR27" s="130"/>
-      <c r="EB27" s="2"/>
+      <c r="DR27" s="168"/>
+      <c r="EB27" s="130"/>
+      <c r="EL27" s="130"/>
       <c r="EV27" s="22"/>
     </row>
     <row r="28" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5443,8 +5599,9 @@
       <c r="CQ28" s="40"/>
       <c r="CR28" s="27"/>
       <c r="CX28" s="22"/>
-      <c r="DR28" s="130"/>
-      <c r="EB28" s="2"/>
+      <c r="DR28" s="168"/>
+      <c r="EB28" s="130"/>
+      <c r="EL28" s="130"/>
       <c r="EV28" s="22"/>
     </row>
     <row r="29" spans="1:152" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5551,7 +5708,7 @@
       <c r="CV29" s="1"/>
       <c r="CW29" s="54"/>
       <c r="CX29" s="89"/>
-      <c r="DR29" s="130"/>
+      <c r="DR29" s="168"/>
       <c r="DS29" s="1"/>
       <c r="DT29" s="1"/>
       <c r="DU29" s="1"/>
@@ -5561,7 +5718,26 @@
       <c r="DY29" s="1"/>
       <c r="DZ29" s="1"/>
       <c r="EA29" s="1"/>
-      <c r="EB29" s="3"/>
+      <c r="EB29" s="131"/>
+      <c r="EC29" s="1"/>
+      <c r="ED29" s="1"/>
+      <c r="EE29" s="1"/>
+      <c r="EF29" s="1"/>
+      <c r="EG29" s="1"/>
+      <c r="EH29" s="1"/>
+      <c r="EI29" s="1"/>
+      <c r="EJ29" s="1"/>
+      <c r="EK29" s="1"/>
+      <c r="EL29" s="131"/>
+      <c r="EM29" s="170"/>
+      <c r="EN29" s="168"/>
+      <c r="EO29" s="168"/>
+      <c r="EP29" s="168"/>
+      <c r="EQ29" s="168"/>
+      <c r="ER29" s="168"/>
+      <c r="ES29" s="168"/>
+      <c r="ET29" s="168"/>
+      <c r="EU29" s="168"/>
       <c r="EV29" s="22"/>
     </row>
     <row r="30" spans="1:152" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -5584,8 +5760,9 @@
       <c r="CU30" s="41"/>
       <c r="CV30" s="26"/>
       <c r="CX30" s="153"/>
-      <c r="DR30" s="130"/>
-      <c r="EB30" s="2"/>
+      <c r="DR30" s="22"/>
+      <c r="EB30" s="130"/>
+      <c r="EL30" s="129"/>
       <c r="EV30" s="22"/>
     </row>
     <row r="31" spans="1:152" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5606,8 +5783,9 @@
       <c r="CT31" s="49"/>
       <c r="CV31" s="37"/>
       <c r="CX31" s="22"/>
-      <c r="DR31" s="130"/>
-      <c r="EB31" s="2"/>
+      <c r="DR31" s="22"/>
+      <c r="EB31" s="130"/>
+      <c r="EL31" s="130"/>
       <c r="EV31" s="22"/>
     </row>
     <row r="32" spans="1:152" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5646,7 +5824,7 @@
       <c r="CV32" s="27"/>
       <c r="CW32" s="1"/>
       <c r="CX32" s="27"/>
-      <c r="DR32" s="130"/>
+      <c r="DR32" s="22"/>
       <c r="DS32" s="1"/>
       <c r="DT32" s="1"/>
       <c r="DU32" s="1"/>
@@ -5656,7 +5834,26 @@
       <c r="DY32" s="1"/>
       <c r="DZ32" s="1"/>
       <c r="EA32" s="1"/>
-      <c r="EB32" s="3"/>
+      <c r="EB32" s="131"/>
+      <c r="EC32" s="1"/>
+      <c r="ED32" s="1"/>
+      <c r="EE32" s="1"/>
+      <c r="EF32" s="1"/>
+      <c r="EG32" s="1"/>
+      <c r="EH32" s="1"/>
+      <c r="EI32" s="1"/>
+      <c r="EJ32" s="1"/>
+      <c r="EK32" s="1"/>
+      <c r="EL32" s="131"/>
+      <c r="EM32" s="170"/>
+      <c r="EN32" s="168"/>
+      <c r="EO32" s="168"/>
+      <c r="EP32" s="168"/>
+      <c r="EQ32" s="168"/>
+      <c r="ER32" s="168"/>
+      <c r="ES32" s="168"/>
+      <c r="ET32" s="168"/>
+      <c r="EU32" s="168"/>
       <c r="EV32" s="22"/>
     </row>
     <row r="33" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -5670,8 +5867,9 @@
       <c r="CL33" s="64"/>
       <c r="CN33" s="113"/>
       <c r="CX33" s="22"/>
-      <c r="DR33" s="130"/>
-      <c r="EB33" s="2"/>
+      <c r="DR33" s="22"/>
+      <c r="EB33" s="130"/>
+      <c r="EL33" s="132"/>
       <c r="EV33" s="22"/>
     </row>
     <row r="34" spans="62:172" x14ac:dyDescent="0.3">
@@ -5689,8 +5887,9 @@
       </c>
       <c r="CN34" s="2"/>
       <c r="CX34" s="22"/>
-      <c r="DR34" s="130"/>
-      <c r="EB34" s="2"/>
+      <c r="DR34" s="22"/>
+      <c r="EB34" s="60"/>
+      <c r="EL34" s="130"/>
       <c r="EV34" s="22"/>
     </row>
     <row r="35" spans="62:172" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5722,7 +5921,7 @@
       <c r="CT35" s="1"/>
       <c r="CU35" s="1"/>
       <c r="CX35" s="27"/>
-      <c r="DR35" s="130"/>
+      <c r="DR35" s="22"/>
       <c r="DS35" s="1"/>
       <c r="DT35" s="1"/>
       <c r="DU35" s="1"/>
@@ -5732,7 +5931,26 @@
       <c r="DY35" s="1"/>
       <c r="DZ35" s="1"/>
       <c r="EA35" s="1"/>
-      <c r="EB35" s="3"/>
+      <c r="EB35" s="61"/>
+      <c r="EC35" s="1"/>
+      <c r="ED35" s="1"/>
+      <c r="EE35" s="1"/>
+      <c r="EF35" s="1"/>
+      <c r="EG35" s="1"/>
+      <c r="EH35" s="1"/>
+      <c r="EI35" s="1"/>
+      <c r="EJ35" s="1"/>
+      <c r="EK35" s="1"/>
+      <c r="EL35" s="131"/>
+      <c r="EM35" s="170"/>
+      <c r="EN35" s="168"/>
+      <c r="EO35" s="168"/>
+      <c r="EP35" s="168"/>
+      <c r="EQ35" s="168"/>
+      <c r="ER35" s="168"/>
+      <c r="ES35" s="168"/>
+      <c r="ET35" s="168"/>
+      <c r="EU35" s="168"/>
       <c r="EV35" s="22"/>
     </row>
     <row r="36" spans="62:172" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -5748,8 +5966,9 @@
       <c r="CU36" s="26"/>
       <c r="CW36" s="22"/>
       <c r="CX36" s="45"/>
-      <c r="DR36" s="130"/>
-      <c r="EB36" s="2"/>
+      <c r="DR36" s="22"/>
+      <c r="EB36" s="132"/>
+      <c r="EL36" s="130"/>
       <c r="EV36" s="22"/>
     </row>
     <row r="37" spans="62:172" x14ac:dyDescent="0.3">
@@ -5764,11 +5983,12 @@
       <c r="CU37" s="22"/>
       <c r="CW37" s="22"/>
       <c r="CX37" s="22"/>
-      <c r="DR37" s="130"/>
-      <c r="DX37" s="50" t="s">
+      <c r="DR37" s="22"/>
+      <c r="EB37" s="130"/>
+      <c r="EG37" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="EB37" s="2"/>
+      <c r="EL37" s="22"/>
       <c r="EV37" s="22"/>
     </row>
     <row r="38" spans="62:172" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5834,27 +6054,27 @@
       <c r="DO38" s="1"/>
       <c r="DP38" s="1"/>
       <c r="DQ38" s="1"/>
-      <c r="DR38" s="131"/>
-      <c r="DS38" s="133"/>
-      <c r="DT38" s="128"/>
-      <c r="DU38" s="128"/>
-      <c r="DV38" s="128"/>
-      <c r="DW38" s="128"/>
-      <c r="DX38" s="128"/>
-      <c r="DY38" s="128"/>
-      <c r="DZ38" s="128"/>
-      <c r="EA38" s="128"/>
-      <c r="EB38" s="136"/>
-      <c r="EC38" s="1"/>
-      <c r="ED38" s="1"/>
-      <c r="EE38" s="1"/>
-      <c r="EF38" s="1"/>
-      <c r="EG38" s="1"/>
-      <c r="EH38" s="1"/>
-      <c r="EI38" s="1"/>
-      <c r="EJ38" s="1"/>
-      <c r="EK38" s="1"/>
-      <c r="EL38" s="1"/>
+      <c r="DR38" s="27"/>
+      <c r="DS38" s="25"/>
+      <c r="DT38" s="1"/>
+      <c r="DU38" s="1"/>
+      <c r="DV38" s="1"/>
+      <c r="DW38" s="1"/>
+      <c r="DX38" s="1"/>
+      <c r="DY38" s="115"/>
+      <c r="DZ38" s="1"/>
+      <c r="EA38" s="1"/>
+      <c r="EB38" s="131"/>
+      <c r="EC38" s="128"/>
+      <c r="ED38" s="128"/>
+      <c r="EE38" s="128"/>
+      <c r="EF38" s="128"/>
+      <c r="EG38" s="128"/>
+      <c r="EH38" s="128"/>
+      <c r="EI38" s="128"/>
+      <c r="EJ38" s="128"/>
+      <c r="EK38" s="128"/>
+      <c r="EL38" s="141"/>
       <c r="EM38" s="1"/>
       <c r="EN38" s="1"/>
       <c r="EO38" s="1"/>
@@ -5897,8 +6117,11 @@
       <c r="CX39" s="22"/>
       <c r="DH39" s="26"/>
       <c r="DR39" s="2"/>
+      <c r="DY39" s="22"/>
+      <c r="DZ39" s="44"/>
       <c r="EB39" s="2"/>
       <c r="EL39" s="2"/>
+      <c r="EN39" s="26"/>
       <c r="EV39" s="22"/>
       <c r="FF39" s="22"/>
       <c r="FP39" s="26"/>
@@ -5917,8 +6140,13 @@
         <v>56</v>
       </c>
       <c r="DR40" s="2"/>
+      <c r="DY40" s="169" t="s">
+        <v>45</v>
+      </c>
+      <c r="DZ40" s="22"/>
       <c r="EB40" s="2"/>
       <c r="EL40" s="2"/>
+      <c r="EN40" s="22"/>
       <c r="EV40" s="22"/>
       <c r="FF40" s="22"/>
       <c r="FP40" s="22"/>
@@ -5978,24 +6206,24 @@
       <c r="DT41" s="1"/>
       <c r="DU41" s="1"/>
       <c r="DV41" s="1"/>
-      <c r="DW41" s="1"/>
-      <c r="DX41" s="1"/>
-      <c r="DY41" s="1"/>
-      <c r="DZ41" s="1"/>
-      <c r="EA41" s="1"/>
-      <c r="EB41" s="3"/>
-      <c r="EC41" s="1"/>
-      <c r="ED41" s="1"/>
-      <c r="EE41" s="1"/>
-      <c r="EF41" s="1"/>
-      <c r="EG41" s="1"/>
-      <c r="EH41" s="1"/>
-      <c r="EI41" s="1"/>
-      <c r="EJ41" s="1"/>
-      <c r="EK41" s="1"/>
-      <c r="EL41" s="3"/>
-      <c r="EM41" s="1"/>
-      <c r="EN41" s="1"/>
+      <c r="DW41" s="168"/>
+      <c r="DX41" s="168"/>
+      <c r="DY41" s="27"/>
+      <c r="DZ41" s="43"/>
+      <c r="EA41" s="168"/>
+      <c r="EB41" s="2"/>
+      <c r="EC41" s="28"/>
+      <c r="ED41" s="168"/>
+      <c r="EE41" s="168"/>
+      <c r="EF41" s="168"/>
+      <c r="EG41" s="168"/>
+      <c r="EH41" s="168"/>
+      <c r="EI41" s="168"/>
+      <c r="EJ41" s="168"/>
+      <c r="EK41" s="168"/>
+      <c r="EL41" s="2"/>
+      <c r="EM41" s="28"/>
+      <c r="EN41" s="22"/>
       <c r="EO41" s="1"/>
       <c r="EP41" s="1"/>
       <c r="EQ41" s="1"/>
@@ -6023,6 +6251,8 @@
       <c r="DO42" s="41"/>
       <c r="DQ42" s="41"/>
       <c r="DR42" s="26"/>
+      <c r="DS42" s="87"/>
+      <c r="DT42" s="26"/>
       <c r="EB42" s="2"/>
       <c r="EL42" s="2"/>
       <c r="EV42" s="22"/>
@@ -6045,6 +6275,7 @@
       <c r="DN43" s="49"/>
       <c r="DP43" s="49"/>
       <c r="DR43" s="37"/>
+      <c r="DT43" s="37"/>
       <c r="EB43" s="2"/>
       <c r="EL43" s="2"/>
       <c r="EV43" s="22"/>
@@ -6114,8 +6345,8 @@
       <c r="DP44" s="1"/>
       <c r="DQ44" s="40"/>
       <c r="DR44" s="27"/>
-      <c r="DS44" s="1"/>
-      <c r="DT44" s="1"/>
+      <c r="DS44" s="48"/>
+      <c r="DT44" s="27"/>
       <c r="DU44" s="1"/>
       <c r="DV44" s="1"/>
       <c r="DW44" s="1"/>
@@ -6127,11 +6358,13 @@
       <c r="EC44" s="1"/>
       <c r="ED44" s="1"/>
       <c r="EE44" s="1"/>
-      <c r="EF44" s="1"/>
-      <c r="EG44" s="1"/>
+      <c r="EF44" s="85"/>
+      <c r="EG44" s="158">
+        <v>5</v>
+      </c>
       <c r="EH44" s="1"/>
       <c r="EI44" s="1"/>
-      <c r="EJ44" s="1"/>
+      <c r="EJ44" s="143"/>
       <c r="EK44" s="1"/>
       <c r="EL44" s="3"/>
       <c r="EM44" s="1"/>
@@ -6170,7 +6403,9 @@
       <c r="DL45" s="15"/>
       <c r="DR45" s="2"/>
       <c r="EB45" s="2"/>
-      <c r="EL45" s="2"/>
+      <c r="EJ45" s="29"/>
+      <c r="EK45" s="168"/>
+      <c r="EL45" s="113"/>
       <c r="EV45" s="22"/>
       <c r="FF45" s="2"/>
       <c r="FP45" s="22"/>
@@ -6199,8 +6434,13 @@
         <v>54</v>
       </c>
       <c r="EB46" s="2"/>
+      <c r="EJ46" s="168"/>
+      <c r="EK46" s="168"/>
       <c r="EL46" s="2"/>
-      <c r="EV46" s="60"/>
+      <c r="EM46" s="168"/>
+      <c r="EV46" s="167" t="s">
+        <v>62</v>
+      </c>
       <c r="FF46" s="2"/>
       <c r="FP46" s="22"/>
     </row>
@@ -6280,11 +6520,13 @@
       <c r="EB47" s="3"/>
       <c r="EC47" s="1"/>
       <c r="ED47" s="1"/>
-      <c r="EE47" s="1"/>
+      <c r="EE47" s="106"/>
       <c r="EF47" s="1"/>
-      <c r="EG47" s="1"/>
+      <c r="EG47" s="106"/>
       <c r="EH47" s="1"/>
-      <c r="EI47" s="1"/>
+      <c r="EI47" s="77">
+        <v>5</v>
+      </c>
       <c r="EJ47" s="1"/>
       <c r="EK47" s="1"/>
       <c r="EL47" s="3"/>

</xml_diff>